<commit_message>
added the last touches and some translations
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C446"/>
+  <dimension ref="A1:C448"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1781,3199 +1781,3215 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>settingsTabs.Time</v>
+        <v>crossPlot.sidebar.no-markers</v>
       </c>
       <c r="B147" t="str">
-        <v>Time</v>
-      </c>
-      <c r="C147" t="str">
-        <v>选择时间区间</v>
+        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>settingsTabs.Preferences</v>
+        <v>crossPlot.sidebar.no-models</v>
       </c>
       <c r="B148" t="str">
-        <v>Preferences</v>
-      </c>
-      <c r="C148" t="str">
-        <v>選擇偏好</v>
+        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>settingsTabs.Column</v>
+        <v>settingsTabs.Time</v>
       </c>
       <c r="B149" t="str">
-        <v>Column</v>
+        <v>Time</v>
       </c>
       <c r="C149" t="str">
-        <v>选择列</v>
+        <v>选择时间区间</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>settingsTabs.Search</v>
+        <v>settingsTabs.Preferences</v>
       </c>
       <c r="B150" t="str">
-        <v>Search</v>
+        <v>Preferences</v>
       </c>
       <c r="C150" t="str">
-        <v>搜索</v>
+        <v>選擇偏好</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>settingsTabs.Font</v>
+        <v>settingsTabs.Column</v>
       </c>
       <c r="B151" t="str">
-        <v>Font</v>
+        <v>Column</v>
       </c>
       <c r="C151" t="str">
-        <v>字体</v>
+        <v>选择列</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>settingsTabs.Map Points</v>
+        <v>settingsTabs.Search</v>
       </c>
       <c r="B152" t="str">
-        <v>Map Points</v>
+        <v>Search</v>
       </c>
       <c r="C152" t="str">
-        <v>地图</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>settingsTabs.Datapacks</v>
+        <v>settingsTabs.Font</v>
       </c>
       <c r="B153" t="str">
-        <v>Datapacks</v>
+        <v>Font</v>
       </c>
       <c r="C153" t="str">
-        <v>选择数据包</v>
+        <v>字体</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>settingsTabs.General</v>
+        <v>settingsTabs.Map Points</v>
       </c>
       <c r="B154" t="str">
-        <v>General</v>
+        <v>Map Points</v>
       </c>
       <c r="C154" t="str">
-        <v>基础选项</v>
+        <v>地图</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>settingsTabs.Data Mining</v>
+        <v>settingsTabs.Datapacks</v>
       </c>
       <c r="B155" t="str">
-        <v>Data Mining</v>
+        <v>Datapacks</v>
       </c>
       <c r="C155" t="str">
-        <v>数据挖掘</v>
+        <v>选择数据包</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>settingsTabs.Curve Drawing</v>
+        <v>settingsTabs.General</v>
       </c>
       <c r="B156" t="str">
-        <v>Curve Drawing</v>
+        <v>General</v>
       </c>
       <c r="C156" t="str">
-        <v>绘制曲线图</v>
+        <v>基础选项</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Data Mining</v>
       </c>
       <c r="B157" t="str">
-        <v>About</v>
+        <v>Data Mining</v>
       </c>
       <c r="C157" t="str">
-        <v>关于</v>
+        <v>数据挖掘</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.Curve Drawing</v>
       </c>
       <c r="B158" t="str">
-        <v>View Data</v>
+        <v>Curve Drawing</v>
       </c>
       <c r="C158" t="str">
-        <v>查看数据</v>
+        <v>绘制曲线图</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B159" t="str">
-        <v>Discussion</v>
+        <v>About</v>
       </c>
       <c r="C159" t="str">
-        <v>讨论</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B160" t="str">
-        <v>Warnings</v>
+        <v>View Data</v>
       </c>
       <c r="C160" t="str">
-        <v>警告</v>
+        <v>查看数据</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B161" t="str">
-        <v>Load/Save</v>
+        <v>Discussion</v>
+      </c>
+      <c r="C161" t="str">
+        <v>讨论</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B162" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Warnings</v>
+      </c>
+      <c r="C162" t="str">
+        <v>警告</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B163" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B164" t="str">
-        <v>Top of Interval</v>
-      </c>
-      <c r="C164" t="str">
-        <v>区间顶部</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B165" t="str">
-        <v>Base of Interval</v>
-      </c>
-      <c r="C165" t="str">
-        <v>区间底部</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B166" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Top of Interval</v>
       </c>
       <c r="C166" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B167" t="str">
-        <v>Base Age/Stage Name</v>
+        <v>Base of Interval</v>
       </c>
       <c r="C167" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间底部</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B168" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C168" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B169" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C169" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B170" t="str">
-        <v>Base age should be older than top age</v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C170" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B171" t="str">
-        <v>Vertical Scale</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+      </c>
+      <c r="C171" t="str">
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B172" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
+        <v>Base age should be older than top age</v>
       </c>
       <c r="C172" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B173" t="str">
-        <v>Add MouseOver info (popups)</v>
-      </c>
-      <c r="C173" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B174" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C174" t="str">
-        <v>启用优先级过滤</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B175" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Add MouseOver info (popups)</v>
       </c>
       <c r="C175" t="str">
-        <v>启用事件列的背景</v>
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B176" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C176" t="str">
-        <v>启用添加图例</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B177" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C177" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B178" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C178" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B179" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C179" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B180" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C180" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B181" t="str">
-        <v>Load Settings</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C181" t="str">
-        <v>上传设置</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B182" t="str">
-        <v>Save Settings</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C182" t="str">
-        <v>保存设置</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B183" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>Load Settings</v>
       </c>
       <c r="C183" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B184" t="str">
-        <v>Cancel</v>
+        <v>Save Settings</v>
       </c>
       <c r="C184" t="str">
-        <v>取消</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B185" t="str">
-        <v>Load</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C185" t="str">
-        <v>上传</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B186" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Cancel</v>
       </c>
       <c r="C186" t="str">
-        <v>请输入文件名</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B187" t="str">
-        <v>Cancel</v>
+        <v>Load</v>
       </c>
       <c r="C187" t="str">
-        <v>取消</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B188" t="str">
-        <v>Save</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C188" t="str">
-        <v>保存</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B189" t="str">
-        <v>Data not included in time range</v>
+        <v>Cancel</v>
+      </c>
+      <c r="C189" t="str">
+        <v>取消</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B190" t="str">
-        <v>Auto Scale</v>
+        <v>Save</v>
       </c>
       <c r="C190" t="str">
-        <v>自动缩放</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B191" t="str">
-        <v>Flip Range</v>
-      </c>
-      <c r="C191" t="str">
-        <v>翻转区间</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B192" t="str">
-        <v>Column Customization</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C192" t="str">
-        <v>个性化设置列</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B193" t="str">
-        <v>Data Mining Settings</v>
+        <v>Flip Range</v>
       </c>
       <c r="C193" t="str">
-        <v>数据挖掘设置</v>
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B194" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Column Customization</v>
       </c>
       <c r="C194" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B195" t="str">
-        <v>Shift Row Positions</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C195" t="str">
-        <v>移动位置</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Edit Title</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C196" t="str">
-        <v>编辑标题</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B197" t="str">
-        <v>Background Color</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C197" t="str">
-        <v>背景颜色</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B198" t="str">
-        <v>Enable Title</v>
+        <v>Edit Title</v>
       </c>
       <c r="C198" t="str">
-        <v>显示标题</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B199" t="str">
-        <v>Show Age Label</v>
+        <v>Background Color</v>
       </c>
       <c r="C199" t="str">
-        <v>显示年代</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B200" t="str">
-        <v>Information and References</v>
+        <v>Enable Title</v>
       </c>
       <c r="C200" t="str">
-        <v>信息与参考</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B201" t="str">
-        <v>Add Blank Column</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C201" t="str">
-        <v>添加一个空白列</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B202" t="str">
-        <v>Add Age Column</v>
+        <v>Information and References</v>
       </c>
       <c r="C202" t="str">
-        <v>添加一个年代列</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B203" t="str">
-        <v>Width</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C203" t="str">
-        <v>宽</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B204" t="str">
-        <v>Label Orientation</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C204" t="str">
-        <v>图标排布</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B205" t="str">
-        <v>Horizontal</v>
+        <v>Width</v>
       </c>
       <c r="C205" t="str">
-        <v>横向</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B206" t="str">
-        <v>Vertical</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C206" t="str">
-        <v>纵向</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B207" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Horizontal</v>
       </c>
       <c r="C207" t="str">
-        <v>显示不确定性</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B208" t="str">
-        <v>Events</v>
+        <v>Vertical</v>
       </c>
       <c r="C208" t="str">
-        <v>事件</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B209" t="str">
-        <v>Ranges</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C209" t="str">
-        <v>范围</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B210" t="str">
-        <v>First Occurrence</v>
+        <v>Events</v>
       </c>
       <c r="C210" t="str">
-        <v>首先发生的优先</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B211" t="str">
-        <v>Last Occurrence</v>
+        <v>Ranges</v>
       </c>
       <c r="C211" t="str">
-        <v>最后发生的优先</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B212" t="str">
-        <v>Alphabetical</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C212" t="str">
-        <v>按字母顺序排列</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B213" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C213" t="str">
-        <v>调整年代刻度尺</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B214" t="str">
-        <v>Left</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C214" t="str">
-        <v>左对齐</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B215" t="str">
-        <v>Right</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C215" t="str">
-        <v>右对齐</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B216" t="str">
-        <v>Change Font</v>
+        <v>Left</v>
       </c>
       <c r="C216" t="str">
-        <v>更改字体</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B217" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Right</v>
       </c>
       <c r="C217" t="str">
-        <v>子列的更多字体选项</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B218" t="str">
-        <v>Data Mining Settings</v>
+        <v>Change Font</v>
       </c>
       <c r="C218" t="str">
-        <v>数据挖掘设置</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B219" t="str">
-        <v>Window Size</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C219" t="str">
-        <v>窗口大小</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B220" t="str">
-        <v>Step Size</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C220" t="str">
-        <v>步长</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B221" t="str">
-        <v>Frequency</v>
+        <v>Window Size</v>
       </c>
       <c r="C221" t="str">
-        <v>频率</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B222" t="str">
-        <v>Maximum Value</v>
+        <v>Step Size</v>
       </c>
       <c r="C222" t="str">
-        <v>最大值</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B223" t="str">
-        <v>Minimum Value</v>
+        <v>Frequency</v>
       </c>
       <c r="C223" t="str">
-        <v>最小值</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B224" t="str">
-        <v>Average Value</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C224" t="str">
-        <v>平均值</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B225" t="str">
-        <v>Rate of Change</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C225" t="str">
-        <v>变化率</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Frequency of LAD</v>
+        <v>Average Value</v>
       </c>
       <c r="C226" t="str">
-        <v>LAD 频率</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B227" t="str">
-        <v>Frequency of FAD</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C227" t="str">
-        <v>FAD 频率</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B228" t="str">
-        <v>Combined Events</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C228" t="str">
-        <v>组合事件</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B229" t="str">
-        <v>Event Type</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C229" t="str">
-        <v>事件类型</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B230" t="str">
-        <v>Chron Type</v>
+        <v>Combined Events</v>
       </c>
       <c r="C230" t="str">
-        <v>年代类型</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B231" t="str">
-        <v>Data Type to Plot</v>
+        <v>Event Type</v>
       </c>
       <c r="C231" t="str">
-        <v>绘制数据类型</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B232" t="str">
-        <v>Point Settings</v>
+        <v>Chron Type</v>
       </c>
       <c r="C232" t="str">
-        <v>点设置</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B233" t="str">
-        <v>Range of Data</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C233" t="str">
-        <v>数据范围</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B234" t="str">
-        <v>Lower Range</v>
+        <v>Point Settings</v>
       </c>
       <c r="C234" t="str">
-        <v>下限</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B235" t="str">
-        <v>Upper Range</v>
+        <v>Range of Data</v>
       </c>
       <c r="C235" t="str">
-        <v>上限</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B236" t="str">
-        <v>Scale Start</v>
+        <v>Lower Range</v>
       </c>
       <c r="C236" t="str">
-        <v>刻度起点</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B237" t="str">
-        <v>Scale Step</v>
+        <v>Upper Range</v>
       </c>
       <c r="C237" t="str">
-        <v>刻度步长</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B238" t="str">
-        <v>Show Scale</v>
+        <v>Scale Start</v>
       </c>
       <c r="C238" t="str">
-        <v>显示刻度</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B239" t="str">
-        <v>Draw Points</v>
+        <v>Scale Step</v>
       </c>
       <c r="C239" t="str">
-        <v>绘制点</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B240" t="str">
-        <v>Point Shape</v>
+        <v>Show Scale</v>
       </c>
       <c r="C240" t="str">
-        <v>点形状</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B241" t="str">
-        <v>Line</v>
+        <v>Draw Points</v>
       </c>
       <c r="C241" t="str">
-        <v>线条</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B242" t="str">
-        <v>Fill</v>
+        <v>Point Shape</v>
       </c>
       <c r="C242" t="str">
-        <v>填充</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B243" t="str">
-        <v>Background Gradient</v>
+        <v>Line</v>
       </c>
       <c r="C243" t="str">
-        <v>背景渐变</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B244" t="str">
-        <v>Curve Gradient</v>
+        <v>Fill</v>
       </c>
       <c r="C244" t="str">
-        <v>曲线渐变</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B245" t="str">
-        <v>Start</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C245" t="str">
-        <v>起点</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B246" t="str">
-        <v>End</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C246" t="str">
-        <v>终点</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B247" t="str">
-        <v>Search</v>
+        <v>Start</v>
       </c>
       <c r="C247" t="str">
-        <v>搜索</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B248" t="str">
-        <v>Found {{count}} Results</v>
+        <v>End</v>
       </c>
       <c r="C248" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>终点</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B249" t="str">
-        <v>Current Time Settings(Top / Base)</v>
+        <v>Search</v>
       </c>
       <c r="C249" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B250" t="str">
-        <v>Column On?</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C250" t="str">
-        <v>是否已选</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B251" t="str">
-        <v>Center</v>
+        <v>Current Time Settings(Top / Base)</v>
       </c>
       <c r="C251" t="str">
-        <v>居中</v>
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B252" t="str">
-        <v>Extend</v>
+        <v>Column On?</v>
       </c>
       <c r="C252" t="str">
-        <v>延展</v>
+        <v>是否已选</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B253" t="str">
-        <v>Column</v>
+        <v>Center</v>
       </c>
       <c r="C253" t="str">
-        <v>列名称</v>
+        <v>居中</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B254" t="str">
-        <v>Age</v>
+        <v>Extend</v>
       </c>
       <c r="C254" t="str">
-        <v>年代</v>
+        <v>延展</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B255" t="str">
-        <v>Type</v>
+        <v>Column</v>
       </c>
       <c r="C255" t="str">
-        <v>类别</v>
+        <v>列名称</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B256" t="str">
-        <v>Notes</v>
+        <v>Age</v>
       </c>
       <c r="C256" t="str">
-        <v>注释</v>
+        <v>年代</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B257" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Type</v>
       </c>
       <c r="C257" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>类别</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B258" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>Notes</v>
       </c>
       <c r="C258" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B259" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>These are the default systemwide fonts.</v>
       </c>
       <c r="C259" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B260" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C260" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B261" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C261" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B262" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C262" t="str">
-        <v>点击加号添加数据包</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B263" t="str">
-        <v>Private Official Datapacks</v>
+        <v>Click a datapack to see more information!</v>
+      </c>
+      <c r="C263" t="str">
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B264" t="str">
-        <v>Official Datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
+      </c>
+      <c r="C264" t="str">
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B265" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B266" t="str">
-        <v>Workshop Datapacks</v>
-      </c>
-      <c r="C266" t="str">
-        <v>工作坊数据包</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B267" t="str">
-        <v>Your Datapacks</v>
-      </c>
-      <c r="C267" t="str">
-        <v>你的数据包</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B268" t="str">
-        <v>No</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C268" t="str">
-        <v>暂无</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B269" t="str">
-        <v>Avaliable</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C269" t="str">
-        <v>可用</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B270" t="str">
-        <v>Upload Datapack</v>
+        <v>No</v>
       </c>
       <c r="C270" t="str">
-        <v>上传数据包</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B271" t="str">
-        <v>PDF Upload</v>
+        <v>Avaliable</v>
+      </c>
+      <c r="C271" t="str">
+        <v>可用</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B272" t="str">
-        <v>See More...</v>
+        <v>Upload Datapack</v>
+      </c>
+      <c r="C272" t="str">
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B273" t="str">
-        <v>See Less...</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B274" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C274" t="str">
-        <v>上传你的数据包</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B275" t="str">
-        <v>No file selected</v>
-      </c>
-      <c r="C275" t="str">
-        <v>没有选择文件</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B276" t="str">
-        <v>Datapack Name</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C276" t="str">
-        <v>数据包名称</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B277" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>No file selected</v>
       </c>
       <c r="C277" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B278" t="str">
-        <v>Authored By</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C278" t="str">
-        <v>作者</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B279" t="str">
-        <v>Credited to...</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C279" t="str">
-        <v>作者为...</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B280" t="str">
-        <v>Datapack Description</v>
+        <v>Authored By</v>
       </c>
       <c r="C280" t="str">
-        <v>数据包概述</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B281" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Credited to...</v>
       </c>
       <c r="C281" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B282" t="str">
-        <v>Tags</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C282" t="str">
-        <v>标签</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B283" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C283" t="str">
-        <v>使数据包对公共可见</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B284" t="str">
-        <v>Add Reference</v>
+        <v>Tags</v>
       </c>
       <c r="C284" t="str">
-        <v>添加引用</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B285" t="str">
-        <v>More Options</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C285" t="str">
-        <v>更多选项</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B286" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>Add Reference</v>
       </c>
       <c r="C286" t="str">
-        <v>完成并上传</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B287" t="str">
-        <v>Start Over</v>
+        <v>More Options</v>
       </c>
       <c r="C287" t="str">
-        <v>重新开始</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B288" t="str">
-        <v>Reference</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C288" t="str">
-        <v>引用</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B289" t="str">
-        <v>Contact</v>
+        <v>Start Over</v>
       </c>
       <c r="C289" t="str">
-        <v>联系方式</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B290" t="str">
-        <v>Enter your contact information</v>
+        <v>Reference</v>
       </c>
       <c r="C290" t="str">
-        <v>输入你的联系方式</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B291" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Contact</v>
       </c>
       <c r="C291" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B292" t="str">
-        <v>Notes</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C292" t="str">
-        <v>注释</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B293" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C293" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B294" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Notes</v>
       </c>
       <c r="C294" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B295" t="str">
-        <v>You have not made a chart yet</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C295" t="str">
-        <v>您还未制作任何图表</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>chart.save</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B296" t="str">
-        <v>Save Chart</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C296" t="str">
-        <v>保存图表</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B297" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C297" t="str">
-        <v>确认更改数据包</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>chart.save</v>
       </c>
       <c r="B298" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>Save Chart</v>
       </c>
       <c r="C298" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B299" t="str">
-        <v>Save</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C299" t="str">
-        <v>保存</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B300" t="str">
-        <v>Discard</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C300" t="str">
-        <v>不保存</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B301" t="str">
-        <v>Use default age range?</v>
+        <v>Save</v>
       </c>
       <c r="C301" t="str">
-        <v>使用默认时间区间？</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B302" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>Discard</v>
+      </c>
+      <c r="C302" t="str">
+        <v>不保存</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>help.qsg.title</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B303" t="str">
-        <v>Quick Start Quide</v>
+        <v>Use default age range?</v>
       </c>
       <c r="C303" t="str">
-        <v>快速指南</v>
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>help.qsg.content</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B304" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
-      </c>
-      <c r="C304" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>help.qsg.button</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B305" t="str">
-        <v>Start QSG</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C305" t="str">
-        <v>开始快速指南</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>help.tour.title</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B306" t="str">
-        <v>Tour</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C306" t="str">
-        <v>导览</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B307" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Start QSG</v>
       </c>
       <c r="C307" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>help.tour.content.settings</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B308" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>Tour</v>
       </c>
       <c r="C308" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B309" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C309" t="str">
-        <v>开始数据包导览</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>help.tour.button.settings</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B310" t="str">
-        <v>Start Settings Tour</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C310" t="str">
-        <v>开始设置导览</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>help.license</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B311" t="str">
-        <v>Software License</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C311" t="str">
-        <v>软件许可</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B312" t="str">
-        <v>File Format Info</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C312" t="str">
-        <v>文件格式信息</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.license</v>
       </c>
       <c r="B313" t="str">
-        <v>View File Format Info</v>
+        <v>Software License</v>
       </c>
       <c r="C313" t="str">
-        <v>查看文件格式信息</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>errors.title</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B314" t="str">
-        <v>Error</v>
+        <v>File Format Info</v>
       </c>
       <c r="C314" t="str">
-        <v>错误</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B315" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C315" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>errors.title</v>
       </c>
       <c r="B316" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C316" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B317" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C317" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B318" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C318" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B319" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C319" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B320" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C320" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B321" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C321" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B322" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C322" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B323" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C323" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B324" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C324" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B325" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C325" t="str">
-        <v>无效的数据包上传</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B326" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
+      </c>
+      <c r="C326" t="str">
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
+        <v>Invalid datapack upload.</v>
       </c>
       <c r="C327" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B328" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
-      </c>
-      <c r="C328" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B329" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B330" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B331" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C331" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B332" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C332" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B333" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C333" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B334" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C334" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B335" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C335" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B336" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C336" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B337" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C337" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B338" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C338" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B339" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C339" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B340" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C340" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B341" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C341" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B342" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C342" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B343" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C343" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B344" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C344" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B345" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C345" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B346" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C346" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B347" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C347" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B348" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C348" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B349" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C349" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B350" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C350" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B351" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C351" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B352" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C352" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B354" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C354" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C355" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B356" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C356" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B357" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C357" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B358" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C358" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B359" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C359" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B360" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C360" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B361" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C361" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B362" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C362" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B363" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C363" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B364" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C364" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B366" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C366" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B367" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C367" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B368" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C368" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B369" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C369" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B370" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C370" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B371" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C371" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B372" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C372" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B373" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C373" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B374" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Server is too busy. Please try again later.</v>
+      </c>
+      <c r="C374" t="str">
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C375" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B376" t="str">
-        <v>Cannot delete root user.</v>
-      </c>
-      <c r="C376" t="str">
-        <v>不能删除根用户。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C377" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B378" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C378" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B379" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B380" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C380" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B381" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C381" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B382" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B383" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B384" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C384" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B385" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B386" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C386" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B387" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C387" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B388" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C388" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B389" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
       </c>
       <c r="C389" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B390" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C390" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B391" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
       </c>
       <c r="C391" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B392" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
       </c>
       <c r="C392" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B393" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>The start date must be before the end date.</v>
       </c>
       <c r="C393" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B394" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Unable to create workshop. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B395" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
+      </c>
+      <c r="C395" t="str">
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B396" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B398" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C398" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B399" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B400" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B401" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B402" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B403" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B404" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B405" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B407" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B408" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B409" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>button.generate</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B410" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C410" t="str">
-        <v>绘制</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B411" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C411" t="str">
-        <v>绘制图表</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate</v>
       </c>
       <c r="B412" t="str">
-        <v>Remove Cache</v>
+        <v>Generate</v>
       </c>
       <c r="C412" t="str">
-        <v>清除缓存</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B413" t="str">
-        <v>Confirm Selection</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C413" t="str">
-        <v>确认选择</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B414" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Remove Cache</v>
+      </c>
+      <c r="C414" t="str">
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>yes</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B415" t="str">
-        <v>Yes</v>
+        <v>Confirm Selection</v>
       </c>
       <c r="C415" t="str">
-        <v>是</v>
+        <v>确认选择</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>no</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B416" t="str">
-        <v>No</v>
-      </c>
-      <c r="C416" t="str">
-        <v>否</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>languageNames.en-US</v>
+        <v>yes</v>
       </c>
       <c r="B417" t="str">
-        <v>English</v>
+        <v>Yes</v>
+      </c>
+      <c r="C417" t="str">
+        <v>是</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>languageNames.en</v>
+        <v>no</v>
       </c>
       <c r="B418" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C418" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B419" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B420" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C420" t="str">
-        <v>退出导览</v>
+        <v>English</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>tours.finish</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B421" t="str">
-        <v>Finish Tour</v>
-      </c>
-      <c r="C421" t="str">
-        <v>结束导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>tours.next</v>
+        <v>tours.quit</v>
       </c>
       <c r="B422" t="str">
-        <v>Next</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C422" t="str">
-        <v>下一步</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>tours.back</v>
+        <v>tours.finish</v>
       </c>
       <c r="B423" t="str">
-        <v>Back</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C423" t="str">
-        <v>上一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.next</v>
       </c>
       <c r="B424" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Next</v>
       </c>
       <c r="C424" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.back</v>
       </c>
       <c r="B425" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>Back</v>
       </c>
       <c r="C425" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B426" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C426" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B427" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C427" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B428" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C428" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B429" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C429" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B430" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C430" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B431" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C431" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B432" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C432" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B433" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C433" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B434" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C434" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B435" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C435" t="str">
-        <v>记得确认您的选择</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B436" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C436" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B437" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C437" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B438" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C438" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B439" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C439" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B440" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C440" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C441" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B442" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C442" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B443" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C443" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B444" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C444" t="str">
-        <v>English</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>language-names.en</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C445" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C446" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C447" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C446" t="str">
+      <c r="C448" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C446"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C448"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add the code for sending a request
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C448"/>
+  <dimension ref="A1:C449"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4606,89 +4606,89 @@
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>button.generate</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B412" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C412" t="str">
-        <v>绘制</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>button.generate-chart</v>
+        <v>button.generate</v>
       </c>
       <c r="B413" t="str">
-        <v>Generate Chart</v>
+        <v>Generate</v>
       </c>
       <c r="C413" t="str">
-        <v>绘制图表</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B414" t="str">
-        <v>Remove Cache</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C414" t="str">
-        <v>清除缓存</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B415" t="str">
-        <v>Confirm Selection</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C415" t="str">
-        <v>确认选择</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B416" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C416" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>yes</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B417" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C417" t="str">
-        <v>是</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="B418" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="C418" t="str">
-        <v>否</v>
+        <v>是</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>languageNames.en-US</v>
+        <v>no</v>
       </c>
       <c r="B419" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C419" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>languageNames.en</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B420" t="str">
         <v>English</v>
@@ -4696,284 +4696,284 @@
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B421" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B422" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C422" t="str">
-        <v>退出导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>tours.finish</v>
+        <v>tours.quit</v>
       </c>
       <c r="B423" t="str">
-        <v>Finish Tour</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C423" t="str">
-        <v>结束导览</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>tours.next</v>
+        <v>tours.finish</v>
       </c>
       <c r="B424" t="str">
-        <v>Next</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C424" t="str">
-        <v>下一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>tours.back</v>
+        <v>tours.next</v>
       </c>
       <c r="B425" t="str">
-        <v>Back</v>
+        <v>Next</v>
       </c>
       <c r="C425" t="str">
-        <v>上一步</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B426" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Back</v>
       </c>
       <c r="C426" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B427" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C427" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B428" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C428" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B429" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C429" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B430" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C430" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B431" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C431" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B432" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C432" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B433" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C433" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B434" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C434" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B435" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C435" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B436" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C436" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B437" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C437" t="str">
-        <v>记得确认您的选择</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B438" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C438" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B439" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C439" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B440" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C440" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C441" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B442" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C442" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B443" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C443" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B444" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C444" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B445" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C445" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>language-names.en-US</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C446" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>language-names.en</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C447" t="str">
         <v>English</v>
@@ -4981,15 +4981,23 @@
     </row>
     <row r="448">
       <c r="A448" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C448" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C448" t="str">
+      <c r="C449" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C448"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C449"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final changes to working code
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C451"/>
+  <dimension ref="A1:C452"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4630,89 +4630,89 @@
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>button.generate</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B415" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C415" t="str">
-        <v>绘制</v>
+        <v>No models available. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>button.generate-chart</v>
+        <v>button.generate</v>
       </c>
       <c r="B416" t="str">
-        <v>Generate Chart</v>
+        <v>Generate</v>
       </c>
       <c r="C416" t="str">
-        <v>绘制图表</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B417" t="str">
-        <v>Remove Cache</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C417" t="str">
-        <v>清除缓存</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B418" t="str">
-        <v>Confirm Selection</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C418" t="str">
-        <v>确认选择</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B419" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C419" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>yes</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B420" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C420" t="str">
-        <v>是</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="B421" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="C421" t="str">
-        <v>否</v>
+        <v>是</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>languageNames.en-US</v>
+        <v>no</v>
       </c>
       <c r="B422" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C422" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>languageNames.en</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B423" t="str">
         <v>English</v>
@@ -4720,284 +4720,284 @@
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B424" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B425" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C425" t="str">
-        <v>退出导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>tours.finish</v>
+        <v>tours.quit</v>
       </c>
       <c r="B426" t="str">
-        <v>Finish Tour</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C426" t="str">
-        <v>结束导览</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>tours.next</v>
+        <v>tours.finish</v>
       </c>
       <c r="B427" t="str">
-        <v>Next</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C427" t="str">
-        <v>下一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.back</v>
+        <v>tours.next</v>
       </c>
       <c r="B428" t="str">
-        <v>Back</v>
+        <v>Next</v>
       </c>
       <c r="C428" t="str">
-        <v>上一步</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B429" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Back</v>
       </c>
       <c r="C429" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B430" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C430" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B431" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C431" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B432" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C432" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B433" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C433" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B434" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C434" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B435" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C435" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B436" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C436" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B437" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C437" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B438" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C438" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B439" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C439" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B440" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C440" t="str">
-        <v>记得确认您的选择</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C441" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B442" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C442" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B443" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C443" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B444" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C444" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B445" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C445" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B446" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C446" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B447" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C447" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B448" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C448" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>language-names.en-US</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C449" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>language-names.en</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C450" t="str">
         <v>English</v>
@@ -5005,15 +5005,23 @@
     </row>
     <row r="451">
       <c r="A451" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C451" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C451" t="str">
+      <c r="C452" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C451"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C452"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add better way to track mismatched settings and limit crossplot conversion to when settings matches
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C452"/>
+  <dimension ref="A1:C453"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4638,89 +4638,89 @@
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>button.generate</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B416" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C416" t="str">
-        <v>绘制</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>button.generate-chart</v>
+        <v>button.generate</v>
       </c>
       <c r="B417" t="str">
-        <v>Generate Chart</v>
+        <v>Generate</v>
       </c>
       <c r="C417" t="str">
-        <v>绘制图表</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B418" t="str">
-        <v>Remove Cache</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C418" t="str">
-        <v>清除缓存</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B419" t="str">
-        <v>Confirm Selection</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C419" t="str">
-        <v>确认选择</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B420" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C420" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>yes</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B421" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C421" t="str">
-        <v>是</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="B422" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="C422" t="str">
-        <v>否</v>
+        <v>是</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>languageNames.en-US</v>
+        <v>no</v>
       </c>
       <c r="B423" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C423" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>languageNames.en</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B424" t="str">
         <v>English</v>
@@ -4728,284 +4728,284 @@
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B425" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B426" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C426" t="str">
-        <v>退出导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>tours.finish</v>
+        <v>tours.quit</v>
       </c>
       <c r="B427" t="str">
-        <v>Finish Tour</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C427" t="str">
-        <v>结束导览</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.next</v>
+        <v>tours.finish</v>
       </c>
       <c r="B428" t="str">
-        <v>Next</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C428" t="str">
-        <v>下一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.back</v>
+        <v>tours.next</v>
       </c>
       <c r="B429" t="str">
-        <v>Back</v>
+        <v>Next</v>
       </c>
       <c r="C429" t="str">
-        <v>上一步</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B430" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Back</v>
       </c>
       <c r="C430" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B431" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C431" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B432" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C432" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B433" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C433" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B434" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C434" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B435" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C435" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B436" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C436" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B437" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C437" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B438" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C438" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B439" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C439" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B440" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C440" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B441" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C441" t="str">
-        <v>记得确认您的选择</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B442" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C442" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B443" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C443" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B444" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C444" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B445" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C445" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B446" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C446" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B447" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C447" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C448" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B449" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C449" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>language-names.en-US</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C450" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>language-names.en</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C451" t="str">
         <v>English</v>
@@ -5013,15 +5013,23 @@
     </row>
     <row r="452">
       <c r="A452" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C452" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C452" t="str">
+      <c r="C453" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C452"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C453"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solve conflict for translation.xlsx
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -1717,82 +1717,82 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B139" t="str">
-        <v>Please select a unit.</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B140" t="str">
-        <v>No units available</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B141" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B142" t="str">
-        <v>Please select a datapack.</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B143" t="str">
-        <v>No unit selected</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.xAxis</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B144" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>crossPlot.time.yAxis</v>
+        <v>crossPlot.time.xAxis</v>
       </c>
       <c r="B145" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>crossPlot.sidebar.no-markers</v>
+        <v>crossPlot.time.yAxis</v>
       </c>
       <c r="B146" t="str">
-        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>crossPlot.sidebar.no-models</v>
+        <v>crossPlot.sidebar.no-markers</v>
       </c>
       <c r="B147" t="str">
-        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
+        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>crossPlot.sidebar.no-models</v>
       </c>
       <c r="B148" t="str">
-        <v>Create Datapack</v>
+        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="149">
@@ -3137,257 +3137,257 @@
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B273" t="str">
-        <v>See More...</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B274" t="str">
-        <v>See Less...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B275" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C275" t="str">
-        <v>上传你的数据包</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B276" t="str">
-        <v>No file selected</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C276" t="str">
-        <v>没有选择文件</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B277" t="str">
-        <v>Datapack Name</v>
+        <v>No file selected</v>
       </c>
       <c r="C277" t="str">
-        <v>数据包名称</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B278" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C278" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B279" t="str">
-        <v>Authored By</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C279" t="str">
-        <v>作者</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B280" t="str">
-        <v>Credited to...</v>
+        <v>Authored By</v>
       </c>
       <c r="C280" t="str">
-        <v>作者为...</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B281" t="str">
-        <v>Datapack Description</v>
+        <v>Credited to...</v>
       </c>
       <c r="C281" t="str">
-        <v>数据包概述</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B282" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C282" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B283" t="str">
-        <v>Tags</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C283" t="str">
-        <v>标签</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B284" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Tags</v>
       </c>
       <c r="C284" t="str">
-        <v>使数据包对公共可见</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B285" t="str">
-        <v>Add Reference</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C285" t="str">
-        <v>添加引用</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B286" t="str">
-        <v>More Options</v>
+        <v>Add Reference</v>
       </c>
       <c r="C286" t="str">
-        <v>更多选项</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B287" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>More Options</v>
       </c>
       <c r="C287" t="str">
-        <v>完成并上传</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B288" t="str">
-        <v>Start Over</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C288" t="str">
-        <v>重新开始</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B289" t="str">
-        <v>Reference</v>
+        <v>Start Over</v>
       </c>
       <c r="C289" t="str">
-        <v>引用</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B290" t="str">
-        <v>Contact</v>
+        <v>Reference</v>
       </c>
       <c r="C290" t="str">
-        <v>联系方式</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B291" t="str">
-        <v>Enter your contact information</v>
+        <v>Contact</v>
       </c>
       <c r="C291" t="str">
-        <v>输入你的联系方式</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B292" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C292" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B293" t="str">
-        <v>Notes</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C293" t="str">
-        <v>注释</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B294" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Notes</v>
       </c>
       <c r="C294" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B295" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C295" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B296" t="str">
-        <v>PDF Upload</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+      </c>
+      <c r="C296" t="str">
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="297">

</xml_diff>

<commit_message>
added hasFiles attribute to datapack
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C475"/>
+  <dimension ref="A1:C453"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,7 +636,7 @@
         <v>landing-page.carousel.upload.collaborate.description</v>
       </c>
       <c r="B32" t="str">
-        <v>View other users&amp;apos; datapacks and collaborate to expand your knowledge and expertise.</v>
+        <v>View other users' datapacks and collaborate to expand your knowledge and expertise.</v>
       </c>
     </row>
     <row r="33">
@@ -813,7 +813,7 @@
         <v>login.signup</v>
       </c>
       <c r="B53" t="str">
-        <v>Don&amp;apos;t have an account? Sign Up</v>
+        <v>Don't have an account? Sign Up</v>
       </c>
       <c r="C53" t="str">
         <v>还没有账户？注册账户</v>
@@ -1464,303 +1464,303 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>workshops.details-page.download-tooltip-not-registered</v>
+        <v>workshops.calendar.switchLabel</v>
       </c>
       <c r="B113" t="str">
-        <v>Contact jogg@purdue.edu to register!</v>
+        <v>Toggle calendar</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>workshops.calendar.switchLabel</v>
+        <v>workshops.calendar.month</v>
       </c>
       <c r="B114" t="str">
-        <v>Toggle calendar</v>
+        <v>Month</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>workshops.calendar.month</v>
+        <v>workshops.calendar.week</v>
       </c>
       <c r="B115" t="str">
-        <v>Month</v>
+        <v>Week</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>workshops.calendar.week</v>
+        <v>workshops.calendar.days.sunday</v>
       </c>
       <c r="B116" t="str">
-        <v>Week</v>
+        <v>Sun</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>workshops.calendar.days.sunday</v>
+        <v>workshops.calendar.days.monday</v>
       </c>
       <c r="B117" t="str">
-        <v>Sun</v>
+        <v>Mon</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>workshops.calendar.days.monday</v>
+        <v>workshops.calendar.days.tuesday</v>
       </c>
       <c r="B118" t="str">
-        <v>Mon</v>
+        <v>Tue</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>workshops.calendar.days.tuesday</v>
+        <v>workshops.calendar.days.wednesday</v>
       </c>
       <c r="B119" t="str">
-        <v>Tue</v>
+        <v>Wed</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>workshops.calendar.days.wednesday</v>
+        <v>workshops.calendar.days.thursday</v>
       </c>
       <c r="B120" t="str">
-        <v>Wed</v>
+        <v>Thu</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>workshops.calendar.days.thursday</v>
+        <v>workshops.calendar.days.friday</v>
       </c>
       <c r="B121" t="str">
-        <v>Thu</v>
+        <v>Fri</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>workshops.calendar.days.friday</v>
+        <v>workshops.calendar.days.saturday</v>
       </c>
       <c r="B122" t="str">
-        <v>Fri</v>
+        <v>Sat</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>workshops.calendar.days.saturday</v>
+        <v>workshops.calendar.months.1</v>
       </c>
       <c r="B123" t="str">
-        <v>Sat</v>
+        <v>January</v>
+      </c>
+      <c r="C123" t="str">
+        <v>一月</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>workshops.calendar.months.1</v>
+        <v>workshops.calendar.months.2</v>
       </c>
       <c r="B124" t="str">
-        <v>January</v>
+        <v>February</v>
       </c>
       <c r="C124" t="str">
-        <v>一月</v>
+        <v>二月</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>workshops.calendar.months.2</v>
+        <v>workshops.calendar.months.3</v>
       </c>
       <c r="B125" t="str">
-        <v>February</v>
+        <v>March</v>
       </c>
       <c r="C125" t="str">
-        <v>二月</v>
+        <v>三月</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>workshops.calendar.months.3</v>
+        <v>workshops.calendar.months.4</v>
       </c>
       <c r="B126" t="str">
-        <v>March</v>
+        <v>April</v>
       </c>
       <c r="C126" t="str">
-        <v>三月</v>
+        <v>四月</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>workshops.calendar.months.4</v>
+        <v>workshops.calendar.months.5</v>
       </c>
       <c r="B127" t="str">
-        <v>April</v>
+        <v>May</v>
       </c>
       <c r="C127" t="str">
-        <v>四月</v>
+        <v>五月</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>workshops.calendar.months.5</v>
+        <v>workshops.calendar.months.6</v>
       </c>
       <c r="B128" t="str">
-        <v>May</v>
+        <v>June</v>
       </c>
       <c r="C128" t="str">
-        <v>五月</v>
+        <v>六月</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>workshops.calendar.months.6</v>
+        <v>workshops.calendar.months.7</v>
       </c>
       <c r="B129" t="str">
-        <v>June</v>
+        <v>July</v>
       </c>
       <c r="C129" t="str">
-        <v>六月</v>
+        <v>七月</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>workshops.calendar.months.7</v>
+        <v>workshops.calendar.months.8</v>
       </c>
       <c r="B130" t="str">
-        <v>July</v>
+        <v>August</v>
       </c>
       <c r="C130" t="str">
-        <v>七月</v>
+        <v>八月</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>workshops.calendar.months.8</v>
+        <v>workshops.calendar.months.9</v>
       </c>
       <c r="B131" t="str">
-        <v>August</v>
+        <v>September</v>
       </c>
       <c r="C131" t="str">
-        <v>八月</v>
+        <v>九月</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>workshops.calendar.months.9</v>
+        <v>workshops.calendar.months.10</v>
       </c>
       <c r="B132" t="str">
-        <v>September</v>
+        <v>October</v>
       </c>
       <c r="C132" t="str">
-        <v>九月</v>
+        <v>十月</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>workshops.calendar.months.10</v>
+        <v>workshops.calendar.months.11</v>
       </c>
       <c r="B133" t="str">
-        <v>October</v>
+        <v>November</v>
       </c>
       <c r="C133" t="str">
-        <v>十月</v>
+        <v>十一月</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>workshops.calendar.months.11</v>
+        <v>workshops.calendar.months.12</v>
       </c>
       <c r="B134" t="str">
-        <v>November</v>
+        <v>December</v>
       </c>
       <c r="C134" t="str">
-        <v>十一月</v>
+        <v>十二月</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>workshops.calendar.months.12</v>
+        <v>loading.loading-chart</v>
       </c>
       <c r="B135" t="str">
-        <v>December</v>
+        <v>Loading Chart...</v>
       </c>
       <c r="C135" t="str">
-        <v>十二月</v>
+        <v>加载图表...</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>loading.loading-chart</v>
+        <v>loading.loading-datapacks</v>
       </c>
       <c r="B136" t="str">
-        <v>Loading Chart...</v>
+        <v>Loading Datapacks</v>
       </c>
       <c r="C136" t="str">
-        <v>加载图表...</v>
+        <v>加载数据包</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>loading.loading-datapacks</v>
+        <v>loading.time</v>
       </c>
       <c r="B137" t="str">
-        <v>Loading Datapacks</v>
+        <v>this could take more than a minute</v>
       </c>
       <c r="C137" t="str">
-        <v>加载数据包</v>
+        <v>这可能需要超过一分钟</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>loading.time</v>
+        <v>loading.fetching-datapacks</v>
       </c>
       <c r="B138" t="str">
-        <v>this could take more than a minute</v>
-      </c>
-      <c r="C138" t="str">
-        <v>这可能需要超过一分钟</v>
+        <v>Fetching Datapacks</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>loading.fetching-datapacks</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B139" t="str">
-        <v>Fetching Datapacks</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B140" t="str">
-        <v>Please select a unit.</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B141" t="str">
-        <v>No units available</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B142" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B143" t="str">
-        <v>Please select a datapack.</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B144" t="str">
-        <v>No unit selected</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="145">
@@ -1797,3418 +1797,3239 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>settingsTabs.Time</v>
       </c>
       <c r="B149" t="str">
-        <v>Create Datapack</v>
+        <v>Time</v>
+      </c>
+      <c r="C149" t="str">
+        <v>选择时间区间</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>settingsTabs.Time</v>
+        <v>settingsTabs.Preferences</v>
       </c>
       <c r="B150" t="str">
-        <v>Time</v>
+        <v>Preferences</v>
       </c>
       <c r="C150" t="str">
-        <v>选择时间区间</v>
+        <v>選擇偏好</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>settingsTabs.Preferences</v>
+        <v>settingsTabs.Column</v>
       </c>
       <c r="B151" t="str">
-        <v>Preferences</v>
+        <v>Column</v>
       </c>
       <c r="C151" t="str">
-        <v>選擇偏好</v>
+        <v>选择列</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>settingsTabs.Column</v>
+        <v>settingsTabs.Search</v>
       </c>
       <c r="B152" t="str">
-        <v>Column</v>
+        <v>Search</v>
       </c>
       <c r="C152" t="str">
-        <v>选择列</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>settingsTabs.Search</v>
+        <v>settingsTabs.Font</v>
       </c>
       <c r="B153" t="str">
-        <v>Search</v>
+        <v>Font</v>
       </c>
       <c r="C153" t="str">
-        <v>搜索</v>
+        <v>字体</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>settingsTabs.Font</v>
+        <v>settingsTabs.Map Points</v>
       </c>
       <c r="B154" t="str">
-        <v>Font</v>
+        <v>Map Points</v>
       </c>
       <c r="C154" t="str">
-        <v>字体</v>
+        <v>地图</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>settingsTabs.Map Points</v>
+        <v>settingsTabs.Datapacks</v>
       </c>
       <c r="B155" t="str">
-        <v>Map Points</v>
+        <v>Datapacks</v>
       </c>
       <c r="C155" t="str">
-        <v>地图</v>
+        <v>选择数据包</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>settingsTabs.Datapacks</v>
+        <v>settingsTabs.General</v>
       </c>
       <c r="B156" t="str">
-        <v>Datapacks</v>
+        <v>General</v>
       </c>
       <c r="C156" t="str">
-        <v>选择数据包</v>
+        <v>基础选项</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>settingsTabs.General</v>
+        <v>settingsTabs.Data Mining</v>
       </c>
       <c r="B157" t="str">
-        <v>General</v>
+        <v>Data Mining</v>
       </c>
       <c r="C157" t="str">
-        <v>基础选项</v>
+        <v>数据挖掘</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>settingsTabs.Data Mining</v>
+        <v>settingsTabs.Curve Drawing</v>
       </c>
       <c r="B158" t="str">
-        <v>Data Mining</v>
+        <v>Curve Drawing</v>
       </c>
       <c r="C158" t="str">
-        <v>数据挖掘</v>
+        <v>绘制曲线图</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.Curve Drawing</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B159" t="str">
-        <v>Curve Drawing</v>
+        <v>About</v>
       </c>
       <c r="C159" t="str">
-        <v>绘制曲线图</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.Overlay</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B160" t="str">
-        <v>Overlay</v>
+        <v>View Data</v>
+      </c>
+      <c r="C160" t="str">
+        <v>查看数据</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B161" t="str">
-        <v>About</v>
+        <v>Discussion</v>
       </c>
       <c r="C161" t="str">
-        <v>关于</v>
+        <v>讨论</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B162" t="str">
-        <v>View Data</v>
+        <v>Warnings</v>
       </c>
       <c r="C162" t="str">
-        <v>查看数据</v>
+        <v>警告</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B163" t="str">
-        <v>Discussion</v>
-      </c>
-      <c r="C163" t="str">
-        <v>讨论</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B164" t="str">
-        <v>Warnings</v>
-      </c>
-      <c r="C164" t="str">
-        <v>警告</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B165" t="str">
-        <v>Load/Save</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B166" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Top of Interval</v>
+      </c>
+      <c r="C166" t="str">
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B167" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>Base of Interval</v>
+      </c>
+      <c r="C167" t="str">
+        <v>区间底部</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B168" t="str">
-        <v>Top of Interval</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C168" t="str">
-        <v>区间顶部</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B169" t="str">
-        <v>Base of Interval</v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C169" t="str">
-        <v>区间底部</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B170" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C170" t="str">
-        <v>年代/阶段 名称</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B171" t="str">
-        <v>Base Age/Stage Name</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
       </c>
       <c r="C171" t="str">
-        <v>年代/阶段 名称</v>
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B172" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Base age should be older than top age</v>
       </c>
       <c r="C172" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B173" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
-      </c>
-      <c r="C173" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B174" t="str">
-        <v>Base age should be older than top age</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C174" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B175" t="str">
-        <v>Vertical Scale</v>
+        <v>Add MouseOver info (popups)</v>
+      </c>
+      <c r="C175" t="str">
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B176" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C176" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B177" t="str">
-        <v>Add MouseOver info (popups)</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C177" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B178" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C178" t="str">
-        <v>启用优先级过滤</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B179" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C179" t="str">
-        <v>启用事件列的背景</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B180" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C180" t="str">
-        <v>启用添加图例</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B181" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C181" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B182" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C182" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B183" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Load Settings</v>
       </c>
       <c r="C183" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B184" t="str">
-        <v>Do not use the Data-Pack&amp;apos;s suggested age span</v>
+        <v>Save Settings</v>
       </c>
       <c r="C184" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B185" t="str">
-        <v>Load Settings</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C185" t="str">
-        <v>上传设置</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B186" t="str">
-        <v>Save Settings</v>
+        <v>Cancel</v>
       </c>
       <c r="C186" t="str">
-        <v>保存设置</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B187" t="str">
-        <v>This will overwrite any changes you&amp;apos;ve made!</v>
+        <v>Load</v>
       </c>
       <c r="C187" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B188" t="str">
-        <v>Cancel</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C188" t="str">
-        <v>取消</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B189" t="str">
-        <v>Load</v>
+        <v>Cancel</v>
       </c>
       <c r="C189" t="str">
-        <v>上传</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B190" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Save</v>
       </c>
       <c r="C190" t="str">
-        <v>请输入文件名</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B191" t="str">
-        <v>Cancel</v>
-      </c>
-      <c r="C191" t="str">
-        <v>取消</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B192" t="str">
-        <v>Save</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C192" t="str">
-        <v>保存</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B193" t="str">
-        <v>Data not included in time range</v>
+        <v>Flip Range</v>
+      </c>
+      <c r="C193" t="str">
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B194" t="str">
-        <v>Auto Scale</v>
+        <v>Column Customization</v>
       </c>
       <c r="C194" t="str">
-        <v>自动缩放</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B195" t="str">
-        <v>Flip Range</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C195" t="str">
-        <v>翻转区间</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Column Customization</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C196" t="str">
-        <v>个性化设置列</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B197" t="str">
-        <v>Data Mining Settings</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C197" t="str">
-        <v>数据挖掘设置</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B198" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Edit Title</v>
       </c>
       <c r="C198" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B199" t="str">
-        <v>Shift Row Positions</v>
+        <v>Background Color</v>
       </c>
       <c r="C199" t="str">
-        <v>移动位置</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B200" t="str">
-        <v>Edit Title</v>
+        <v>Enable Title</v>
       </c>
       <c r="C200" t="str">
-        <v>编辑标题</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B201" t="str">
-        <v>Background Color</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C201" t="str">
-        <v>背景颜色</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B202" t="str">
-        <v>Enable Title</v>
+        <v>Information and References</v>
       </c>
       <c r="C202" t="str">
-        <v>显示标题</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B203" t="str">
-        <v>Show Age Label</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C203" t="str">
-        <v>显示年代</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B204" t="str">
-        <v>Information and References</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C204" t="str">
-        <v>信息与参考</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B205" t="str">
-        <v>Add Blank Column</v>
+        <v>Width</v>
       </c>
       <c r="C205" t="str">
-        <v>添加一个空白列</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B206" t="str">
-        <v>Add Age Column</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C206" t="str">
-        <v>添加一个年代列</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B207" t="str">
-        <v>Width</v>
+        <v>Horizontal</v>
       </c>
       <c r="C207" t="str">
-        <v>宽</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B208" t="str">
-        <v>Label Orientation</v>
+        <v>Vertical</v>
       </c>
       <c r="C208" t="str">
-        <v>图标排布</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B209" t="str">
-        <v>Horizontal</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C209" t="str">
-        <v>横向</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B210" t="str">
-        <v>Vertical</v>
+        <v>Events</v>
       </c>
       <c r="C210" t="str">
-        <v>纵向</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B211" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Ranges</v>
       </c>
       <c r="C211" t="str">
-        <v>显示不确定性</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B212" t="str">
-        <v>Events</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C212" t="str">
-        <v>事件</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B213" t="str">
-        <v>Ranges</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C213" t="str">
-        <v>范围</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B214" t="str">
-        <v>First Occurrence</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C214" t="str">
-        <v>首先发生的优先</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B215" t="str">
-        <v>Last Occurrence</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C215" t="str">
-        <v>最后发生的优先</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B216" t="str">
-        <v>Alphabetical</v>
+        <v>Left</v>
       </c>
       <c r="C216" t="str">
-        <v>按字母顺序排列</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B217" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Right</v>
       </c>
       <c r="C217" t="str">
-        <v>调整年代刻度尺</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B218" t="str">
-        <v>Left</v>
+        <v>Change Font</v>
       </c>
       <c r="C218" t="str">
-        <v>左对齐</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B219" t="str">
-        <v>Right</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C219" t="str">
-        <v>右对齐</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B220" t="str">
-        <v>Change Font</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C220" t="str">
-        <v>更改字体</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B221" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Window Size</v>
       </c>
       <c r="C221" t="str">
-        <v>子列的更多字体选项</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B222" t="str">
-        <v>Data Mining Settings</v>
+        <v>Step Size</v>
       </c>
       <c r="C222" t="str">
-        <v>数据挖掘设置</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B223" t="str">
-        <v>Window Size</v>
+        <v>Frequency</v>
       </c>
       <c r="C223" t="str">
-        <v>窗口大小</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B224" t="str">
-        <v>Step Size</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C224" t="str">
-        <v>步长</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B225" t="str">
-        <v>Frequency</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C225" t="str">
-        <v>频率</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Maximum Value</v>
+        <v>Average Value</v>
       </c>
       <c r="C226" t="str">
-        <v>最大值</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B227" t="str">
-        <v>Minimum Value</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C227" t="str">
-        <v>最小值</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B228" t="str">
-        <v>Average Value</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C228" t="str">
-        <v>平均值</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B229" t="str">
-        <v>Rate of Change</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C229" t="str">
-        <v>变化率</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B230" t="str">
-        <v>Frequency of LAD</v>
+        <v>Combined Events</v>
       </c>
       <c r="C230" t="str">
-        <v>LAD 频率</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B231" t="str">
-        <v>Frequency of FAD</v>
+        <v>Event Type</v>
       </c>
       <c r="C231" t="str">
-        <v>FAD 频率</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B232" t="str">
-        <v>Combined Events</v>
+        <v>Chron Type</v>
       </c>
       <c r="C232" t="str">
-        <v>组合事件</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B233" t="str">
-        <v>Event Type</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C233" t="str">
-        <v>事件类型</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B234" t="str">
-        <v>Chron Type</v>
+        <v>Point Settings</v>
       </c>
       <c r="C234" t="str">
-        <v>年代类型</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B235" t="str">
-        <v>Data Type to Plot</v>
+        <v>Range of Data</v>
       </c>
       <c r="C235" t="str">
-        <v>绘制数据类型</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B236" t="str">
-        <v>Point Settings</v>
+        <v>Lower Range</v>
       </c>
       <c r="C236" t="str">
-        <v>点设置</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B237" t="str">
-        <v>Range of Data</v>
+        <v>Upper Range</v>
       </c>
       <c r="C237" t="str">
-        <v>数据范围</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B238" t="str">
-        <v>Lower Range</v>
+        <v>Scale Start</v>
       </c>
       <c r="C238" t="str">
-        <v>下限</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B239" t="str">
-        <v>Upper Range</v>
+        <v>Scale Step</v>
       </c>
       <c r="C239" t="str">
-        <v>上限</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B240" t="str">
-        <v>Scale Start</v>
+        <v>Show Scale</v>
       </c>
       <c r="C240" t="str">
-        <v>刻度起点</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B241" t="str">
-        <v>Scale Step</v>
+        <v>Draw Points</v>
       </c>
       <c r="C241" t="str">
-        <v>刻度步长</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B242" t="str">
-        <v>Show Scale</v>
+        <v>Point Shape</v>
       </c>
       <c r="C242" t="str">
-        <v>显示刻度</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B243" t="str">
-        <v>Draw Points</v>
+        <v>Line</v>
       </c>
       <c r="C243" t="str">
-        <v>绘制点</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B244" t="str">
-        <v>Point Shape</v>
+        <v>Fill</v>
       </c>
       <c r="C244" t="str">
-        <v>点形状</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B245" t="str">
-        <v>Line</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C245" t="str">
-        <v>线条</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B246" t="str">
-        <v>Fill</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C246" t="str">
-        <v>填充</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B247" t="str">
-        <v>Background Gradient</v>
+        <v>Start</v>
       </c>
       <c r="C247" t="str">
-        <v>背景渐变</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B248" t="str">
-        <v>Curve Gradient</v>
+        <v>End</v>
       </c>
       <c r="C248" t="str">
-        <v>曲线渐变</v>
+        <v>终点</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B249" t="str">
-        <v>Start</v>
+        <v>Search</v>
       </c>
       <c r="C249" t="str">
-        <v>起点</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B250" t="str">
-        <v>End</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C250" t="str">
-        <v>终点</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.column.overlay-menu.title</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B251" t="str">
-        <v>Overlay Settings</v>
+        <v>Current Time Settings(Top / Base)</v>
+      </c>
+      <c r="C251" t="str">
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.column.overlay-menu.display-overlay</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B252" t="str">
-        <v>Display Overlay</v>
+        <v>Column On?</v>
+      </c>
+      <c r="C252" t="str">
+        <v>是否已选</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.column.overlay-menu.overlay-column-header</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B253" t="str">
-        <v>Overlaying</v>
+        <v>Center</v>
+      </c>
+      <c r="C253" t="str">
+        <v>居中</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.column.overlay-menu.overlay-column-preposition</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B254" t="str">
-        <v>On</v>
+        <v>Extend</v>
+      </c>
+      <c r="C254" t="str">
+        <v>延展</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B255" t="str">
-        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
+        <v>Column</v>
+      </c>
+      <c r="C255" t="str">
+        <v>列名称</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B256" t="str">
-        <v>Not an Event or Point Column</v>
+        <v>Age</v>
+      </c>
+      <c r="C256" t="str">
+        <v>年代</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.column.overlay-menu.column-not-selected</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B257" t="str">
-        <v>Select Column from Menu</v>
+        <v>Type</v>
+      </c>
+      <c r="C257" t="str">
+        <v>类别</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B258" t="str">
-        <v>Search</v>
+        <v>Notes</v>
       </c>
       <c r="C258" t="str">
-        <v>搜索</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B259" t="str">
-        <v>Found {{count}} Results</v>
+        <v>These are the default systemwide fonts.</v>
       </c>
       <c r="C259" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B260" t="str">
-        <v>Current Time Settings(Top / Base)</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C260" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B261" t="str">
-        <v>Column On?</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C261" t="str">
-        <v>是否已选</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B262" t="str">
-        <v>Center</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C262" t="str">
-        <v>居中</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B263" t="str">
-        <v>Extend</v>
+        <v>Click a datapack to see more information!</v>
       </c>
       <c r="C263" t="str">
-        <v>延展</v>
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B264" t="str">
-        <v>Column</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C264" t="str">
-        <v>列名称</v>
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B265" t="str">
-        <v>Age</v>
-      </c>
-      <c r="C265" t="str">
-        <v>年代</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B266" t="str">
-        <v>Type</v>
-      </c>
-      <c r="C266" t="str">
-        <v>类别</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B267" t="str">
-        <v>Notes</v>
-      </c>
-      <c r="C267" t="str">
-        <v>注释</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B268" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C268" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B269" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C269" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B270" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>No</v>
       </c>
       <c r="C270" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B271" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>Avaliable</v>
       </c>
       <c r="C271" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B272" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>Upload Datapack</v>
       </c>
       <c r="C272" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B273" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
-      </c>
-      <c r="C273" t="str">
-        <v>点击加号添加数据包</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B274" t="str">
-        <v>Private Official Datapacks</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B275" t="str">
-        <v>Official Datapacks</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B276" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>Upload Your Own Datapack</v>
+      </c>
+      <c r="C276" t="str">
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B277" t="str">
-        <v>Workshop Datapacks</v>
+        <v>No file selected</v>
       </c>
       <c r="C277" t="str">
-        <v>工作坊数据包</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B278" t="str">
-        <v>Your Datapacks</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C278" t="str">
-        <v>你的数据包</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.title.treatise</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B279" t="str">
-        <v>Treatise Datapacks</v>
+        <v>Enter a name for your datapack.</v>
+      </c>
+      <c r="C279" t="str">
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B280" t="str">
-        <v>No</v>
+        <v>Authored By</v>
       </c>
       <c r="C280" t="str">
-        <v>暂无</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B281" t="str">
-        <v>Avaliable</v>
+        <v>Credited to...</v>
       </c>
       <c r="C281" t="str">
-        <v>可用</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B282" t="str">
-        <v>Upload Datapack</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C282" t="str">
-        <v>上传数据包</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B283" t="str">
-        <v>See More...</v>
+        <v>Enter a description for your datapack.</v>
+      </c>
+      <c r="C283" t="str">
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B284" t="str">
-        <v>See Less...</v>
+        <v>Tags</v>
+      </c>
+      <c r="C284" t="str">
+        <v>标签</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B285" t="str">
-        <v>Upload Your Own Datapack</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C285" t="str">
-        <v>上传你的数据包</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B286" t="str">
-        <v>No file selected</v>
+        <v>Add Reference</v>
       </c>
       <c r="C286" t="str">
-        <v>没有选择文件</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B287" t="str">
-        <v>Datapack Name</v>
+        <v>More Options</v>
       </c>
       <c r="C287" t="str">
-        <v>数据包名称</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B288" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C288" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B289" t="str">
-        <v>Authored By</v>
+        <v>Start Over</v>
       </c>
       <c r="C289" t="str">
-        <v>作者</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B290" t="str">
-        <v>Credited to...</v>
+        <v>Reference</v>
       </c>
       <c r="C290" t="str">
-        <v>作者为...</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B291" t="str">
-        <v>Datapack Description</v>
+        <v>Contact</v>
       </c>
       <c r="C291" t="str">
-        <v>数据包概述</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B292" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C292" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B293" t="str">
-        <v>Tags</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C293" t="str">
-        <v>标签</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B294" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Notes</v>
       </c>
       <c r="C294" t="str">
-        <v>使数据包对公共可见</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B295" t="str">
-        <v>Add Reference</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C295" t="str">
-        <v>添加引用</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B296" t="str">
-        <v>More Options</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C296" t="str">
-        <v>更多选项</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B297" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C297" t="str">
-        <v>完成并上传</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>chart.save</v>
       </c>
       <c r="B298" t="str">
-        <v>Start Over</v>
+        <v>Save Chart</v>
       </c>
       <c r="C298" t="str">
-        <v>重新开始</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B299" t="str">
-        <v>Reference</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C299" t="str">
-        <v>引用</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B300" t="str">
-        <v>Contact</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C300" t="str">
-        <v>联系方式</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B301" t="str">
-        <v>Enter your contact information</v>
+        <v>Save</v>
       </c>
       <c r="C301" t="str">
-        <v>输入你的联系方式</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B302" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Discard</v>
       </c>
       <c r="C302" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B303" t="str">
-        <v>Notes</v>
+        <v>Use default age range?</v>
       </c>
       <c r="C303" t="str">
-        <v>注释</v>
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B304" t="str">
-        <v>Enter notes for the datapack here</v>
-      </c>
-      <c r="C304" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B305" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C305" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B306" t="str">
-        <v>PDF Upload</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+      </c>
+      <c r="C306" t="str">
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B307" t="str">
-        <v>You have not made a chart yet</v>
+        <v>Start QSG</v>
       </c>
       <c r="C307" t="str">
-        <v>您还未制作任何图表</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>chart.save</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B308" t="str">
-        <v>Save Chart</v>
+        <v>Tour</v>
       </c>
       <c r="C308" t="str">
-        <v>保存图表</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B309" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C309" t="str">
-        <v>确认更改数据包</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B310" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C310" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B311" t="str">
-        <v>Save</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C311" t="str">
-        <v>保存</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B312" t="str">
-        <v>Discard</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C312" t="str">
-        <v>不保存</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>help.license</v>
       </c>
       <c r="B313" t="str">
-        <v>Use default age range?</v>
+        <v>Software License</v>
       </c>
       <c r="C313" t="str">
-        <v>使用默认时间区间？</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B314" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>File Format Info</v>
+      </c>
+      <c r="C314" t="str">
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.qsg.title</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B315" t="str">
-        <v>Quick Start Quide</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C315" t="str">
-        <v>快速指南</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>help.qsg.content</v>
+        <v>errors.title</v>
       </c>
       <c r="B316" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the &amp;apos;Start QSG&amp;apos; button to begin.</v>
+        <v>Error</v>
       </c>
       <c r="C316" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>help.qsg.button</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B317" t="str">
-        <v>Start QSG</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C317" t="str">
-        <v>开始快速指南</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>help.tour.title</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B318" t="str">
-        <v>Tour</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C318" t="str">
-        <v>导览</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B319" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C319" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>help.tour.content.settings</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B320" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C320" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B321" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C321" t="str">
-        <v>开始数据包导览</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>help.tour.button.settings</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B322" t="str">
-        <v>Start Settings Tour</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C322" t="str">
-        <v>开始设置导览</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>help.license</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B323" t="str">
-        <v>Software License</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C323" t="str">
-        <v>软件许可</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>help.file-format-info.title</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B324" t="str">
-        <v>File Format Info</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C324" t="str">
-        <v>文件格式信息</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>help.file-format-info.link</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B325" t="str">
-        <v>View File Format Info</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C325" t="str">
-        <v>查看文件格式信息</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.title</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B326" t="str">
-        <v>Error</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C326" t="str">
-        <v>错误</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B327" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>Invalid datapack upload.</v>
       </c>
       <c r="C327" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B328" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
-      </c>
-      <c r="C328" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B331" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C331" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B332" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C332" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B333" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C333" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B334" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C334" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B335" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C335" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B336" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C336" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B337" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C337" t="str">
-        <v>无效的数据包上传</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.INVALID_DATAPACK_PHYLUM</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B338" t="str">
-        <v>Invalid treatise datapack phylum provided.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
+      </c>
+      <c r="C338" t="str">
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B339" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Base age must be greater than the top age.</v>
+      </c>
+      <c r="C339" t="str">
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B340" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C340" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B341" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C341" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B342" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C342" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B343" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C343" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B344" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C344" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B345" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C345" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B346" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C346" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B347" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C347" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B348" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C348" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B349" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C349" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B350" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C350" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B351" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C351" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B352" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C352" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B354" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C354" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B355" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C355" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B356" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C356" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B357" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C357" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B358" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C358" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B359" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C359" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B360" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C360" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B361" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C361" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B362" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C362" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B363" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C363" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B364" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C364" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B367" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C367" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B368" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C368" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B369" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C369" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B370" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C370" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B371" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C371" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B372" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C372" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B373" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C373" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B374" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C374" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B375" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C375" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
-      </c>
-      <c r="C376" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C377" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B378" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C378" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B379" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C379" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B380" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C380" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B381" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B382" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B383" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B384" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C384" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B385" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B386" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C386" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B387" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
+      </c>
+      <c r="C387" t="str">
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B388" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C388" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B389" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
       </c>
       <c r="C389" t="str">
-        <v>不能删除根用户。</v>
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B390" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C390" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B391" t="str">
-        <v>Unable to modify user. Please try again later.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+      </c>
+      <c r="C391" t="str">
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B392" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
       </c>
       <c r="C392" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B393" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>The start date must be before the end date.</v>
       </c>
       <c r="C393" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B394" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to create workshop. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B395" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
       </c>
       <c r="C395" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B396" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B397" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
-      </c>
-      <c r="C397" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B398" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
       </c>
       <c r="C398" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B399" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
-      </c>
-      <c r="C399" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B400" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
-      </c>
-      <c r="C400" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B401" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
-      </c>
-      <c r="C401" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B402" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
-      </c>
-      <c r="C402" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B403" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
-      </c>
-      <c r="C403" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B404" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
-      </c>
-      <c r="C404" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B405" t="str">
-        <v>The start date must be before the end date.</v>
-      </c>
-      <c r="C405" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
-      </c>
-      <c r="C406" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B407" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
-      </c>
-      <c r="C407" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B408" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
-      </c>
-      <c r="C408" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B409" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B410" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
-      </c>
-      <c r="C410" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B411" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B412" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B413" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B414" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B415" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>No models available. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B416" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>button.generate</v>
       </c>
       <c r="B417" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Generate</v>
+      </c>
+      <c r="C417" t="str">
+        <v>绘制</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B418" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Generate Chart</v>
+      </c>
+      <c r="C418" t="str">
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B419" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Remove Cache</v>
+      </c>
+      <c r="C419" t="str">
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B420" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C420" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B421" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>yes</v>
       </c>
       <c r="B422" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Yes</v>
+      </c>
+      <c r="C422" t="str">
+        <v>是</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>no</v>
       </c>
       <c r="B423" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>No</v>
+      </c>
+      <c r="C423" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B424" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>English</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B425" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>English</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B426" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>tours.quit</v>
       </c>
       <c r="B427" t="str">
-        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
+        <v>Quit Tour</v>
+      </c>
+      <c r="C427" t="str">
+        <v>退出导览</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>tours.finish</v>
       </c>
       <c r="B428" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>Finish Tour</v>
+      </c>
+      <c r="C428" t="str">
+        <v>结束导览</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
+        <v>tours.next</v>
       </c>
       <c r="B429" t="str">
-        <v>Failed to add files to workshop</v>
+        <v>Next</v>
+      </c>
+      <c r="C429" t="str">
+        <v>下一步</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
+        <v>tours.back</v>
       </c>
       <c r="B430" t="str">
-        <v>Failed to add cover to workshop</v>
+        <v>Back</v>
+      </c>
+      <c r="C430" t="str">
+        <v>上一步</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>errors.INVALID_FILE_FORMAT</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B431" t="str">
-        <v>Invalid file format.</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+      </c>
+      <c r="C431" t="str">
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>errors.WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B432" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C432" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>errors.WORKSHOP_FILE_DOWNLOAD_NOT_AUTHORIZED</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B433" t="str">
-        <v>Please register for the workshop to download the file.</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+      </c>
+      <c r="C433" t="str">
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>errors.INVALID_DATAPACK_HASH</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B434" t="str">
-        <v>Invalid treatise datapack hash provided.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+      </c>
+      <c r="C434" t="str">
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>errors.USER_FETCH_HISTORY_FAILED</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B435" t="str">
-        <v>Failed to fetch user history. Please try again later.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+      </c>
+      <c r="C435" t="str">
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>errors.USER_DELETE_HISTORY_FAILED</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B436" t="str">
-        <v>Failed to delete user history. Please try again later</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+      </c>
+      <c r="C436" t="str">
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>errors.USER_FETCH_HISTORY_METADATA_FAILED</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B437" t="str">
-        <v>Failed to fetch user history metadata. Please try again later</v>
+        <v>The About Page provides information about our development team.</v>
+      </c>
+      <c r="C437" t="str">
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>errors.USER_FETCH_HISTORY_FAILED_DATAPACKS_MISSING</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B438" t="str">
-        <v>This chart entry couldn&amp;apos;t be loaded due to missing files and has been removed from your history.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+      </c>
+      <c r="C438" t="str">
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>button.generate</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B439" t="str">
-        <v>Generate</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C439" t="str">
-        <v>绘制</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>button.generate-chart</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B440" t="str">
-        <v>Generate Chart</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C440" t="str">
-        <v>绘制图表</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>button.remove-cache</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B441" t="str">
-        <v>Remove Cache</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C441" t="str">
-        <v>清除缓存</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>button.confirm-selection</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B442" t="str">
-        <v>Confirm Selection</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C442" t="str">
-        <v>确认选择</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B443" t="str">
-        <v>Generate Cross Plot</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+      </c>
+      <c r="C443" t="str">
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>yes</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B444" t="str">
-        <v>Yes</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C444" t="str">
-        <v>是</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>no</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B445" t="str">
-        <v>No</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C445" t="str">
-        <v>否</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>languageNames.en-US</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B446" t="str">
-        <v>English</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+      </c>
+      <c r="C446" t="str">
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>languageNames.en</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B447" t="str">
-        <v>English</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+      </c>
+      <c r="C447" t="str">
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>languageNames.zh</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B448" t="str">
-        <v>中文</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+      </c>
+      <c r="C448" t="str">
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.quit</v>
+        <v>tours.settings.step7</v>
       </c>
       <c r="B449" t="str">
-        <v>Quit Tour</v>
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C449" t="str">
-        <v>退出导览</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.finish</v>
-      </c>
-      <c r="B450" t="str">
-        <v>Finish Tour</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C450" t="str">
-        <v>结束导览</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.next</v>
-      </c>
-      <c r="B451" t="str">
-        <v>Next</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C451" t="str">
-        <v>下一步</v>
+        <v>English</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.back</v>
-      </c>
-      <c r="B452" t="str">
-        <v>Back</v>
+        <v>language-names.en</v>
       </c>
       <c r="C452" t="str">
-        <v>上一步</v>
+        <v>English</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.qsg.step1</v>
-      </c>
-      <c r="B453" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>language-names.zh</v>
       </c>
       <c r="C453" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" t="str">
-        <v>tours.qsg.step2</v>
-      </c>
-      <c r="B454" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
-      </c>
-      <c r="C454" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" t="str">
-        <v>tours.qsg.step3</v>
-      </c>
-      <c r="B455" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
-      </c>
-      <c r="C455" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" t="str">
-        <v>tours.qsg.step4</v>
-      </c>
-      <c r="B456" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
-      </c>
-      <c r="C456" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" t="str">
-        <v>tours.qsg.step5</v>
-      </c>
-      <c r="B457" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
-      </c>
-      <c r="C457" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" t="str">
-        <v>tours.qsg.step6</v>
-      </c>
-      <c r="B458" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
-      </c>
-      <c r="C458" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" t="str">
-        <v>tours.qsg.step7</v>
-      </c>
-      <c r="B459" t="str">
-        <v>The About Page provides information about our development team.</v>
-      </c>
-      <c r="C459" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" t="str">
-        <v>tours.qsg.step8</v>
-      </c>
-      <c r="B460" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
-      </c>
-      <c r="C460" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" t="str">
-        <v>tours.datapack.step1</v>
-      </c>
-      <c r="B461" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
-      </c>
-      <c r="C461" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" t="str">
-        <v>tours.datapack.step2</v>
-      </c>
-      <c r="B462" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
-      </c>
-      <c r="C462" t="str">
-        <v>勾选添加您想要的数据包</v>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" t="str">
-        <v>tours.datapack.step3</v>
-      </c>
-      <c r="B463" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
-      </c>
-      <c r="C463" t="str">
-        <v>点此取消选择所有数据包</v>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" t="str">
-        <v>tours.datapack.step4</v>
-      </c>
-      <c r="B464" t="str">
-        <v>Remember to confirm your selection</v>
-      </c>
-      <c r="C464" t="str">
-        <v>记得确认您的选择</v>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" t="str">
-        <v>tours.settings.step1</v>
-      </c>
-      <c r="B465" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
-      </c>
-      <c r="C465" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" t="str">
-        <v>tours.settings.step2</v>
-      </c>
-      <c r="B466" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
-      </c>
-      <c r="C466" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" t="str">
-        <v>tours.settings.step3</v>
-      </c>
-      <c r="B467" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
-      </c>
-      <c r="C467" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" t="str">
-        <v>tours.settings.step4</v>
-      </c>
-      <c r="B468" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
-      </c>
-      <c r="C468" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" t="str">
-        <v>tours.settings.step5</v>
-      </c>
-      <c r="B469" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
-      </c>
-      <c r="C469" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" t="str">
-        <v>tours.settings.step6</v>
-      </c>
-      <c r="B470" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
-      </c>
-      <c r="C470" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" t="str">
-        <v>tours.settings.step7</v>
-      </c>
-      <c r="B471" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
-      </c>
-      <c r="C471" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
-      </c>
-      <c r="C472" t="str">
-        <v>数据不在所选时间区间内</v>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" t="str">
-        <v>language-names.en-US</v>
-      </c>
-      <c r="C473" t="str">
-        <v>English</v>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" t="str">
-        <v>language-names.en</v>
-      </c>
-      <c r="C474" t="str">
-        <v>English</v>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" t="str">
-        <v>language-names.zh</v>
-      </c>
-      <c r="C475" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C475"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C453"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add minor fixes to frontend and test case additions
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C458"/>
+  <dimension ref="A1:C466"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1717,82 +1717,82 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B139" t="str">
-        <v>Create Datapack</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B140" t="str">
-        <v>No unit selected</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B141" t="str">
-        <v>Please select a unit.</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B142" t="str">
-        <v>No units available</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B143" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.xAxis</v>
       </c>
       <c r="B144" t="str">
-        <v>Please select a datapack.</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>crossPlot.time.xAxis</v>
+        <v>crossPlot.time.yAxis</v>
       </c>
       <c r="B145" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>crossPlot.time.yAxis</v>
+        <v>crossPlot.sidebar.no-markers</v>
       </c>
       <c r="B146" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>crossPlot.sidebar.no-markers</v>
+        <v>crossPlot.sidebar.no-models</v>
       </c>
       <c r="B147" t="str">
-        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
+        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>crossPlot.sidebar.no-models</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B148" t="str">
-        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="149">
@@ -1907,111 +1907,108 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Overlay</v>
       </c>
       <c r="B159" t="str">
-        <v>About</v>
-      </c>
-      <c r="C159" t="str">
-        <v>关于</v>
+        <v>Overlay</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B160" t="str">
-        <v>View Data</v>
+        <v>About</v>
       </c>
       <c r="C160" t="str">
-        <v>查看数据</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B161" t="str">
-        <v>Discussion</v>
+        <v>View Data</v>
       </c>
       <c r="C161" t="str">
-        <v>讨论</v>
+        <v>查看数据</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B162" t="str">
-        <v>Warnings</v>
+        <v>Discussion</v>
       </c>
       <c r="C162" t="str">
-        <v>警告</v>
+        <v>讨论</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B163" t="str">
-        <v>Load/Save</v>
+        <v>Warnings</v>
+      </c>
+      <c r="C163" t="str">
+        <v>警告</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B164" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B165" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B166" t="str">
-        <v>Top of Interval</v>
-      </c>
-      <c r="C166" t="str">
-        <v>区间顶部</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B167" t="str">
-        <v>Base of Interval</v>
+        <v>Top of Interval</v>
       </c>
       <c r="C167" t="str">
-        <v>区间底部</v>
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B168" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Base of Interval</v>
       </c>
       <c r="C168" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间底部</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B169" t="str">
-        <v>Base Age/Stage Name</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C169" t="str">
         <v>年代/阶段 名称</v>
@@ -2019,2235 +2016,2214 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B170" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C170" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B171" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C171" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B172" t="str">
-        <v>Base age should be older than top age</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
       </c>
       <c r="C172" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B173" t="str">
-        <v>Vertical Scale</v>
+        <v>Base age should be older than top age</v>
+      </c>
+      <c r="C173" t="str">
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B174" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
-      </c>
-      <c r="C174" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B175" t="str">
-        <v>Add MouseOver info (popups)</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C175" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B176" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Add MouseOver info (popups)</v>
       </c>
       <c r="C176" t="str">
-        <v>启用优先级过滤</v>
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B177" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C177" t="str">
-        <v>启用事件列的背景</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B178" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C178" t="str">
-        <v>启用添加图例</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B179" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C179" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B180" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C180" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B181" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C181" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B182" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C182" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B183" t="str">
-        <v>Load Settings</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C183" t="str">
-        <v>上传设置</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B184" t="str">
-        <v>Save Settings</v>
+        <v>Load Settings</v>
       </c>
       <c r="C184" t="str">
-        <v>保存设置</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B185" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>Save Settings</v>
       </c>
       <c r="C185" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B186" t="str">
-        <v>Cancel</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C186" t="str">
-        <v>取消</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B187" t="str">
-        <v>Load</v>
+        <v>Cancel</v>
       </c>
       <c r="C187" t="str">
-        <v>上传</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B188" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Load</v>
       </c>
       <c r="C188" t="str">
-        <v>请输入文件名</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B189" t="str">
-        <v>Cancel</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C189" t="str">
-        <v>取消</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B190" t="str">
-        <v>Save</v>
+        <v>Cancel</v>
       </c>
       <c r="C190" t="str">
-        <v>保存</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B191" t="str">
-        <v>Data not included in time range</v>
+        <v>Save</v>
+      </c>
+      <c r="C191" t="str">
+        <v>保存</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B192" t="str">
-        <v>Auto Scale</v>
-      </c>
-      <c r="C192" t="str">
-        <v>自动缩放</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B193" t="str">
-        <v>Flip Range</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C193" t="str">
-        <v>翻转区间</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B194" t="str">
-        <v>Column Customization</v>
+        <v>Flip Range</v>
       </c>
       <c r="C194" t="str">
-        <v>个性化设置列</v>
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B195" t="str">
-        <v>Data Mining Settings</v>
+        <v>Column Customization</v>
       </c>
       <c r="C195" t="str">
-        <v>数据挖掘设置</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C196" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B197" t="str">
-        <v>Shift Row Positions</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C197" t="str">
-        <v>移动位置</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B198" t="str">
-        <v>Edit Title</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C198" t="str">
-        <v>编辑标题</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B199" t="str">
-        <v>Background Color</v>
+        <v>Edit Title</v>
       </c>
       <c r="C199" t="str">
-        <v>背景颜色</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B200" t="str">
-        <v>Enable Title</v>
+        <v>Background Color</v>
       </c>
       <c r="C200" t="str">
-        <v>显示标题</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B201" t="str">
-        <v>Show Age Label</v>
+        <v>Enable Title</v>
       </c>
       <c r="C201" t="str">
-        <v>显示年代</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B202" t="str">
-        <v>Information and References</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C202" t="str">
-        <v>信息与参考</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B203" t="str">
-        <v>Add Blank Column</v>
+        <v>Information and References</v>
       </c>
       <c r="C203" t="str">
-        <v>添加一个空白列</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B204" t="str">
-        <v>Add Age Column</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C204" t="str">
-        <v>添加一个年代列</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B205" t="str">
-        <v>Width</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C205" t="str">
-        <v>宽</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B206" t="str">
-        <v>Label Orientation</v>
+        <v>Width</v>
       </c>
       <c r="C206" t="str">
-        <v>图标排布</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B207" t="str">
-        <v>Horizontal</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C207" t="str">
-        <v>横向</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B208" t="str">
-        <v>Vertical</v>
+        <v>Horizontal</v>
       </c>
       <c r="C208" t="str">
-        <v>纵向</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B209" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Vertical</v>
       </c>
       <c r="C209" t="str">
-        <v>显示不确定性</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B210" t="str">
-        <v>Events</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C210" t="str">
-        <v>事件</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B211" t="str">
-        <v>Ranges</v>
+        <v>Events</v>
       </c>
       <c r="C211" t="str">
-        <v>范围</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B212" t="str">
-        <v>First Occurrence</v>
+        <v>Ranges</v>
       </c>
       <c r="C212" t="str">
-        <v>首先发生的优先</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B213" t="str">
-        <v>Last Occurrence</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C213" t="str">
-        <v>最后发生的优先</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B214" t="str">
-        <v>Alphabetical</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C214" t="str">
-        <v>按字母顺序排列</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B215" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C215" t="str">
-        <v>调整年代刻度尺</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B216" t="str">
-        <v>Left</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C216" t="str">
-        <v>左对齐</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B217" t="str">
-        <v>Right</v>
+        <v>Left</v>
       </c>
       <c r="C217" t="str">
-        <v>右对齐</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B218" t="str">
-        <v>Change Font</v>
+        <v>Right</v>
       </c>
       <c r="C218" t="str">
-        <v>更改字体</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B219" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Change Font</v>
       </c>
       <c r="C219" t="str">
-        <v>子列的更多字体选项</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B220" t="str">
-        <v>Data Mining Settings</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C220" t="str">
-        <v>数据挖掘设置</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B221" t="str">
-        <v>Window Size</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C221" t="str">
-        <v>窗口大小</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B222" t="str">
-        <v>Step Size</v>
+        <v>Window Size</v>
       </c>
       <c r="C222" t="str">
-        <v>步长</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B223" t="str">
-        <v>Frequency</v>
+        <v>Step Size</v>
       </c>
       <c r="C223" t="str">
-        <v>频率</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B224" t="str">
-        <v>Maximum Value</v>
+        <v>Frequency</v>
       </c>
       <c r="C224" t="str">
-        <v>最大值</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B225" t="str">
-        <v>Minimum Value</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C225" t="str">
-        <v>最小值</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Average Value</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C226" t="str">
-        <v>平均值</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B227" t="str">
-        <v>Rate of Change</v>
+        <v>Average Value</v>
       </c>
       <c r="C227" t="str">
-        <v>变化率</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B228" t="str">
-        <v>Frequency of LAD</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C228" t="str">
-        <v>LAD 频率</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B229" t="str">
-        <v>Frequency of FAD</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C229" t="str">
-        <v>FAD 频率</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B230" t="str">
-        <v>Combined Events</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C230" t="str">
-        <v>组合事件</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B231" t="str">
-        <v>Event Type</v>
+        <v>Combined Events</v>
       </c>
       <c r="C231" t="str">
-        <v>事件类型</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B232" t="str">
-        <v>Chron Type</v>
+        <v>Event Type</v>
       </c>
       <c r="C232" t="str">
-        <v>年代类型</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B233" t="str">
-        <v>Data Type to Plot</v>
+        <v>Chron Type</v>
       </c>
       <c r="C233" t="str">
-        <v>绘制数据类型</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B234" t="str">
-        <v>Point Settings</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C234" t="str">
-        <v>点设置</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B235" t="str">
-        <v>Range of Data</v>
+        <v>Point Settings</v>
       </c>
       <c r="C235" t="str">
-        <v>数据范围</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B236" t="str">
-        <v>Lower Range</v>
+        <v>Range of Data</v>
       </c>
       <c r="C236" t="str">
-        <v>下限</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B237" t="str">
-        <v>Upper Range</v>
+        <v>Lower Range</v>
       </c>
       <c r="C237" t="str">
-        <v>上限</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B238" t="str">
-        <v>Scale Start</v>
+        <v>Upper Range</v>
       </c>
       <c r="C238" t="str">
-        <v>刻度起点</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B239" t="str">
-        <v>Scale Step</v>
+        <v>Scale Start</v>
       </c>
       <c r="C239" t="str">
-        <v>刻度步长</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B240" t="str">
-        <v>Show Scale</v>
+        <v>Scale Step</v>
       </c>
       <c r="C240" t="str">
-        <v>显示刻度</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B241" t="str">
-        <v>Draw Points</v>
+        <v>Show Scale</v>
       </c>
       <c r="C241" t="str">
-        <v>绘制点</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B242" t="str">
-        <v>Point Shape</v>
+        <v>Draw Points</v>
       </c>
       <c r="C242" t="str">
-        <v>点形状</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B243" t="str">
-        <v>Line</v>
+        <v>Point Shape</v>
       </c>
       <c r="C243" t="str">
-        <v>线条</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B244" t="str">
-        <v>Fill</v>
+        <v>Line</v>
       </c>
       <c r="C244" t="str">
-        <v>填充</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B245" t="str">
-        <v>Background Gradient</v>
+        <v>Fill</v>
       </c>
       <c r="C245" t="str">
-        <v>背景渐变</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B246" t="str">
-        <v>Curve Gradient</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C246" t="str">
-        <v>曲线渐变</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B247" t="str">
-        <v>Start</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C247" t="str">
-        <v>起点</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B248" t="str">
-        <v>End</v>
+        <v>Start</v>
       </c>
       <c r="C248" t="str">
-        <v>终点</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B249" t="str">
-        <v>Search</v>
+        <v>End</v>
       </c>
       <c r="C249" t="str">
-        <v>搜索</v>
+        <v>终点</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.column.overlay-menu.title</v>
       </c>
       <c r="B250" t="str">
-        <v>Found {{count}} Results</v>
-      </c>
-      <c r="C250" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>Overlay Settings</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.column.overlay-menu.display-overlay</v>
       </c>
       <c r="B251" t="str">
-        <v>Current Time Settings(Top / Base)</v>
-      </c>
-      <c r="C251" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>Display Overlay</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.column.overlay-menu.overlay-column-header</v>
       </c>
       <c r="B252" t="str">
-        <v>Column On?</v>
-      </c>
-      <c r="C252" t="str">
-        <v>是否已选</v>
+        <v>Overlaying</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.column.overlay-menu.overlay-column-preposition</v>
       </c>
       <c r="B253" t="str">
-        <v>Center</v>
-      </c>
-      <c r="C253" t="str">
-        <v>居中</v>
+        <v>On</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
       </c>
       <c r="B254" t="str">
-        <v>Extend</v>
-      </c>
-      <c r="C254" t="str">
-        <v>延展</v>
+        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
       </c>
       <c r="B255" t="str">
-        <v>Column</v>
-      </c>
-      <c r="C255" t="str">
-        <v>列名称</v>
+        <v>Not an Event or Point Column</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.column.overlay-menu.column-not-selected</v>
       </c>
       <c r="B256" t="str">
-        <v>Age</v>
-      </c>
-      <c r="C256" t="str">
-        <v>年代</v>
+        <v>Select Column from Menu</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B257" t="str">
-        <v>Type</v>
+        <v>Search</v>
       </c>
       <c r="C257" t="str">
-        <v>类别</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B258" t="str">
-        <v>Notes</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C258" t="str">
-        <v>注释</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B259" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Current Time Settings(Top / Base)</v>
       </c>
       <c r="C259" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B260" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>Column On?</v>
       </c>
       <c r="C260" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>是否已选</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B261" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>Center</v>
       </c>
       <c r="C261" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>居中</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B262" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>Extend</v>
       </c>
       <c r="C262" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>延展</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B263" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>Column</v>
       </c>
       <c r="C263" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>列名称</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B264" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Age</v>
       </c>
       <c r="C264" t="str">
-        <v>点击加号添加数据包</v>
+        <v>年代</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B265" t="str">
-        <v>Private Official Datapacks</v>
+        <v>Type</v>
+      </c>
+      <c r="C265" t="str">
+        <v>类别</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B266" t="str">
-        <v>Official Datapacks</v>
+        <v>Notes</v>
+      </c>
+      <c r="C266" t="str">
+        <v>注释</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B267" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>These are the default systemwide fonts.</v>
+      </c>
+      <c r="C267" t="str">
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B268" t="str">
-        <v>Workshop Datapacks</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C268" t="str">
-        <v>工作坊数据包</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B269" t="str">
-        <v>Your Datapacks</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C269" t="str">
-        <v>你的数据包</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B270" t="str">
-        <v>No</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C270" t="str">
-        <v>暂无</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B271" t="str">
-        <v>Avaliable</v>
+        <v>Click a datapack to see more information!</v>
       </c>
       <c r="C271" t="str">
-        <v>可用</v>
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B272" t="str">
-        <v>Upload Datapack</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C272" t="str">
-        <v>上传数据包</v>
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B273" t="str">
-        <v>PDF Upload</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B274" t="str">
-        <v>See More...</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B275" t="str">
-        <v>See Less...</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B276" t="str">
-        <v>Upload Your Own Datapack</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C276" t="str">
-        <v>上传你的数据包</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B277" t="str">
-        <v>No file selected</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C277" t="str">
-        <v>没有选择文件</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B278" t="str">
-        <v>Datapack Name</v>
+        <v>No</v>
       </c>
       <c r="C278" t="str">
-        <v>数据包名称</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B279" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Avaliable</v>
       </c>
       <c r="C279" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B280" t="str">
-        <v>Authored By</v>
+        <v>Upload Datapack</v>
       </c>
       <c r="C280" t="str">
-        <v>作者</v>
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B281" t="str">
-        <v>Credited to...</v>
-      </c>
-      <c r="C281" t="str">
-        <v>作者为...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B282" t="str">
-        <v>Datapack Description</v>
-      </c>
-      <c r="C282" t="str">
-        <v>数据包概述</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B283" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C283" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B284" t="str">
-        <v>Tags</v>
+        <v>No file selected</v>
       </c>
       <c r="C284" t="str">
-        <v>标签</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B285" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C285" t="str">
-        <v>使数据包对公共可见</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B286" t="str">
-        <v>Add Reference</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C286" t="str">
-        <v>添加引用</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B287" t="str">
-        <v>More Options</v>
+        <v>Authored By</v>
       </c>
       <c r="C287" t="str">
-        <v>更多选项</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B288" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>Credited to...</v>
       </c>
       <c r="C288" t="str">
-        <v>完成并上传</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B289" t="str">
-        <v>Start Over</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C289" t="str">
-        <v>重新开始</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B290" t="str">
-        <v>Reference</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C290" t="str">
-        <v>引用</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B291" t="str">
-        <v>Contact</v>
+        <v>Tags</v>
       </c>
       <c r="C291" t="str">
-        <v>联系方式</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B292" t="str">
-        <v>Enter your contact information</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C292" t="str">
-        <v>输入你的联系方式</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B293" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Add Reference</v>
       </c>
       <c r="C293" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B294" t="str">
-        <v>Notes</v>
+        <v>More Options</v>
       </c>
       <c r="C294" t="str">
-        <v>注释</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B295" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C295" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B296" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Start Over</v>
       </c>
       <c r="C296" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B297" t="str">
-        <v>You have not made a chart yet</v>
+        <v>Reference</v>
       </c>
       <c r="C297" t="str">
-        <v>您还未制作任何图表</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>chart.save</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B298" t="str">
-        <v>Save Chart</v>
+        <v>Contact</v>
       </c>
       <c r="C298" t="str">
-        <v>保存图表</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B299" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C299" t="str">
-        <v>确认更改数据包</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B300" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C300" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B301" t="str">
-        <v>Save</v>
+        <v>Notes</v>
       </c>
       <c r="C301" t="str">
-        <v>保存</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B302" t="str">
-        <v>Discard</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C302" t="str">
-        <v>不保存</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B303" t="str">
-        <v>Use default age range?</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C303" t="str">
-        <v>使用默认时间区间？</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B304" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>help.qsg.title</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B305" t="str">
-        <v>Quick Start Quide</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C305" t="str">
-        <v>快速指南</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>help.qsg.content</v>
+        <v>chart.save</v>
       </c>
       <c r="B306" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Save Chart</v>
       </c>
       <c r="C306" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>help.qsg.button</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B307" t="str">
-        <v>Start QSG</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C307" t="str">
-        <v>开始快速指南</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>help.tour.title</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B308" t="str">
-        <v>Tour</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C308" t="str">
-        <v>导览</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B309" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Save</v>
       </c>
       <c r="C309" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>help.tour.content.settings</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B310" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>Discard</v>
       </c>
       <c r="C310" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B311" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>Use default age range?</v>
       </c>
       <c r="C311" t="str">
-        <v>开始数据包导览</v>
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>help.tour.button.settings</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B312" t="str">
-        <v>Start Settings Tour</v>
-      </c>
-      <c r="C312" t="str">
-        <v>开始设置导览</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.license</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B313" t="str">
-        <v>Software License</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C313" t="str">
-        <v>软件许可</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B314" t="str">
-        <v>File Format Info</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C314" t="str">
-        <v>文件格式信息</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B315" t="str">
-        <v>View File Format Info</v>
+        <v>Start QSG</v>
       </c>
       <c r="C315" t="str">
-        <v>查看文件格式信息</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>errors.title</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B316" t="str">
-        <v>Error</v>
+        <v>Tour</v>
       </c>
       <c r="C316" t="str">
-        <v>错误</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B317" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C317" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B318" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C318" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B319" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C319" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B320" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C320" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>help.license</v>
       </c>
       <c r="B321" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Software License</v>
       </c>
       <c r="C321" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B322" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>File Format Info</v>
       </c>
       <c r="C322" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B323" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C323" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.title</v>
       </c>
       <c r="B324" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C324" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B325" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C325" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B326" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C326" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C327" t="str">
-        <v>无效的数据包上传</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B328" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
+      </c>
+      <c r="C328" t="str">
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B331" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B332" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B333" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C333" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B334" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C334" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B335" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Invalid datapack upload.</v>
       </c>
       <c r="C335" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B336" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
-      </c>
-      <c r="C336" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B337" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C337" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B338" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C338" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B339" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C339" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B340" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C340" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B341" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C341" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B342" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C342" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B343" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C343" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B344" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C344" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B345" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C345" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B346" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C346" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B347" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C347" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B348" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C348" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B349" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C349" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B350" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C350" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B351" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C351" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B352" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C352" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C354" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C355" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B356" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C356" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B357" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C357" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B358" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C358" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B359" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C359" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B360" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C360" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B361" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C361" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B362" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B363" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C363" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B364" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C364" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B367" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C367" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B368" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C368" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B369" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C369" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B370" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C370" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B371" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C371" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B372" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C372" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B373" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C373" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B374" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C374" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C375" t="str">
         <v>无法删除用户。请稍后再试。</v>
@@ -4255,824 +4231,912 @@
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Incorrect password. Please try again.</v>
+      </c>
+      <c r="C376" t="str">
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C377" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B378" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C378" t="str">
-        <v>不能删除根用户。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B379" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to modify user. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
+      </c>
+      <c r="C380" t="str">
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B381" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B382" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B383" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B384" t="str">
-        <v>Server file metadata error. Please try again later.</v>
-      </c>
-      <c r="C384" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B385" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B386" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C386" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B387" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C387" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
       </c>
       <c r="B388" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
-      </c>
-      <c r="C388" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>Unable to modify user. Please try again later.</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B389" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C389" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B390" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C390" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B391" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C391" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B392" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C392" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B393" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C393" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B394" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B395" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C395" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B396" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C397" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B398" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
+      </c>
+      <c r="C398" t="str">
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B399" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C399" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B400" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+      </c>
+      <c r="C400" t="str">
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B401" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+      </c>
+      <c r="C401" t="str">
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B402" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>The start date must be before the end date.</v>
+      </c>
+      <c r="C402" t="str">
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B403" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Unable to create workshop. Please try again later.</v>
+      </c>
+      <c r="C403" t="str">
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B404" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
+      </c>
+      <c r="C404" t="str">
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B405" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C405" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B407" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C407" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B408" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B410" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B411" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B413" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B414" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B415" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B416" t="str">
-        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B417" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B418" t="str">
-        <v>Failed to add files to workshop</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B419" t="str">
-        <v>Failed to add cover to workshop</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>errors.INVALID_FILE_FORMAT</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B420" t="str">
-        <v>Invalid file format.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B421" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
-      </c>
-      <c r="C421" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>button.generate</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B422" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C422" t="str">
-        <v>绘制</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B423" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C423" t="str">
-        <v>绘制图表</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>button.remove-cache</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B424" t="str">
-        <v>Remove Cache</v>
-      </c>
-      <c r="C424" t="str">
-        <v>清除缓存</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>button.confirm-selection</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B425" t="str">
-        <v>Confirm Selection</v>
-      </c>
-      <c r="C425" t="str">
-        <v>确认选择</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B426" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Failed to add files to workshop</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>yes</v>
+        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B427" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C427" t="str">
-        <v>是</v>
+        <v>Failed to add cover to workshop</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>no</v>
+        <v>errors.INVALID_FILE_FORMAT</v>
       </c>
       <c r="B428" t="str">
-        <v>No</v>
-      </c>
-      <c r="C428" t="str">
-        <v>否</v>
+        <v>Invalid file format.</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>languageNames.en-US</v>
+        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B429" t="str">
-        <v>English</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
+      </c>
+      <c r="C429" t="str">
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>languageNames.en</v>
+        <v>button.generate</v>
       </c>
       <c r="B430" t="str">
-        <v>English</v>
+        <v>Generate</v>
+      </c>
+      <c r="C430" t="str">
+        <v>绘制</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>languageNames.zh</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B431" t="str">
-        <v>中文</v>
+        <v>Generate Chart</v>
+      </c>
+      <c r="C431" t="str">
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.quit</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B432" t="str">
-        <v>Quit Tour</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C432" t="str">
-        <v>退出导览</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.finish</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B433" t="str">
-        <v>Finish Tour</v>
+        <v>Confirm Selection</v>
       </c>
       <c r="C433" t="str">
-        <v>结束导览</v>
+        <v>确认选择</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.next</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B434" t="str">
-        <v>Next</v>
-      </c>
-      <c r="C434" t="str">
-        <v>下一步</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.back</v>
+        <v>yes</v>
       </c>
       <c r="B435" t="str">
-        <v>Back</v>
+        <v>Yes</v>
       </c>
       <c r="C435" t="str">
-        <v>上一步</v>
+        <v>是</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step1</v>
+        <v>no</v>
       </c>
       <c r="B436" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>No</v>
       </c>
       <c r="C436" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>否</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.qsg.step2</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B437" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
-      </c>
-      <c r="C437" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.qsg.step3</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B438" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
-      </c>
-      <c r="C438" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.qsg.step4</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B439" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
-      </c>
-      <c r="C439" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.quit</v>
       </c>
       <c r="B440" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C440" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.finish</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C441" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.next</v>
       </c>
       <c r="B442" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>Next</v>
       </c>
       <c r="C442" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.back</v>
       </c>
       <c r="B443" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>Back</v>
       </c>
       <c r="C443" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B444" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C444" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B445" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C445" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B446" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C446" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B447" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C447" t="str">
-        <v>记得确认您的选择</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C448" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C449" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B450" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C450" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B451" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C451" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B452" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C452" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B453" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C453" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B454" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C454" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.datapack.step4</v>
+      </c>
+      <c r="B455" t="str">
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C455" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.settings.step1</v>
+      </c>
+      <c r="B456" t="str">
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C456" t="str">
-        <v>English</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="str">
-        <v>language-names.en</v>
+        <v>tours.settings.step2</v>
+      </c>
+      <c r="B457" t="str">
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C457" t="str">
-        <v>English</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="str">
+        <v>tours.settings.step3</v>
+      </c>
+      <c r="B458" t="str">
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+      </c>
+      <c r="C458" t="str">
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="str">
+        <v>tours.settings.step4</v>
+      </c>
+      <c r="B459" t="str">
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+      </c>
+      <c r="C459" t="str">
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="str">
+        <v>tours.settings.step5</v>
+      </c>
+      <c r="B460" t="str">
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+      </c>
+      <c r="C460" t="str">
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="str">
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B461" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+      </c>
+      <c r="C461" t="str">
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="str">
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B462" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+      </c>
+      <c r="C462" t="str">
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="str">
+        <v>settings.column.tooltip.note-in-range</v>
+      </c>
+      <c r="C463" t="str">
+        <v>数据不在所选时间区间内</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C464" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C465" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C458" t="str">
+      <c r="C466" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C458"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C466"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new display for treatise and changed display of datapack for ogg
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C454"/>
+  <dimension ref="A1:C455"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3104,1639 +3104,1639 @@
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.datapacks.title.treatise</v>
       </c>
       <c r="B270" t="str">
-        <v>No</v>
-      </c>
-      <c r="C270" t="str">
-        <v>暂无</v>
+        <v>Treatise Datapacks</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B271" t="str">
-        <v>Avaliable</v>
+        <v>No</v>
       </c>
       <c r="C271" t="str">
-        <v>可用</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B272" t="str">
-        <v>Upload Datapack</v>
+        <v>Avaliable</v>
       </c>
       <c r="C272" t="str">
-        <v>上传数据包</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B273" t="str">
-        <v>PDF Upload</v>
+        <v>Upload Datapack</v>
+      </c>
+      <c r="C273" t="str">
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B274" t="str">
-        <v>See More...</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B275" t="str">
-        <v>See Less...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B276" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C276" t="str">
-        <v>上传你的数据包</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B277" t="str">
-        <v>No file selected</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C277" t="str">
-        <v>没有选择文件</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B278" t="str">
-        <v>Datapack Name</v>
+        <v>No file selected</v>
       </c>
       <c r="C278" t="str">
-        <v>数据包名称</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B279" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C279" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B280" t="str">
-        <v>Authored By</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C280" t="str">
-        <v>作者</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B281" t="str">
-        <v>Credited to...</v>
+        <v>Authored By</v>
       </c>
       <c r="C281" t="str">
-        <v>作者为...</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B282" t="str">
-        <v>Datapack Description</v>
+        <v>Credited to...</v>
       </c>
       <c r="C282" t="str">
-        <v>数据包概述</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B283" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C283" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B284" t="str">
-        <v>Tags</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C284" t="str">
-        <v>标签</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B285" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Tags</v>
       </c>
       <c r="C285" t="str">
-        <v>使数据包对公共可见</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B286" t="str">
-        <v>Add Reference</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C286" t="str">
-        <v>添加引用</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B287" t="str">
-        <v>More Options</v>
+        <v>Add Reference</v>
       </c>
       <c r="C287" t="str">
-        <v>更多选项</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B288" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>More Options</v>
       </c>
       <c r="C288" t="str">
-        <v>完成并上传</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B289" t="str">
-        <v>Start Over</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C289" t="str">
-        <v>重新开始</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B290" t="str">
-        <v>Reference</v>
+        <v>Start Over</v>
       </c>
       <c r="C290" t="str">
-        <v>引用</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B291" t="str">
-        <v>Contact</v>
+        <v>Reference</v>
       </c>
       <c r="C291" t="str">
-        <v>联系方式</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B292" t="str">
-        <v>Enter your contact information</v>
+        <v>Contact</v>
       </c>
       <c r="C292" t="str">
-        <v>输入你的联系方式</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B293" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C293" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B294" t="str">
-        <v>Notes</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C294" t="str">
-        <v>注释</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B295" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Notes</v>
       </c>
       <c r="C295" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B296" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C296" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B297" t="str">
-        <v>You have not made a chart yet</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C297" t="str">
-        <v>您还未制作任何图表</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>chart.save</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B298" t="str">
-        <v>Save Chart</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C298" t="str">
-        <v>保存图表</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>chart.save</v>
       </c>
       <c r="B299" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Save Chart</v>
       </c>
       <c r="C299" t="str">
-        <v>确认更改数据包</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B300" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C300" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B301" t="str">
-        <v>Save</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C301" t="str">
-        <v>保存</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B302" t="str">
-        <v>Discard</v>
+        <v>Save</v>
       </c>
       <c r="C302" t="str">
-        <v>不保存</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B303" t="str">
-        <v>Use default age range?</v>
+        <v>Discard</v>
       </c>
       <c r="C303" t="str">
-        <v>使用默认时间区间？</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B304" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>Use default age range?</v>
+      </c>
+      <c r="C304" t="str">
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>help.qsg.title</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B305" t="str">
-        <v>Quick Start Quide</v>
-      </c>
-      <c r="C305" t="str">
-        <v>快速指南</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>help.qsg.content</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B306" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C306" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>help.qsg.button</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B307" t="str">
-        <v>Start QSG</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C307" t="str">
-        <v>开始快速指南</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>help.tour.title</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B308" t="str">
-        <v>Tour</v>
+        <v>Start QSG</v>
       </c>
       <c r="C308" t="str">
-        <v>导览</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B309" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Tour</v>
       </c>
       <c r="C309" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>help.tour.content.settings</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B310" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C310" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B311" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C311" t="str">
-        <v>开始数据包导览</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>help.tour.button.settings</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B312" t="str">
-        <v>Start Settings Tour</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C312" t="str">
-        <v>开始设置导览</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.license</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B313" t="str">
-        <v>Software License</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C313" t="str">
-        <v>软件许可</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.license</v>
       </c>
       <c r="B314" t="str">
-        <v>File Format Info</v>
+        <v>Software License</v>
       </c>
       <c r="C314" t="str">
-        <v>文件格式信息</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B315" t="str">
-        <v>View File Format Info</v>
+        <v>File Format Info</v>
       </c>
       <c r="C315" t="str">
-        <v>查看文件格式信息</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>errors.title</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B316" t="str">
-        <v>Error</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C316" t="str">
-        <v>错误</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>errors.title</v>
       </c>
       <c r="B317" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C317" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B318" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C318" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B319" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C319" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B320" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C320" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B321" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C321" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B322" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C322" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B323" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C323" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B324" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C324" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B325" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C325" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B326" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C326" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C327" t="str">
-        <v>无效的数据包上传</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.INVALID_DATAPACK_HASH</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B328" t="str">
-        <v>Invalid treatise datapack hash provided.</v>
+        <v>Invalid datapack upload.</v>
+      </c>
+      <c r="C328" t="str">
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_DATAPACK_HASH</v>
       </c>
       <c r="B329" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid treatise datapack hash provided.</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
-      </c>
-      <c r="C330" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B331" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B332" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B333" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C333" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B334" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C334" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B335" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C335" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B336" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C336" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B337" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C337" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B338" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C338" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B339" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C339" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B340" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C340" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B341" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C341" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B342" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C342" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B343" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C343" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B344" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C344" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B345" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C345" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B346" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C346" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B347" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C347" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B348" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C348" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B349" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C349" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B350" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C350" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B351" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C351" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B352" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C352" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B353" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C353" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C354" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C355" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B356" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C356" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B357" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C357" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B358" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C358" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B359" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C359" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B360" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C360" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B361" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C361" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B362" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B363" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C363" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B364" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C364" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B365" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C365" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B367" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C367" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B368" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C368" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B369" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C369" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B370" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C370" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B371" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C371" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B372" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C372" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B373" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C373" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B374" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C374" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B375" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C375" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C376" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
+      </c>
+      <c r="C377" t="str">
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B378" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
-      </c>
-      <c r="C378" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B379" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C379" t="str">
-        <v>不能删除根用户。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C380" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B381" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B382" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B383" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C383" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B384" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C384" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B385" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B386" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C386" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B387" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C387" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B388" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C388" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B389" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C389" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B390" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C390" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B391" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
       </c>
       <c r="C391" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B392" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C392" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B393" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
       </c>
       <c r="C393" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B394" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
       </c>
       <c r="C394" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B395" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>The start date must be before the end date.</v>
       </c>
       <c r="C395" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B396" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>Unable to create workshop. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
       </c>
       <c r="C397" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B398" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C398" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B399" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
-      </c>
-      <c r="C399" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B400" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C400" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B401" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B402" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B403" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B404" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B405" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B406" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B407" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B408" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B410" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B411" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B413" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B414" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B415" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B416" t="str">
-        <v>No models available. Please add a model by clicking the chart in the main view.</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B417" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>No models available. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>button.generate</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B418" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C418" t="str">
-        <v>绘制</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>button.generate-chart</v>
+        <v>button.generate</v>
       </c>
       <c r="B419" t="str">
-        <v>Generate Chart</v>
+        <v>Generate</v>
       </c>
       <c r="C419" t="str">
-        <v>绘制图表</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B420" t="str">
-        <v>Remove Cache</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C420" t="str">
-        <v>清除缓存</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B421" t="str">
-        <v>Confirm Selection</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C421" t="str">
-        <v>确认选择</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B422" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C422" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>yes</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B423" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C423" t="str">
-        <v>是</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="B424" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="C424" t="str">
-        <v>否</v>
+        <v>是</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>languageNames.en-US</v>
+        <v>no</v>
       </c>
       <c r="B425" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C425" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>languageNames.en</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B426" t="str">
         <v>English</v>
@@ -4744,284 +4744,284 @@
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B427" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B428" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C428" t="str">
-        <v>退出导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.finish</v>
+        <v>tours.quit</v>
       </c>
       <c r="B429" t="str">
-        <v>Finish Tour</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C429" t="str">
-        <v>结束导览</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.next</v>
+        <v>tours.finish</v>
       </c>
       <c r="B430" t="str">
-        <v>Next</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C430" t="str">
-        <v>下一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.back</v>
+        <v>tours.next</v>
       </c>
       <c r="B431" t="str">
-        <v>Back</v>
+        <v>Next</v>
       </c>
       <c r="C431" t="str">
-        <v>上一步</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B432" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Back</v>
       </c>
       <c r="C432" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B433" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C433" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B434" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C434" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B435" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C435" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B436" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C436" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B437" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C437" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B438" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C438" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B439" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C439" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B440" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C440" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B441" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C441" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B442" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C442" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B443" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C443" t="str">
-        <v>记得确认您的选择</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B444" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C444" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B445" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C445" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B446" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C446" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B447" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C447" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B448" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C448" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C449" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B450" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C450" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B451" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C451" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>language-names.en-US</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C452" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>language-names.en</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C453" t="str">
         <v>English</v>
@@ -5029,15 +5029,23 @@
     </row>
     <row r="454">
       <c r="A454" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C454" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C454" t="str">
+      <c r="C455" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C454"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C455"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed dsiplay name of treatise
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C460"/>
+  <dimension ref="A1:C461"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3738,10 +3738,10 @@
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_DATAPACK_HASH</v>
+        <v>errors.INVALID_DATAPACK_PHYLUM</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid treatise datapack hash provided.</v>
+        <v>Invalid treatise datapack phylum provided.</v>
       </c>
     </row>
     <row r="330">
@@ -4657,7 +4657,7 @@
         <v>errors.NO_MODELS</v>
       </c>
       <c r="B418" t="str">
-        <v>No models available. Please add a model by clicking the chart in the main view.</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="419">
@@ -4705,89 +4705,89 @@
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>button.generate</v>
+        <v>errors.INVALID_DATAPACK_HASH</v>
       </c>
       <c r="B424" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C424" t="str">
-        <v>绘制</v>
+        <v>Invalid treatise datapack hash provided.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>button.generate-chart</v>
+        <v>button.generate</v>
       </c>
       <c r="B425" t="str">
-        <v>Generate Chart</v>
+        <v>Generate</v>
       </c>
       <c r="C425" t="str">
-        <v>绘制图表</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>button.remove-cache</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B426" t="str">
-        <v>Remove Cache</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C426" t="str">
-        <v>清除缓存</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B427" t="str">
-        <v>Confirm Selection</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C427" t="str">
-        <v>确认选择</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B428" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C428" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>yes</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B429" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C429" t="str">
-        <v>是</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="B430" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="C430" t="str">
-        <v>否</v>
+        <v>是</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>languageNames.en-US</v>
+        <v>no</v>
       </c>
       <c r="B431" t="str">
-        <v>English</v>
+        <v>No</v>
+      </c>
+      <c r="C431" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>languageNames.en</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B432" t="str">
         <v>English</v>
@@ -4795,284 +4795,284 @@
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>languageNames.zh</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B433" t="str">
-        <v>中文</v>
+        <v>English</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B434" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C434" t="str">
-        <v>退出导览</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.finish</v>
+        <v>tours.quit</v>
       </c>
       <c r="B435" t="str">
-        <v>Finish Tour</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C435" t="str">
-        <v>结束导览</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.next</v>
+        <v>tours.finish</v>
       </c>
       <c r="B436" t="str">
-        <v>Next</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C436" t="str">
-        <v>下一步</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.back</v>
+        <v>tours.next</v>
       </c>
       <c r="B437" t="str">
-        <v>Back</v>
+        <v>Next</v>
       </c>
       <c r="C437" t="str">
-        <v>上一步</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B438" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Back</v>
       </c>
       <c r="C438" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B439" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C439" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B440" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C440" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C441" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B442" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C442" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B443" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C443" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B444" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C444" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B445" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C445" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B446" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C446" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B447" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C447" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B448" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C448" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B449" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C449" t="str">
-        <v>记得确认您的选择</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B450" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C450" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B451" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C451" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B452" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C452" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B453" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C453" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B454" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C454" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step5</v>
       </c>
       <c r="B455" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C455" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step6</v>
       </c>
       <c r="B456" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C456" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B457" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C457" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="str">
-        <v>language-names.en-US</v>
+        <v>settings.column.tooltip.note-in-range</v>
       </c>
       <c r="C458" t="str">
-        <v>English</v>
+        <v>数据不在所选时间区间内</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="str">
-        <v>language-names.en</v>
+        <v>language-names.en-US</v>
       </c>
       <c r="C459" t="str">
         <v>English</v>
@@ -5080,15 +5080,23 @@
     </row>
     <row r="460">
       <c r="A460" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C460" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C460" t="str">
+      <c r="C461" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C460"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C461"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removing recaptcha from workshops and refactoring
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C458"/>
+  <dimension ref="A1:C467"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1717,82 +1717,82 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B139" t="str">
-        <v>Create Datapack</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B140" t="str">
-        <v>No unit selected</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B141" t="str">
-        <v>Please select a unit.</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B142" t="str">
-        <v>No units available</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B143" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.xAxis</v>
       </c>
       <c r="B144" t="str">
-        <v>Please select a datapack.</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>crossPlot.time.xAxis</v>
+        <v>crossPlot.time.yAxis</v>
       </c>
       <c r="B145" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>crossPlot.time.yAxis</v>
+        <v>crossPlot.sidebar.no-markers</v>
       </c>
       <c r="B146" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>crossPlot.sidebar.no-markers</v>
+        <v>crossPlot.sidebar.no-models</v>
       </c>
       <c r="B147" t="str">
-        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
+        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>crossPlot.sidebar.no-models</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B148" t="str">
-        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="149">
@@ -1907,111 +1907,108 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Overlay</v>
       </c>
       <c r="B159" t="str">
-        <v>About</v>
-      </c>
-      <c r="C159" t="str">
-        <v>关于</v>
+        <v>Overlay</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B160" t="str">
-        <v>View Data</v>
+        <v>About</v>
       </c>
       <c r="C160" t="str">
-        <v>查看数据</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B161" t="str">
-        <v>Discussion</v>
+        <v>View Data</v>
       </c>
       <c r="C161" t="str">
-        <v>讨论</v>
+        <v>查看数据</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B162" t="str">
-        <v>Warnings</v>
+        <v>Discussion</v>
       </c>
       <c r="C162" t="str">
-        <v>警告</v>
+        <v>讨论</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B163" t="str">
-        <v>Load/Save</v>
+        <v>Warnings</v>
+      </c>
+      <c r="C163" t="str">
+        <v>警告</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B164" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B165" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B166" t="str">
-        <v>Top of Interval</v>
-      </c>
-      <c r="C166" t="str">
-        <v>区间顶部</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B167" t="str">
-        <v>Base of Interval</v>
+        <v>Top of Interval</v>
       </c>
       <c r="C167" t="str">
-        <v>区间底部</v>
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B168" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Base of Interval</v>
       </c>
       <c r="C168" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间底部</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B169" t="str">
-        <v>Base Age/Stage Name</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C169" t="str">
         <v>年代/阶段 名称</v>
@@ -2019,2235 +2016,2214 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B170" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C170" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B171" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C171" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B172" t="str">
-        <v>Base age should be older than top age</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
       </c>
       <c r="C172" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B173" t="str">
-        <v>Vertical Scale</v>
+        <v>Base age should be older than top age</v>
+      </c>
+      <c r="C173" t="str">
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B174" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
-      </c>
-      <c r="C174" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B175" t="str">
-        <v>Add MouseOver info (popups)</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C175" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B176" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Add MouseOver info (popups)</v>
       </c>
       <c r="C176" t="str">
-        <v>启用优先级过滤</v>
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B177" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C177" t="str">
-        <v>启用事件列的背景</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B178" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C178" t="str">
-        <v>启用添加图例</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B179" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C179" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B180" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C180" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B181" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C181" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B182" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C182" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B183" t="str">
-        <v>Load Settings</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C183" t="str">
-        <v>上传设置</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B184" t="str">
-        <v>Save Settings</v>
+        <v>Load Settings</v>
       </c>
       <c r="C184" t="str">
-        <v>保存设置</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B185" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>Save Settings</v>
       </c>
       <c r="C185" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B186" t="str">
-        <v>Cancel</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C186" t="str">
-        <v>取消</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B187" t="str">
-        <v>Load</v>
+        <v>Cancel</v>
       </c>
       <c r="C187" t="str">
-        <v>上传</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B188" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Load</v>
       </c>
       <c r="C188" t="str">
-        <v>请输入文件名</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B189" t="str">
-        <v>Cancel</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C189" t="str">
-        <v>取消</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B190" t="str">
-        <v>Save</v>
+        <v>Cancel</v>
       </c>
       <c r="C190" t="str">
-        <v>保存</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B191" t="str">
-        <v>Data not included in time range</v>
+        <v>Save</v>
+      </c>
+      <c r="C191" t="str">
+        <v>保存</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B192" t="str">
-        <v>Auto Scale</v>
-      </c>
-      <c r="C192" t="str">
-        <v>自动缩放</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B193" t="str">
-        <v>Flip Range</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C193" t="str">
-        <v>翻转区间</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B194" t="str">
-        <v>Column Customization</v>
+        <v>Flip Range</v>
       </c>
       <c r="C194" t="str">
-        <v>个性化设置列</v>
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B195" t="str">
-        <v>Data Mining Settings</v>
+        <v>Column Customization</v>
       </c>
       <c r="C195" t="str">
-        <v>数据挖掘设置</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C196" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B197" t="str">
-        <v>Shift Row Positions</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C197" t="str">
-        <v>移动位置</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B198" t="str">
-        <v>Edit Title</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C198" t="str">
-        <v>编辑标题</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B199" t="str">
-        <v>Background Color</v>
+        <v>Edit Title</v>
       </c>
       <c r="C199" t="str">
-        <v>背景颜色</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B200" t="str">
-        <v>Enable Title</v>
+        <v>Background Color</v>
       </c>
       <c r="C200" t="str">
-        <v>显示标题</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B201" t="str">
-        <v>Show Age Label</v>
+        <v>Enable Title</v>
       </c>
       <c r="C201" t="str">
-        <v>显示年代</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B202" t="str">
-        <v>Information and References</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C202" t="str">
-        <v>信息与参考</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B203" t="str">
-        <v>Add Blank Column</v>
+        <v>Information and References</v>
       </c>
       <c r="C203" t="str">
-        <v>添加一个空白列</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B204" t="str">
-        <v>Add Age Column</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C204" t="str">
-        <v>添加一个年代列</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B205" t="str">
-        <v>Width</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C205" t="str">
-        <v>宽</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B206" t="str">
-        <v>Label Orientation</v>
+        <v>Width</v>
       </c>
       <c r="C206" t="str">
-        <v>图标排布</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B207" t="str">
-        <v>Horizontal</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C207" t="str">
-        <v>横向</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B208" t="str">
-        <v>Vertical</v>
+        <v>Horizontal</v>
       </c>
       <c r="C208" t="str">
-        <v>纵向</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B209" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Vertical</v>
       </c>
       <c r="C209" t="str">
-        <v>显示不确定性</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B210" t="str">
-        <v>Events</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C210" t="str">
-        <v>事件</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B211" t="str">
-        <v>Ranges</v>
+        <v>Events</v>
       </c>
       <c r="C211" t="str">
-        <v>范围</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B212" t="str">
-        <v>First Occurrence</v>
+        <v>Ranges</v>
       </c>
       <c r="C212" t="str">
-        <v>首先发生的优先</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B213" t="str">
-        <v>Last Occurrence</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C213" t="str">
-        <v>最后发生的优先</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B214" t="str">
-        <v>Alphabetical</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C214" t="str">
-        <v>按字母顺序排列</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B215" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C215" t="str">
-        <v>调整年代刻度尺</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B216" t="str">
-        <v>Left</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C216" t="str">
-        <v>左对齐</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B217" t="str">
-        <v>Right</v>
+        <v>Left</v>
       </c>
       <c r="C217" t="str">
-        <v>右对齐</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B218" t="str">
-        <v>Change Font</v>
+        <v>Right</v>
       </c>
       <c r="C218" t="str">
-        <v>更改字体</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B219" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Change Font</v>
       </c>
       <c r="C219" t="str">
-        <v>子列的更多字体选项</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B220" t="str">
-        <v>Data Mining Settings</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C220" t="str">
-        <v>数据挖掘设置</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B221" t="str">
-        <v>Window Size</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C221" t="str">
-        <v>窗口大小</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B222" t="str">
-        <v>Step Size</v>
+        <v>Window Size</v>
       </c>
       <c r="C222" t="str">
-        <v>步长</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B223" t="str">
-        <v>Frequency</v>
+        <v>Step Size</v>
       </c>
       <c r="C223" t="str">
-        <v>频率</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B224" t="str">
-        <v>Maximum Value</v>
+        <v>Frequency</v>
       </c>
       <c r="C224" t="str">
-        <v>最大值</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B225" t="str">
-        <v>Minimum Value</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C225" t="str">
-        <v>最小值</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Average Value</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C226" t="str">
-        <v>平均值</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B227" t="str">
-        <v>Rate of Change</v>
+        <v>Average Value</v>
       </c>
       <c r="C227" t="str">
-        <v>变化率</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B228" t="str">
-        <v>Frequency of LAD</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C228" t="str">
-        <v>LAD 频率</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B229" t="str">
-        <v>Frequency of FAD</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C229" t="str">
-        <v>FAD 频率</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B230" t="str">
-        <v>Combined Events</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C230" t="str">
-        <v>组合事件</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B231" t="str">
-        <v>Event Type</v>
+        <v>Combined Events</v>
       </c>
       <c r="C231" t="str">
-        <v>事件类型</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B232" t="str">
-        <v>Chron Type</v>
+        <v>Event Type</v>
       </c>
       <c r="C232" t="str">
-        <v>年代类型</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B233" t="str">
-        <v>Data Type to Plot</v>
+        <v>Chron Type</v>
       </c>
       <c r="C233" t="str">
-        <v>绘制数据类型</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B234" t="str">
-        <v>Point Settings</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C234" t="str">
-        <v>点设置</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B235" t="str">
-        <v>Range of Data</v>
+        <v>Point Settings</v>
       </c>
       <c r="C235" t="str">
-        <v>数据范围</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B236" t="str">
-        <v>Lower Range</v>
+        <v>Range of Data</v>
       </c>
       <c r="C236" t="str">
-        <v>下限</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B237" t="str">
-        <v>Upper Range</v>
+        <v>Lower Range</v>
       </c>
       <c r="C237" t="str">
-        <v>上限</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B238" t="str">
-        <v>Scale Start</v>
+        <v>Upper Range</v>
       </c>
       <c r="C238" t="str">
-        <v>刻度起点</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B239" t="str">
-        <v>Scale Step</v>
+        <v>Scale Start</v>
       </c>
       <c r="C239" t="str">
-        <v>刻度步长</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B240" t="str">
-        <v>Show Scale</v>
+        <v>Scale Step</v>
       </c>
       <c r="C240" t="str">
-        <v>显示刻度</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B241" t="str">
-        <v>Draw Points</v>
+        <v>Show Scale</v>
       </c>
       <c r="C241" t="str">
-        <v>绘制点</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B242" t="str">
-        <v>Point Shape</v>
+        <v>Draw Points</v>
       </c>
       <c r="C242" t="str">
-        <v>点形状</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B243" t="str">
-        <v>Line</v>
+        <v>Point Shape</v>
       </c>
       <c r="C243" t="str">
-        <v>线条</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B244" t="str">
-        <v>Fill</v>
+        <v>Line</v>
       </c>
       <c r="C244" t="str">
-        <v>填充</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B245" t="str">
-        <v>Background Gradient</v>
+        <v>Fill</v>
       </c>
       <c r="C245" t="str">
-        <v>背景渐变</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B246" t="str">
-        <v>Curve Gradient</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C246" t="str">
-        <v>曲线渐变</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B247" t="str">
-        <v>Start</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C247" t="str">
-        <v>起点</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B248" t="str">
-        <v>End</v>
+        <v>Start</v>
       </c>
       <c r="C248" t="str">
-        <v>终点</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B249" t="str">
-        <v>Search</v>
+        <v>End</v>
       </c>
       <c r="C249" t="str">
-        <v>搜索</v>
+        <v>终点</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.column.overlay-menu.title</v>
       </c>
       <c r="B250" t="str">
-        <v>Found {{count}} Results</v>
-      </c>
-      <c r="C250" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>Overlay Settings</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.column.overlay-menu.display-overlay</v>
       </c>
       <c r="B251" t="str">
-        <v>Current Time Settings(Top / Base)</v>
-      </c>
-      <c r="C251" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>Display Overlay</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.column.overlay-menu.overlay-column-header</v>
       </c>
       <c r="B252" t="str">
-        <v>Column On?</v>
-      </c>
-      <c r="C252" t="str">
-        <v>是否已选</v>
+        <v>Overlaying</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.column.overlay-menu.overlay-column-preposition</v>
       </c>
       <c r="B253" t="str">
-        <v>Center</v>
-      </c>
-      <c r="C253" t="str">
-        <v>居中</v>
+        <v>On</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
       </c>
       <c r="B254" t="str">
-        <v>Extend</v>
-      </c>
-      <c r="C254" t="str">
-        <v>延展</v>
+        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
       </c>
       <c r="B255" t="str">
-        <v>Column</v>
-      </c>
-      <c r="C255" t="str">
-        <v>列名称</v>
+        <v>Not an Event or Point Column</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.column.overlay-menu.column-not-selected</v>
       </c>
       <c r="B256" t="str">
-        <v>Age</v>
-      </c>
-      <c r="C256" t="str">
-        <v>年代</v>
+        <v>Select Column from Menu</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B257" t="str">
-        <v>Type</v>
+        <v>Search</v>
       </c>
       <c r="C257" t="str">
-        <v>类别</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B258" t="str">
-        <v>Notes</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C258" t="str">
-        <v>注释</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B259" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Current Time Settings(Top / Base)</v>
       </c>
       <c r="C259" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B260" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>Column On?</v>
       </c>
       <c r="C260" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>是否已选</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B261" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>Center</v>
       </c>
       <c r="C261" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>居中</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B262" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>Extend</v>
       </c>
       <c r="C262" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>延展</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B263" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>Column</v>
       </c>
       <c r="C263" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>列名称</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B264" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Age</v>
       </c>
       <c r="C264" t="str">
-        <v>点击加号添加数据包</v>
+        <v>年代</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B265" t="str">
-        <v>Private Official Datapacks</v>
+        <v>Type</v>
+      </c>
+      <c r="C265" t="str">
+        <v>类别</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B266" t="str">
-        <v>Official Datapacks</v>
+        <v>Notes</v>
+      </c>
+      <c r="C266" t="str">
+        <v>注释</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B267" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>These are the default systemwide fonts.</v>
+      </c>
+      <c r="C267" t="str">
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B268" t="str">
-        <v>Workshop Datapacks</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C268" t="str">
-        <v>工作坊数据包</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B269" t="str">
-        <v>Your Datapacks</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C269" t="str">
-        <v>你的数据包</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B270" t="str">
-        <v>No</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C270" t="str">
-        <v>暂无</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B271" t="str">
-        <v>Avaliable</v>
+        <v>Click a datapack to see more information!</v>
       </c>
       <c r="C271" t="str">
-        <v>可用</v>
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B272" t="str">
-        <v>Upload Datapack</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C272" t="str">
-        <v>上传数据包</v>
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B273" t="str">
-        <v>PDF Upload</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B274" t="str">
-        <v>See More...</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B275" t="str">
-        <v>See Less...</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B276" t="str">
-        <v>Upload Your Own Datapack</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C276" t="str">
-        <v>上传你的数据包</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B277" t="str">
-        <v>No file selected</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C277" t="str">
-        <v>没有选择文件</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B278" t="str">
-        <v>Datapack Name</v>
+        <v>No</v>
       </c>
       <c r="C278" t="str">
-        <v>数据包名称</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B279" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Avaliable</v>
       </c>
       <c r="C279" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B280" t="str">
-        <v>Authored By</v>
+        <v>Upload Datapack</v>
       </c>
       <c r="C280" t="str">
-        <v>作者</v>
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B281" t="str">
-        <v>Credited to...</v>
-      </c>
-      <c r="C281" t="str">
-        <v>作者为...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B282" t="str">
-        <v>Datapack Description</v>
-      </c>
-      <c r="C282" t="str">
-        <v>数据包概述</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B283" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C283" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B284" t="str">
-        <v>Tags</v>
+        <v>No file selected</v>
       </c>
       <c r="C284" t="str">
-        <v>标签</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B285" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C285" t="str">
-        <v>使数据包对公共可见</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B286" t="str">
-        <v>Add Reference</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C286" t="str">
-        <v>添加引用</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B287" t="str">
-        <v>More Options</v>
+        <v>Authored By</v>
       </c>
       <c r="C287" t="str">
-        <v>更多选项</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B288" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>Credited to...</v>
       </c>
       <c r="C288" t="str">
-        <v>完成并上传</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B289" t="str">
-        <v>Start Over</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C289" t="str">
-        <v>重新开始</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B290" t="str">
-        <v>Reference</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C290" t="str">
-        <v>引用</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B291" t="str">
-        <v>Contact</v>
+        <v>Tags</v>
       </c>
       <c r="C291" t="str">
-        <v>联系方式</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B292" t="str">
-        <v>Enter your contact information</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C292" t="str">
-        <v>输入你的联系方式</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B293" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Add Reference</v>
       </c>
       <c r="C293" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B294" t="str">
-        <v>Notes</v>
+        <v>More Options</v>
       </c>
       <c r="C294" t="str">
-        <v>注释</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B295" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C295" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B296" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Start Over</v>
       </c>
       <c r="C296" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B297" t="str">
-        <v>You have not made a chart yet</v>
+        <v>Reference</v>
       </c>
       <c r="C297" t="str">
-        <v>您还未制作任何图表</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>chart.save</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B298" t="str">
-        <v>Save Chart</v>
+        <v>Contact</v>
       </c>
       <c r="C298" t="str">
-        <v>保存图表</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B299" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C299" t="str">
-        <v>确认更改数据包</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B300" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C300" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B301" t="str">
-        <v>Save</v>
+        <v>Notes</v>
       </c>
       <c r="C301" t="str">
-        <v>保存</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B302" t="str">
-        <v>Discard</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C302" t="str">
-        <v>不保存</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B303" t="str">
-        <v>Use default age range?</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C303" t="str">
-        <v>使用默认时间区间？</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B304" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>help.qsg.title</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B305" t="str">
-        <v>Quick Start Quide</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C305" t="str">
-        <v>快速指南</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>help.qsg.content</v>
+        <v>chart.save</v>
       </c>
       <c r="B306" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Save Chart</v>
       </c>
       <c r="C306" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>help.qsg.button</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B307" t="str">
-        <v>Start QSG</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C307" t="str">
-        <v>开始快速指南</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>help.tour.title</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B308" t="str">
-        <v>Tour</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C308" t="str">
-        <v>导览</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B309" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Save</v>
       </c>
       <c r="C309" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>help.tour.content.settings</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B310" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>Discard</v>
       </c>
       <c r="C310" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B311" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>Use default age range?</v>
       </c>
       <c r="C311" t="str">
-        <v>开始数据包导览</v>
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>help.tour.button.settings</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B312" t="str">
-        <v>Start Settings Tour</v>
-      </c>
-      <c r="C312" t="str">
-        <v>开始设置导览</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.license</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B313" t="str">
-        <v>Software License</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C313" t="str">
-        <v>软件许可</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B314" t="str">
-        <v>File Format Info</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C314" t="str">
-        <v>文件格式信息</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B315" t="str">
-        <v>View File Format Info</v>
+        <v>Start QSG</v>
       </c>
       <c r="C315" t="str">
-        <v>查看文件格式信息</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>errors.title</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B316" t="str">
-        <v>Error</v>
+        <v>Tour</v>
       </c>
       <c r="C316" t="str">
-        <v>错误</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B317" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C317" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B318" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C318" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B319" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C319" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B320" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C320" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>help.license</v>
       </c>
       <c r="B321" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Software License</v>
       </c>
       <c r="C321" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B322" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>File Format Info</v>
       </c>
       <c r="C322" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B323" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C323" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.title</v>
       </c>
       <c r="B324" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C324" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B325" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C325" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B326" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C326" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C327" t="str">
-        <v>无效的数据包上传</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B328" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
+      </c>
+      <c r="C328" t="str">
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B331" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B332" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B333" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C333" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B334" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C334" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B335" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Invalid datapack upload.</v>
       </c>
       <c r="C335" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B336" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
-      </c>
-      <c r="C336" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B337" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C337" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B338" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C338" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B339" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C339" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B340" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C340" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B341" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C341" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B342" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C342" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B343" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C343" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B344" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C344" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B345" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C345" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B346" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C346" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B347" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C347" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B348" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C348" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B349" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C349" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B350" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C350" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B351" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C351" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B352" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C352" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C354" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C355" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B356" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C356" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B357" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C357" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B358" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C358" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B359" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C359" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B360" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C360" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B361" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C361" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B362" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B363" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C363" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B364" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C364" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B367" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C367" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B368" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C368" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B369" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C369" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B370" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C370" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B371" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C371" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B372" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C372" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B373" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C373" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B374" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C374" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C375" t="str">
         <v>无法删除用户。请稍后再试。</v>
@@ -4255,824 +4231,923 @@
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Incorrect password. Please try again.</v>
+      </c>
+      <c r="C376" t="str">
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C377" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B378" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C378" t="str">
-        <v>不能删除根用户。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B379" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to modify user. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
+      </c>
+      <c r="C380" t="str">
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B381" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B382" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B383" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B384" t="str">
-        <v>Server file metadata error. Please try again later.</v>
-      </c>
-      <c r="C384" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B385" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B386" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C386" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B387" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C387" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
       </c>
       <c r="B388" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
-      </c>
-      <c r="C388" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>Unable to modify user. Please try again later.</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B389" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C389" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B390" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C390" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B391" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C391" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B392" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C392" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B393" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C393" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B394" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B395" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C395" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B396" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C397" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B398" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
+      </c>
+      <c r="C398" t="str">
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B399" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C399" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B400" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+      </c>
+      <c r="C400" t="str">
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B401" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+      </c>
+      <c r="C401" t="str">
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B402" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>The start date must be before the end date.</v>
+      </c>
+      <c r="C402" t="str">
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B403" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Unable to create workshop. Please try again later.</v>
+      </c>
+      <c r="C403" t="str">
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B404" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
+      </c>
+      <c r="C404" t="str">
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B405" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C405" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B407" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C407" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B408" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B410" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B411" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B413" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B414" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B415" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B416" t="str">
-        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B417" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B418" t="str">
-        <v>Failed to add files to workshop</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B419" t="str">
-        <v>Failed to add cover to workshop</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>errors.INVALID_FILE_FORMAT</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B420" t="str">
-        <v>Invalid file format.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B421" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
-      </c>
-      <c r="C421" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>button.generate</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B422" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C422" t="str">
-        <v>绘制</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B423" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C423" t="str">
-        <v>绘制图表</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>button.remove-cache</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B424" t="str">
-        <v>Remove Cache</v>
-      </c>
-      <c r="C424" t="str">
-        <v>清除缓存</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>button.confirm-selection</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B425" t="str">
-        <v>Confirm Selection</v>
-      </c>
-      <c r="C425" t="str">
-        <v>确认选择</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B426" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Failed to add files to workshop</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>yes</v>
+        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B427" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C427" t="str">
-        <v>是</v>
+        <v>Failed to add cover to workshop</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>no</v>
+        <v>errors.INVALID_FILE_FORMAT</v>
       </c>
       <c r="B428" t="str">
-        <v>No</v>
-      </c>
-      <c r="C428" t="str">
-        <v>否</v>
+        <v>Invalid file format.</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>languageNames.en-US</v>
+        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B429" t="str">
-        <v>English</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
+      </c>
+      <c r="C429" t="str">
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>languageNames.en</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B430" t="str">
-        <v>English</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C430" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>languageNames.zh</v>
+        <v>button.generate</v>
       </c>
       <c r="B431" t="str">
-        <v>中文</v>
+        <v>Generate</v>
+      </c>
+      <c r="C431" t="str">
+        <v>绘制</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.quit</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B432" t="str">
-        <v>Quit Tour</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C432" t="str">
-        <v>退出导览</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.finish</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B433" t="str">
-        <v>Finish Tour</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C433" t="str">
-        <v>结束导览</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.next</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B434" t="str">
-        <v>Next</v>
+        <v>Confirm Selection</v>
       </c>
       <c r="C434" t="str">
-        <v>下一步</v>
+        <v>确认选择</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.back</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B435" t="str">
-        <v>Back</v>
-      </c>
-      <c r="C435" t="str">
-        <v>上一步</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step1</v>
+        <v>yes</v>
       </c>
       <c r="B436" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Yes</v>
       </c>
       <c r="C436" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>是</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.qsg.step2</v>
+        <v>no</v>
       </c>
       <c r="B437" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>No</v>
       </c>
       <c r="C437" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>否</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.qsg.step3</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B438" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
-      </c>
-      <c r="C438" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.qsg.step4</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B439" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
-      </c>
-      <c r="C439" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.qsg.step5</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B440" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
-      </c>
-      <c r="C440" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.quit</v>
       </c>
       <c r="B441" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C441" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.finish</v>
       </c>
       <c r="B442" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C442" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.next</v>
       </c>
       <c r="B443" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>Next</v>
       </c>
       <c r="C443" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.back</v>
       </c>
       <c r="B444" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Back</v>
       </c>
       <c r="C444" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B445" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C445" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B446" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C446" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B447" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C447" t="str">
-        <v>记得确认您的选择</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C448" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C449" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B450" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C450" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B451" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C451" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B452" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C452" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B453" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C453" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B454" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C454" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.datapack.step3</v>
+      </c>
+      <c r="B455" t="str">
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C455" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.datapack.step4</v>
+      </c>
+      <c r="B456" t="str">
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C456" t="str">
-        <v>English</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="str">
-        <v>language-names.en</v>
+        <v>tours.settings.step1</v>
+      </c>
+      <c r="B457" t="str">
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C457" t="str">
-        <v>English</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="str">
+        <v>tours.settings.step2</v>
+      </c>
+      <c r="B458" t="str">
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+      </c>
+      <c r="C458" t="str">
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="str">
+        <v>tours.settings.step3</v>
+      </c>
+      <c r="B459" t="str">
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+      </c>
+      <c r="C459" t="str">
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="str">
+        <v>tours.settings.step4</v>
+      </c>
+      <c r="B460" t="str">
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+      </c>
+      <c r="C460" t="str">
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="str">
+        <v>tours.settings.step5</v>
+      </c>
+      <c r="B461" t="str">
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+      </c>
+      <c r="C461" t="str">
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="str">
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B462" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+      </c>
+      <c r="C462" t="str">
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="str">
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B463" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+      </c>
+      <c r="C463" t="str">
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="str">
+        <v>settings.column.tooltip.note-in-range</v>
+      </c>
+      <c r="C464" t="str">
+        <v>数据不在所选时间区间内</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C465" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C466" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C458" t="str">
+      <c r="C467" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C458"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C467"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor download workshop files and add user checks
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C467"/>
+  <dimension ref="A1:C470"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1464,562 +1464,559 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>workshops.calendar.switchLabel</v>
+        <v>workshops.details-page.download-tooltip-not-registered</v>
       </c>
       <c r="B113" t="str">
-        <v>Toggle calendar</v>
+        <v>Please register for the workshop to download the files.</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>workshops.calendar.month</v>
+        <v>workshops.calendar.switchLabel</v>
       </c>
       <c r="B114" t="str">
-        <v>Month</v>
+        <v>Toggle calendar</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>workshops.calendar.week</v>
+        <v>workshops.calendar.month</v>
       </c>
       <c r="B115" t="str">
-        <v>Week</v>
+        <v>Month</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>workshops.calendar.days.sunday</v>
+        <v>workshops.calendar.week</v>
       </c>
       <c r="B116" t="str">
-        <v>Sun</v>
+        <v>Week</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>workshops.calendar.days.monday</v>
+        <v>workshops.calendar.days.sunday</v>
       </c>
       <c r="B117" t="str">
-        <v>Mon</v>
+        <v>Sun</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>workshops.calendar.days.tuesday</v>
+        <v>workshops.calendar.days.monday</v>
       </c>
       <c r="B118" t="str">
-        <v>Tue</v>
+        <v>Mon</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>workshops.calendar.days.wednesday</v>
+        <v>workshops.calendar.days.tuesday</v>
       </c>
       <c r="B119" t="str">
-        <v>Wed</v>
+        <v>Tue</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>workshops.calendar.days.thursday</v>
+        <v>workshops.calendar.days.wednesday</v>
       </c>
       <c r="B120" t="str">
-        <v>Thu</v>
+        <v>Wed</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>workshops.calendar.days.friday</v>
+        <v>workshops.calendar.days.thursday</v>
       </c>
       <c r="B121" t="str">
-        <v>Fri</v>
+        <v>Thu</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>workshops.calendar.days.saturday</v>
+        <v>workshops.calendar.days.friday</v>
       </c>
       <c r="B122" t="str">
-        <v>Sat</v>
+        <v>Fri</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>workshops.calendar.months.1</v>
+        <v>workshops.calendar.days.saturday</v>
       </c>
       <c r="B123" t="str">
-        <v>January</v>
-      </c>
-      <c r="C123" t="str">
-        <v>一月</v>
+        <v>Sat</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>workshops.calendar.months.2</v>
+        <v>workshops.calendar.months.1</v>
       </c>
       <c r="B124" t="str">
-        <v>February</v>
+        <v>January</v>
       </c>
       <c r="C124" t="str">
-        <v>二月</v>
+        <v>一月</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>workshops.calendar.months.3</v>
+        <v>workshops.calendar.months.2</v>
       </c>
       <c r="B125" t="str">
-        <v>March</v>
+        <v>February</v>
       </c>
       <c r="C125" t="str">
-        <v>三月</v>
+        <v>二月</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>workshops.calendar.months.4</v>
+        <v>workshops.calendar.months.3</v>
       </c>
       <c r="B126" t="str">
-        <v>April</v>
+        <v>March</v>
       </c>
       <c r="C126" t="str">
-        <v>四月</v>
+        <v>三月</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>workshops.calendar.months.5</v>
+        <v>workshops.calendar.months.4</v>
       </c>
       <c r="B127" t="str">
-        <v>May</v>
+        <v>April</v>
       </c>
       <c r="C127" t="str">
-        <v>五月</v>
+        <v>四月</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>workshops.calendar.months.6</v>
+        <v>workshops.calendar.months.5</v>
       </c>
       <c r="B128" t="str">
-        <v>June</v>
+        <v>May</v>
       </c>
       <c r="C128" t="str">
-        <v>六月</v>
+        <v>五月</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>workshops.calendar.months.7</v>
+        <v>workshops.calendar.months.6</v>
       </c>
       <c r="B129" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="C129" t="str">
-        <v>七月</v>
+        <v>六月</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>workshops.calendar.months.8</v>
+        <v>workshops.calendar.months.7</v>
       </c>
       <c r="B130" t="str">
-        <v>August</v>
+        <v>July</v>
       </c>
       <c r="C130" t="str">
-        <v>八月</v>
+        <v>七月</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>workshops.calendar.months.9</v>
+        <v>workshops.calendar.months.8</v>
       </c>
       <c r="B131" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="C131" t="str">
-        <v>九月</v>
+        <v>八月</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>workshops.calendar.months.10</v>
+        <v>workshops.calendar.months.9</v>
       </c>
       <c r="B132" t="str">
-        <v>October</v>
+        <v>September</v>
       </c>
       <c r="C132" t="str">
-        <v>十月</v>
+        <v>九月</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>workshops.calendar.months.11</v>
+        <v>workshops.calendar.months.10</v>
       </c>
       <c r="B133" t="str">
-        <v>November</v>
+        <v>October</v>
       </c>
       <c r="C133" t="str">
-        <v>十一月</v>
+        <v>十月</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>workshops.calendar.months.12</v>
+        <v>workshops.calendar.months.11</v>
       </c>
       <c r="B134" t="str">
-        <v>December</v>
+        <v>November</v>
       </c>
       <c r="C134" t="str">
-        <v>十二月</v>
+        <v>十一月</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>loading.loading-chart</v>
+        <v>workshops.calendar.months.12</v>
       </c>
       <c r="B135" t="str">
-        <v>Loading Chart...</v>
+        <v>December</v>
       </c>
       <c r="C135" t="str">
-        <v>加载图表...</v>
+        <v>十二月</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>loading.loading-datapacks</v>
+        <v>loading.loading-chart</v>
       </c>
       <c r="B136" t="str">
-        <v>Loading Datapacks</v>
+        <v>Loading Chart...</v>
       </c>
       <c r="C136" t="str">
-        <v>加载数据包</v>
+        <v>加载图表...</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>loading.time</v>
+        <v>loading.loading-datapacks</v>
       </c>
       <c r="B137" t="str">
-        <v>this could take more than a minute</v>
+        <v>Loading Datapacks</v>
       </c>
       <c r="C137" t="str">
-        <v>这可能需要超过一分钟</v>
+        <v>加载数据包</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>loading.fetching-datapacks</v>
+        <v>loading.time</v>
       </c>
       <c r="B138" t="str">
-        <v>Fetching Datapacks</v>
+        <v>this could take more than a minute</v>
+      </c>
+      <c r="C138" t="str">
+        <v>这可能需要超过一分钟</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>loading.fetching-datapacks</v>
       </c>
       <c r="B139" t="str">
-        <v>Please select a unit.</v>
+        <v>Fetching Datapacks</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B140" t="str">
-        <v>No units available</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B141" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B142" t="str">
-        <v>Please select a datapack.</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B143" t="str">
-        <v>No unit selected</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.xAxis</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B144" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>crossPlot.time.yAxis</v>
+        <v>crossPlot.time.xAxis</v>
       </c>
       <c r="B145" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>crossPlot.sidebar.no-markers</v>
+        <v>crossPlot.time.yAxis</v>
       </c>
       <c r="B146" t="str">
-        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>crossPlot.sidebar.no-models</v>
+        <v>crossPlot.sidebar.no-markers</v>
       </c>
       <c r="B147" t="str">
-        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
+        <v xml:space="preserve"> No Markers Available (Please Add a Marker by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>crossPlot.sidebar.no-models</v>
       </c>
       <c r="B148" t="str">
-        <v>Create Datapack</v>
+        <v>No Models Available (Please Add a Model by Clicking the Chart in the Main View)</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>settingsTabs.Time</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B149" t="str">
-        <v>Time</v>
-      </c>
-      <c r="C149" t="str">
-        <v>选择时间区间</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>settingsTabs.Preferences</v>
+        <v>settingsTabs.Time</v>
       </c>
       <c r="B150" t="str">
-        <v>Preferences</v>
+        <v>Time</v>
       </c>
       <c r="C150" t="str">
-        <v>選擇偏好</v>
+        <v>选择时间区间</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>settingsTabs.Column</v>
+        <v>settingsTabs.Preferences</v>
       </c>
       <c r="B151" t="str">
-        <v>Column</v>
+        <v>Preferences</v>
       </c>
       <c r="C151" t="str">
-        <v>选择列</v>
+        <v>選擇偏好</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>settingsTabs.Search</v>
+        <v>settingsTabs.Column</v>
       </c>
       <c r="B152" t="str">
-        <v>Search</v>
+        <v>Column</v>
       </c>
       <c r="C152" t="str">
-        <v>搜索</v>
+        <v>选择列</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>settingsTabs.Font</v>
+        <v>settingsTabs.Search</v>
       </c>
       <c r="B153" t="str">
-        <v>Font</v>
+        <v>Search</v>
       </c>
       <c r="C153" t="str">
-        <v>字体</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>settingsTabs.Map Points</v>
+        <v>settingsTabs.Font</v>
       </c>
       <c r="B154" t="str">
-        <v>Map Points</v>
+        <v>Font</v>
       </c>
       <c r="C154" t="str">
-        <v>地图</v>
+        <v>字体</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>settingsTabs.Datapacks</v>
+        <v>settingsTabs.Map Points</v>
       </c>
       <c r="B155" t="str">
-        <v>Datapacks</v>
+        <v>Map Points</v>
       </c>
       <c r="C155" t="str">
-        <v>选择数据包</v>
+        <v>地图</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>settingsTabs.General</v>
+        <v>settingsTabs.Datapacks</v>
       </c>
       <c r="B156" t="str">
-        <v>General</v>
+        <v>Datapacks</v>
       </c>
       <c r="C156" t="str">
-        <v>基础选项</v>
+        <v>选择数据包</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>settingsTabs.Data Mining</v>
+        <v>settingsTabs.General</v>
       </c>
       <c r="B157" t="str">
-        <v>Data Mining</v>
+        <v>General</v>
       </c>
       <c r="C157" t="str">
-        <v>数据挖掘</v>
+        <v>基础选项</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>settingsTabs.Curve Drawing</v>
+        <v>settingsTabs.Data Mining</v>
       </c>
       <c r="B158" t="str">
-        <v>Curve Drawing</v>
+        <v>Data Mining</v>
       </c>
       <c r="C158" t="str">
-        <v>绘制曲线图</v>
+        <v>数据挖掘</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.Overlay</v>
+        <v>settingsTabs.Curve Drawing</v>
       </c>
       <c r="B159" t="str">
-        <v>Overlay</v>
+        <v>Curve Drawing</v>
+      </c>
+      <c r="C159" t="str">
+        <v>绘制曲线图</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Overlay</v>
       </c>
       <c r="B160" t="str">
-        <v>About</v>
-      </c>
-      <c r="C160" t="str">
-        <v>关于</v>
+        <v>Overlay</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B161" t="str">
-        <v>View Data</v>
+        <v>About</v>
       </c>
       <c r="C161" t="str">
-        <v>查看数据</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B162" t="str">
-        <v>Discussion</v>
+        <v>View Data</v>
       </c>
       <c r="C162" t="str">
-        <v>讨论</v>
+        <v>查看数据</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B163" t="str">
-        <v>Warnings</v>
+        <v>Discussion</v>
       </c>
       <c r="C163" t="str">
-        <v>警告</v>
+        <v>讨论</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B164" t="str">
-        <v>Load/Save</v>
+        <v>Warnings</v>
+      </c>
+      <c r="C164" t="str">
+        <v>警告</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B165" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B166" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B167" t="str">
-        <v>Top of Interval</v>
-      </c>
-      <c r="C167" t="str">
-        <v>区间顶部</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B168" t="str">
-        <v>Base of Interval</v>
+        <v>Top of Interval</v>
       </c>
       <c r="C168" t="str">
-        <v>区间底部</v>
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B169" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Base of Interval</v>
       </c>
       <c r="C169" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间底部</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B170" t="str">
-        <v>Base Age/Stage Name</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C170" t="str">
         <v>年代/阶段 名称</v>
@@ -2027,3127 +2024,3157 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B171" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C171" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B172" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C172" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B173" t="str">
-        <v>Base age should be older than top age</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
       </c>
       <c r="C173" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B174" t="str">
-        <v>Vertical Scale</v>
+        <v>Base age should be older than top age</v>
+      </c>
+      <c r="C174" t="str">
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B175" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
-      </c>
-      <c r="C175" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B176" t="str">
-        <v>Add MouseOver info (popups)</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C176" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B177" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Add MouseOver info (popups)</v>
       </c>
       <c r="C177" t="str">
-        <v>启用优先级过滤</v>
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B178" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C178" t="str">
-        <v>启用事件列的背景</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B179" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C179" t="str">
-        <v>启用添加图例</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B180" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C180" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B181" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C181" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B182" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C182" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B183" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C183" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B184" t="str">
-        <v>Load Settings</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C184" t="str">
-        <v>上传设置</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B185" t="str">
-        <v>Save Settings</v>
+        <v>Load Settings</v>
       </c>
       <c r="C185" t="str">
-        <v>保存设置</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B186" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>Save Settings</v>
       </c>
       <c r="C186" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B187" t="str">
-        <v>Cancel</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C187" t="str">
-        <v>取消</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B188" t="str">
-        <v>Load</v>
+        <v>Cancel</v>
       </c>
       <c r="C188" t="str">
-        <v>上传</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B189" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Load</v>
       </c>
       <c r="C189" t="str">
-        <v>请输入文件名</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B190" t="str">
-        <v>Cancel</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C190" t="str">
-        <v>取消</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B191" t="str">
-        <v>Save</v>
+        <v>Cancel</v>
       </c>
       <c r="C191" t="str">
-        <v>保存</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B192" t="str">
-        <v>Data not included in time range</v>
+        <v>Save</v>
+      </c>
+      <c r="C192" t="str">
+        <v>保存</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B193" t="str">
-        <v>Auto Scale</v>
-      </c>
-      <c r="C193" t="str">
-        <v>自动缩放</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B194" t="str">
-        <v>Flip Range</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C194" t="str">
-        <v>翻转区间</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B195" t="str">
-        <v>Column Customization</v>
+        <v>Flip Range</v>
       </c>
       <c r="C195" t="str">
-        <v>个性化设置列</v>
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Data Mining Settings</v>
+        <v>Column Customization</v>
       </c>
       <c r="C196" t="str">
-        <v>数据挖掘设置</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B197" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C197" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B198" t="str">
-        <v>Shift Row Positions</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C198" t="str">
-        <v>移动位置</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B199" t="str">
-        <v>Edit Title</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C199" t="str">
-        <v>编辑标题</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B200" t="str">
-        <v>Background Color</v>
+        <v>Edit Title</v>
       </c>
       <c r="C200" t="str">
-        <v>背景颜色</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B201" t="str">
-        <v>Enable Title</v>
+        <v>Background Color</v>
       </c>
       <c r="C201" t="str">
-        <v>显示标题</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B202" t="str">
-        <v>Show Age Label</v>
+        <v>Enable Title</v>
       </c>
       <c r="C202" t="str">
-        <v>显示年代</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B203" t="str">
-        <v>Information and References</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C203" t="str">
-        <v>信息与参考</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B204" t="str">
-        <v>Add Blank Column</v>
+        <v>Information and References</v>
       </c>
       <c r="C204" t="str">
-        <v>添加一个空白列</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B205" t="str">
-        <v>Add Age Column</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C205" t="str">
-        <v>添加一个年代列</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B206" t="str">
-        <v>Width</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C206" t="str">
-        <v>宽</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B207" t="str">
-        <v>Label Orientation</v>
+        <v>Width</v>
       </c>
       <c r="C207" t="str">
-        <v>图标排布</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B208" t="str">
-        <v>Horizontal</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C208" t="str">
-        <v>横向</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B209" t="str">
-        <v>Vertical</v>
+        <v>Horizontal</v>
       </c>
       <c r="C209" t="str">
-        <v>纵向</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B210" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Vertical</v>
       </c>
       <c r="C210" t="str">
-        <v>显示不确定性</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B211" t="str">
-        <v>Events</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C211" t="str">
-        <v>事件</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B212" t="str">
-        <v>Ranges</v>
+        <v>Events</v>
       </c>
       <c r="C212" t="str">
-        <v>范围</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B213" t="str">
-        <v>First Occurrence</v>
+        <v>Ranges</v>
       </c>
       <c r="C213" t="str">
-        <v>首先发生的优先</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B214" t="str">
-        <v>Last Occurrence</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C214" t="str">
-        <v>最后发生的优先</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B215" t="str">
-        <v>Alphabetical</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C215" t="str">
-        <v>按字母顺序排列</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B216" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C216" t="str">
-        <v>调整年代刻度尺</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B217" t="str">
-        <v>Left</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C217" t="str">
-        <v>左对齐</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B218" t="str">
-        <v>Right</v>
+        <v>Left</v>
       </c>
       <c r="C218" t="str">
-        <v>右对齐</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B219" t="str">
-        <v>Change Font</v>
+        <v>Right</v>
       </c>
       <c r="C219" t="str">
-        <v>更改字体</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B220" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Change Font</v>
       </c>
       <c r="C220" t="str">
-        <v>子列的更多字体选项</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B221" t="str">
-        <v>Data Mining Settings</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C221" t="str">
-        <v>数据挖掘设置</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B222" t="str">
-        <v>Window Size</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C222" t="str">
-        <v>窗口大小</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B223" t="str">
-        <v>Step Size</v>
+        <v>Window Size</v>
       </c>
       <c r="C223" t="str">
-        <v>步长</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B224" t="str">
-        <v>Frequency</v>
+        <v>Step Size</v>
       </c>
       <c r="C224" t="str">
-        <v>频率</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B225" t="str">
-        <v>Maximum Value</v>
+        <v>Frequency</v>
       </c>
       <c r="C225" t="str">
-        <v>最大值</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Minimum Value</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C226" t="str">
-        <v>最小值</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B227" t="str">
-        <v>Average Value</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C227" t="str">
-        <v>平均值</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B228" t="str">
-        <v>Rate of Change</v>
+        <v>Average Value</v>
       </c>
       <c r="C228" t="str">
-        <v>变化率</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B229" t="str">
-        <v>Frequency of LAD</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C229" t="str">
-        <v>LAD 频率</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B230" t="str">
-        <v>Frequency of FAD</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C230" t="str">
-        <v>FAD 频率</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B231" t="str">
-        <v>Combined Events</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C231" t="str">
-        <v>组合事件</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B232" t="str">
-        <v>Event Type</v>
+        <v>Combined Events</v>
       </c>
       <c r="C232" t="str">
-        <v>事件类型</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B233" t="str">
-        <v>Chron Type</v>
+        <v>Event Type</v>
       </c>
       <c r="C233" t="str">
-        <v>年代类型</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B234" t="str">
-        <v>Data Type to Plot</v>
+        <v>Chron Type</v>
       </c>
       <c r="C234" t="str">
-        <v>绘制数据类型</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B235" t="str">
-        <v>Point Settings</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C235" t="str">
-        <v>点设置</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B236" t="str">
-        <v>Range of Data</v>
+        <v>Point Settings</v>
       </c>
       <c r="C236" t="str">
-        <v>数据范围</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B237" t="str">
-        <v>Lower Range</v>
+        <v>Range of Data</v>
       </c>
       <c r="C237" t="str">
-        <v>下限</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B238" t="str">
-        <v>Upper Range</v>
+        <v>Lower Range</v>
       </c>
       <c r="C238" t="str">
-        <v>上限</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B239" t="str">
-        <v>Scale Start</v>
+        <v>Upper Range</v>
       </c>
       <c r="C239" t="str">
-        <v>刻度起点</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B240" t="str">
-        <v>Scale Step</v>
+        <v>Scale Start</v>
       </c>
       <c r="C240" t="str">
-        <v>刻度步长</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B241" t="str">
-        <v>Show Scale</v>
+        <v>Scale Step</v>
       </c>
       <c r="C241" t="str">
-        <v>显示刻度</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B242" t="str">
-        <v>Draw Points</v>
+        <v>Show Scale</v>
       </c>
       <c r="C242" t="str">
-        <v>绘制点</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B243" t="str">
-        <v>Point Shape</v>
+        <v>Draw Points</v>
       </c>
       <c r="C243" t="str">
-        <v>点形状</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B244" t="str">
-        <v>Line</v>
+        <v>Point Shape</v>
       </c>
       <c r="C244" t="str">
-        <v>线条</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B245" t="str">
-        <v>Fill</v>
+        <v>Line</v>
       </c>
       <c r="C245" t="str">
-        <v>填充</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B246" t="str">
-        <v>Background Gradient</v>
+        <v>Fill</v>
       </c>
       <c r="C246" t="str">
-        <v>背景渐变</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B247" t="str">
-        <v>Curve Gradient</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C247" t="str">
-        <v>曲线渐变</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B248" t="str">
-        <v>Start</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C248" t="str">
-        <v>起点</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B249" t="str">
-        <v>End</v>
+        <v>Start</v>
       </c>
       <c r="C249" t="str">
-        <v>终点</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.column.overlay-menu.title</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B250" t="str">
-        <v>Overlay Settings</v>
+        <v>End</v>
+      </c>
+      <c r="C250" t="str">
+        <v>终点</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.column.overlay-menu.display-overlay</v>
+        <v>settings.column.overlay-menu.title</v>
       </c>
       <c r="B251" t="str">
-        <v>Display Overlay</v>
+        <v>Overlay Settings</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.column.overlay-menu.overlay-column-header</v>
+        <v>settings.column.overlay-menu.display-overlay</v>
       </c>
       <c r="B252" t="str">
-        <v>Overlaying</v>
+        <v>Display Overlay</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.column.overlay-menu.overlay-column-preposition</v>
+        <v>settings.column.overlay-menu.overlay-column-header</v>
       </c>
       <c r="B253" t="str">
-        <v>On</v>
+        <v>Overlaying</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
+        <v>settings.column.overlay-menu.overlay-column-preposition</v>
       </c>
       <c r="B254" t="str">
-        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
+        <v>On</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
+        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
       </c>
       <c r="B255" t="str">
-        <v>Not an Event or Point Column</v>
+        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.column.overlay-menu.column-not-selected</v>
+        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
       </c>
       <c r="B256" t="str">
-        <v>Select Column from Menu</v>
+        <v>Not an Event or Point Column</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.column.overlay-menu.column-not-selected</v>
       </c>
       <c r="B257" t="str">
-        <v>Search</v>
-      </c>
-      <c r="C257" t="str">
-        <v>搜索</v>
+        <v>Select Column from Menu</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B258" t="str">
-        <v>Found {{count}} Results</v>
+        <v>Search</v>
       </c>
       <c r="C258" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B259" t="str">
-        <v>Current Time Settings(Top / Base)</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C259" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B260" t="str">
-        <v>Column On?</v>
+        <v>Current Time Settings(Top / Base)</v>
       </c>
       <c r="C260" t="str">
-        <v>是否已选</v>
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B261" t="str">
-        <v>Center</v>
+        <v>Column On?</v>
       </c>
       <c r="C261" t="str">
-        <v>居中</v>
+        <v>是否已选</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B262" t="str">
-        <v>Extend</v>
+        <v>Center</v>
       </c>
       <c r="C262" t="str">
-        <v>延展</v>
+        <v>居中</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B263" t="str">
-        <v>Column</v>
+        <v>Extend</v>
       </c>
       <c r="C263" t="str">
-        <v>列名称</v>
+        <v>延展</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B264" t="str">
-        <v>Age</v>
+        <v>Column</v>
       </c>
       <c r="C264" t="str">
-        <v>年代</v>
+        <v>列名称</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B265" t="str">
-        <v>Type</v>
+        <v>Age</v>
       </c>
       <c r="C265" t="str">
-        <v>类别</v>
+        <v>年代</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B266" t="str">
-        <v>Notes</v>
+        <v>Type</v>
       </c>
       <c r="C266" t="str">
-        <v>注释</v>
+        <v>类别</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B267" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Notes</v>
       </c>
       <c r="C267" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B268" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>These are the default systemwide fonts.</v>
       </c>
       <c r="C268" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B269" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C269" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B270" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C270" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B271" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C271" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B272" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Click a datapack to see more information!</v>
       </c>
       <c r="C272" t="str">
-        <v>点击加号添加数据包</v>
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B273" t="str">
-        <v>Private Official Datapacks</v>
+        <v>Add a datapack by clicking the checkbox</v>
+      </c>
+      <c r="C273" t="str">
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B274" t="str">
-        <v>Official Datapacks</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B275" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B276" t="str">
-        <v>Workshop Datapacks</v>
-      </c>
-      <c r="C276" t="str">
-        <v>工作坊数据包</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B277" t="str">
-        <v>Your Datapacks</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C277" t="str">
-        <v>你的数据包</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B278" t="str">
-        <v>No</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C278" t="str">
-        <v>暂无</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B279" t="str">
-        <v>Avaliable</v>
+        <v>No</v>
       </c>
       <c r="C279" t="str">
-        <v>可用</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B280" t="str">
-        <v>Upload Datapack</v>
+        <v>Avaliable</v>
       </c>
       <c r="C280" t="str">
-        <v>上传数据包</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B281" t="str">
-        <v>See More...</v>
+        <v>Upload Datapack</v>
+      </c>
+      <c r="C281" t="str">
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B282" t="str">
-        <v>See Less...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B283" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C283" t="str">
-        <v>上传你的数据包</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B284" t="str">
-        <v>No file selected</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C284" t="str">
-        <v>没有选择文件</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B285" t="str">
-        <v>Datapack Name</v>
+        <v>No file selected</v>
       </c>
       <c r="C285" t="str">
-        <v>数据包名称</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B286" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C286" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B287" t="str">
-        <v>Authored By</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C287" t="str">
-        <v>作者</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B288" t="str">
-        <v>Credited to...</v>
+        <v>Authored By</v>
       </c>
       <c r="C288" t="str">
-        <v>作者为...</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B289" t="str">
-        <v>Datapack Description</v>
+        <v>Credited to...</v>
       </c>
       <c r="C289" t="str">
-        <v>数据包概述</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B290" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C290" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B291" t="str">
-        <v>Tags</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C291" t="str">
-        <v>标签</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B292" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Tags</v>
       </c>
       <c r="C292" t="str">
-        <v>使数据包对公共可见</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B293" t="str">
-        <v>Add Reference</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C293" t="str">
-        <v>添加引用</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B294" t="str">
-        <v>More Options</v>
+        <v>Add Reference</v>
       </c>
       <c r="C294" t="str">
-        <v>更多选项</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B295" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>More Options</v>
       </c>
       <c r="C295" t="str">
-        <v>完成并上传</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B296" t="str">
-        <v>Start Over</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C296" t="str">
-        <v>重新开始</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B297" t="str">
-        <v>Reference</v>
+        <v>Start Over</v>
       </c>
       <c r="C297" t="str">
-        <v>引用</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B298" t="str">
-        <v>Contact</v>
+        <v>Reference</v>
       </c>
       <c r="C298" t="str">
-        <v>联系方式</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B299" t="str">
-        <v>Enter your contact information</v>
+        <v>Contact</v>
       </c>
       <c r="C299" t="str">
-        <v>输入你的联系方式</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B300" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C300" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B301" t="str">
-        <v>Notes</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C301" t="str">
-        <v>注释</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B302" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Notes</v>
       </c>
       <c r="C302" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B303" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C303" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B304" t="str">
-        <v>PDF Upload</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+      </c>
+      <c r="C304" t="str">
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B305" t="str">
-        <v>You have not made a chart yet</v>
-      </c>
-      <c r="C305" t="str">
-        <v>您还未制作任何图表</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>chart.save</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B306" t="str">
-        <v>Save Chart</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C306" t="str">
-        <v>保存图表</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>chart.save</v>
       </c>
       <c r="B307" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Save Chart</v>
       </c>
       <c r="C307" t="str">
-        <v>确认更改数据包</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B308" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C308" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B309" t="str">
-        <v>Save</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C309" t="str">
-        <v>保存</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B310" t="str">
-        <v>Discard</v>
+        <v>Save</v>
       </c>
       <c r="C310" t="str">
-        <v>不保存</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B311" t="str">
-        <v>Use default age range?</v>
+        <v>Discard</v>
       </c>
       <c r="C311" t="str">
-        <v>使用默认时间区间？</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B312" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>Use default age range?</v>
+      </c>
+      <c r="C312" t="str">
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.qsg.title</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B313" t="str">
-        <v>Quick Start Quide</v>
-      </c>
-      <c r="C313" t="str">
-        <v>快速指南</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.qsg.content</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B314" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C314" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.qsg.button</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B315" t="str">
-        <v>Start QSG</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C315" t="str">
-        <v>开始快速指南</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>help.tour.title</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B316" t="str">
-        <v>Tour</v>
+        <v>Start QSG</v>
       </c>
       <c r="C316" t="str">
-        <v>导览</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B317" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Tour</v>
       </c>
       <c r="C317" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>help.tour.content.settings</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B318" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C318" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B319" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C319" t="str">
-        <v>开始数据包导览</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>help.tour.button.settings</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B320" t="str">
-        <v>Start Settings Tour</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C320" t="str">
-        <v>开始设置导览</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>help.license</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B321" t="str">
-        <v>Software License</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C321" t="str">
-        <v>软件许可</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.license</v>
       </c>
       <c r="B322" t="str">
-        <v>File Format Info</v>
+        <v>Software License</v>
       </c>
       <c r="C322" t="str">
-        <v>文件格式信息</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B323" t="str">
-        <v>View File Format Info</v>
+        <v>File Format Info</v>
       </c>
       <c r="C323" t="str">
-        <v>查看文件格式信息</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.title</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B324" t="str">
-        <v>Error</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C324" t="str">
-        <v>错误</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>errors.title</v>
       </c>
       <c r="B325" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C325" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B326" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C326" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C327" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B328" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C328" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B330" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B331" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B332" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B333" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C333" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B334" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C334" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B335" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C335" t="str">
-        <v>无效的数据包上传</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B336" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid datapack upload.</v>
+      </c>
+      <c r="C336" t="str">
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B337" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
-      </c>
-      <c r="C337" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B338" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C338" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B339" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C339" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B340" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C340" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B341" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C341" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B342" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C342" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B343" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C343" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B344" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C344" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B345" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C345" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B346" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C346" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B347" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C347" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B348" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C348" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B349" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C349" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B350" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C350" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B351" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C351" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B352" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C352" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C354" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B355" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C355" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B356" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C356" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B357" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C357" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B358" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C358" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B359" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C359" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B360" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C360" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B361" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C361" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B362" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B363" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C363" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B364" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C364" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B366" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C366" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B367" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C367" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B368" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C368" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B369" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C369" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B370" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C370" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B371" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C371" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B372" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C372" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B373" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C373" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B374" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C374" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C375" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B376" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C376" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B377" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C377" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B378" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C378" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B379" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C380" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B381" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C381" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B382" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B383" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B384" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
+      </c>
+      <c r="C384" t="str">
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B385" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
-      </c>
-      <c r="C385" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B386" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C386" t="str">
-        <v>不能删除根用户。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B387" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C387" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B388" t="str">
-        <v>Unable to modify user. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
+      </c>
+      <c r="C388" t="str">
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
       </c>
       <c r="B389" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
-      </c>
-      <c r="C389" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>Unable to modify user. Please try again later.</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B390" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C390" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B391" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C391" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B392" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C392" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B393" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C393" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B394" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B395" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C395" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B396" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C396" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C397" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B398" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C398" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B399" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
       </c>
       <c r="C399" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B400" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C400" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B401" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
       </c>
       <c r="C401" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B402" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
       </c>
       <c r="C402" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B403" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>The start date must be before the end date.</v>
       </c>
       <c r="C403" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B404" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>Unable to create workshop. Please try again later.</v>
       </c>
       <c r="C404" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B405" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
       </c>
       <c r="C405" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C406" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B407" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
-      </c>
-      <c r="C407" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B408" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C408" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B410" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B411" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B413" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B414" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B415" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B416" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B417" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B418" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B419" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B420" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B421" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B422" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B423" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B424" t="str">
-        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B425" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B426" t="str">
-        <v>Failed to add files to workshop</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B427" t="str">
-        <v>Failed to add cover to workshop</v>
+        <v>Failed to add files to workshop</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>errors.INVALID_FILE_FORMAT</v>
+        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B428" t="str">
-        <v>Invalid file format.</v>
+        <v>Failed to add cover to workshop</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.INVALID_FILE_FORMAT</v>
       </c>
       <c r="B429" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
-      </c>
-      <c r="C429" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>Invalid file format.</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B430" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C430" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>button.generate</v>
+        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B431" t="str">
-        <v>Generate</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
       </c>
       <c r="C431" t="str">
-        <v>绘制</v>
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.WORKSHOP_FILE_DOWNLOAD_NOT_AUTHORIZED</v>
       </c>
       <c r="B432" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C432" t="str">
-        <v>绘制图表</v>
+        <v>Please register for the workshop to download the file.</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>button.remove-cache</v>
+        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B433" t="str">
-        <v>Remove Cache</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C433" t="str">
-        <v>清除缓存</v>
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>button.confirm-selection</v>
+        <v>button.generate</v>
       </c>
       <c r="B434" t="str">
-        <v>Confirm Selection</v>
+        <v>Generate</v>
       </c>
       <c r="C434" t="str">
-        <v>确认选择</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B435" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Generate Chart</v>
+      </c>
+      <c r="C435" t="str">
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>yes</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B436" t="str">
-        <v>Yes</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C436" t="str">
-        <v>是</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>no</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B437" t="str">
-        <v>No</v>
+        <v>Confirm Selection</v>
       </c>
       <c r="C437" t="str">
-        <v>否</v>
+        <v>确认选择</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>languageNames.en-US</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B438" t="str">
-        <v>English</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>languageNames.en</v>
+        <v>yes</v>
       </c>
       <c r="B439" t="str">
-        <v>English</v>
+        <v>Yes</v>
+      </c>
+      <c r="C439" t="str">
+        <v>是</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>languageNames.zh</v>
+        <v>no</v>
       </c>
       <c r="B440" t="str">
-        <v>中文</v>
+        <v>No</v>
+      </c>
+      <c r="C440" t="str">
+        <v>否</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.quit</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B441" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C441" t="str">
-        <v>退出导览</v>
+        <v>English</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.finish</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B442" t="str">
-        <v>Finish Tour</v>
-      </c>
-      <c r="C442" t="str">
-        <v>结束导览</v>
+        <v>English</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.next</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B443" t="str">
-        <v>Next</v>
-      </c>
-      <c r="C443" t="str">
-        <v>下一步</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.back</v>
+        <v>tours.quit</v>
       </c>
       <c r="B444" t="str">
-        <v>Back</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C444" t="str">
-        <v>上一步</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.qsg.step1</v>
+        <v>tours.finish</v>
       </c>
       <c r="B445" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C445" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.next</v>
       </c>
       <c r="B446" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>Next</v>
       </c>
       <c r="C446" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.back</v>
       </c>
       <c r="B447" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>Back</v>
       </c>
       <c r="C447" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C448" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C449" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B450" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C450" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B451" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C451" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B452" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C452" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B453" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C453" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B454" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C454" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B455" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C455" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B456" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C456" t="str">
-        <v>记得确认您的选择</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B457" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C457" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B458" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C458" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B459" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C459" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B460" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C460" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B461" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C461" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step3</v>
       </c>
       <c r="B462" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C462" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step4</v>
       </c>
       <c r="B463" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C463" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step5</v>
+      </c>
+      <c r="B464" t="str">
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C464" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B465" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
       </c>
       <c r="C465" t="str">
-        <v>English</v>
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="str">
-        <v>language-names.en</v>
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B466" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
       </c>
       <c r="C466" t="str">
-        <v>English</v>
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="str">
+        <v>settings.column.tooltip.note-in-range</v>
+      </c>
+      <c r="C467" t="str">
+        <v>数据不在所选时间区间内</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C468" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C469" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C467" t="str">
+      <c r="C470" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C467"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C470"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
linter and translation fixes
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C470"/>
+  <dimension ref="A1:C475"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3176,2005 +3176,2039 @@
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.datapacks.title.treatise</v>
       </c>
       <c r="B279" t="str">
-        <v>No</v>
-      </c>
-      <c r="C279" t="str">
-        <v>暂无</v>
+        <v>Treatise Datapacks</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B280" t="str">
-        <v>Avaliable</v>
+        <v>No</v>
       </c>
       <c r="C280" t="str">
-        <v>可用</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B281" t="str">
-        <v>Upload Datapack</v>
+        <v>Avaliable</v>
       </c>
       <c r="C281" t="str">
-        <v>上传数据包</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B282" t="str">
-        <v>See More...</v>
+        <v>Upload Datapack</v>
+      </c>
+      <c r="C282" t="str">
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B283" t="str">
-        <v>See Less...</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B284" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C284" t="str">
-        <v>上传你的数据包</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B285" t="str">
-        <v>No file selected</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C285" t="str">
-        <v>没有选择文件</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B286" t="str">
-        <v>Datapack Name</v>
+        <v>No file selected</v>
       </c>
       <c r="C286" t="str">
-        <v>数据包名称</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B287" t="str">
-        <v>Enter a name for your datapack.</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C287" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B288" t="str">
-        <v>Authored By</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C288" t="str">
-        <v>作者</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B289" t="str">
-        <v>Credited to...</v>
+        <v>Authored By</v>
       </c>
       <c r="C289" t="str">
-        <v>作者为...</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B290" t="str">
-        <v>Datapack Description</v>
+        <v>Credited to...</v>
       </c>
       <c r="C290" t="str">
-        <v>数据包概述</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B291" t="str">
-        <v>Enter a description for your datapack.</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C291" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B292" t="str">
-        <v>Tags</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C292" t="str">
-        <v>标签</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B293" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Tags</v>
       </c>
       <c r="C293" t="str">
-        <v>使数据包对公共可见</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B294" t="str">
-        <v>Add Reference</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C294" t="str">
-        <v>添加引用</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B295" t="str">
-        <v>More Options</v>
+        <v>Add Reference</v>
       </c>
       <c r="C295" t="str">
-        <v>更多选项</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B296" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>More Options</v>
       </c>
       <c r="C296" t="str">
-        <v>完成并上传</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B297" t="str">
-        <v>Start Over</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C297" t="str">
-        <v>重新开始</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B298" t="str">
-        <v>Reference</v>
+        <v>Start Over</v>
       </c>
       <c r="C298" t="str">
-        <v>引用</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B299" t="str">
-        <v>Contact</v>
+        <v>Reference</v>
       </c>
       <c r="C299" t="str">
-        <v>联系方式</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B300" t="str">
-        <v>Enter your contact information</v>
+        <v>Contact</v>
       </c>
       <c r="C300" t="str">
-        <v>输入你的联系方式</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B301" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C301" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B302" t="str">
-        <v>Notes</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C302" t="str">
-        <v>注释</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B303" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Notes</v>
       </c>
       <c r="C303" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B304" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>Enter notes for the datapack here</v>
       </c>
       <c r="C304" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B305" t="str">
-        <v>PDF Upload</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+      </c>
+      <c r="C305" t="str">
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B306" t="str">
-        <v>You have not made a chart yet</v>
-      </c>
-      <c r="C306" t="str">
-        <v>您还未制作任何图表</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>chart.save</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B307" t="str">
-        <v>Save Chart</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C307" t="str">
-        <v>保存图表</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>chart.save</v>
       </c>
       <c r="B308" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Save Chart</v>
       </c>
       <c r="C308" t="str">
-        <v>确认更改数据包</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B309" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C309" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B310" t="str">
-        <v>Save</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C310" t="str">
-        <v>保存</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B311" t="str">
-        <v>Discard</v>
+        <v>Save</v>
       </c>
       <c r="C311" t="str">
-        <v>不保存</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B312" t="str">
-        <v>Use default age range?</v>
+        <v>Discard</v>
       </c>
       <c r="C312" t="str">
-        <v>使用默认时间区间？</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B313" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>Use default age range?</v>
+      </c>
+      <c r="C313" t="str">
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.qsg.title</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B314" t="str">
-        <v>Quick Start Quide</v>
-      </c>
-      <c r="C314" t="str">
-        <v>快速指南</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.qsg.content</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B315" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C315" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>help.qsg.button</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B316" t="str">
-        <v>Start QSG</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C316" t="str">
-        <v>开始快速指南</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>help.tour.title</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B317" t="str">
-        <v>Tour</v>
+        <v>Start QSG</v>
       </c>
       <c r="C317" t="str">
-        <v>导览</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B318" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Tour</v>
       </c>
       <c r="C318" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>help.tour.content.settings</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B319" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C319" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B320" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C320" t="str">
-        <v>开始数据包导览</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>help.tour.button.settings</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B321" t="str">
-        <v>Start Settings Tour</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C321" t="str">
-        <v>开始设置导览</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>help.license</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B322" t="str">
-        <v>Software License</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C322" t="str">
-        <v>软件许可</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>help.file-format-info.title</v>
+        <v>help.license</v>
       </c>
       <c r="B323" t="str">
-        <v>File Format Info</v>
+        <v>Software License</v>
       </c>
       <c r="C323" t="str">
-        <v>文件格式信息</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B324" t="str">
-        <v>View File Format Info</v>
+        <v>File Format Info</v>
       </c>
       <c r="C324" t="str">
-        <v>查看文件格式信息</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.title</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B325" t="str">
-        <v>Error</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C325" t="str">
-        <v>错误</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>errors.title</v>
       </c>
       <c r="B326" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>Error</v>
       </c>
       <c r="C326" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C327" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B328" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
       </c>
       <c r="C328" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B331" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B332" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B333" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C333" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B334" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C334" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B335" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C335" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B336" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C336" t="str">
-        <v>无效的数据包上传</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B337" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid datapack upload.</v>
+      </c>
+      <c r="C337" t="str">
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_DATAPACK_PHYLUM</v>
       </c>
       <c r="B338" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
-      </c>
-      <c r="C338" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>Invalid treatise datapack phylum provided.</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B339" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
-      </c>
-      <c r="C339" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B340" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C340" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B341" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C341" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B342" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C342" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B343" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C343" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B344" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C344" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B345" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C345" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B346" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C346" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B347" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C347" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B348" t="str">
-        <v>Base age must be greater than the top age.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C348" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B349" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C349" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B350" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C350" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B351" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C351" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B352" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C352" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B353" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C353" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C354" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C355" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B356" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C356" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B357" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C357" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B358" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C358" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B359" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C359" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B360" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C360" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B361" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C361" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B362" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B363" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C363" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B364" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C364" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B365" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C365" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B367" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C367" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B368" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C368" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B369" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C369" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B370" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C370" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B371" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C371" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B372" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C372" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B373" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C373" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B374" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C374" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C375" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
       </c>
       <c r="C376" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B377" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C377" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B378" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C378" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B379" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C380" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B381" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B382" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B383" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B384" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C384" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B385" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Server is too busy. Please try again later.</v>
+      </c>
+      <c r="C385" t="str">
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B386" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C386" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B387" t="str">
-        <v>Cannot delete root user.</v>
-      </c>
-      <c r="C387" t="str">
-        <v>不能删除根用户。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B388" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C388" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B389" t="str">
-        <v>Unable to modify user. Please try again later.</v>
+        <v>Cannot delete root user.</v>
+      </c>
+      <c r="C389" t="str">
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B390" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C390" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
       </c>
       <c r="B391" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
-      </c>
-      <c r="C391" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>Unable to modify user. Please try again later.</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B392" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C392" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B393" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C393" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B394" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B395" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C395" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B396" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B397" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
       </c>
       <c r="C397" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B398" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C398" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B399" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
       </c>
       <c r="C399" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B400" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
       </c>
       <c r="C400" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B401" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
       </c>
       <c r="C401" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B402" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
       </c>
       <c r="C402" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B403" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
       </c>
       <c r="C403" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B404" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
       </c>
       <c r="C404" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B405" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>The start date must be before the end date.</v>
       </c>
       <c r="C405" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Unable to create workshop. Please try again later.</v>
       </c>
       <c r="C406" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B407" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
+      </c>
+      <c r="C407" t="str">
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B408" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
       </c>
       <c r="C408" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B410" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C410" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B411" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B413" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B414" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B415" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B416" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B417" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B418" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B419" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B420" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B421" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B422" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B423" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B424" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B425" t="str">
-        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B426" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B427" t="str">
-        <v>Failed to add files to workshop</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B428" t="str">
-        <v>Failed to add cover to workshop</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>errors.INVALID_FILE_FORMAT</v>
+        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B429" t="str">
-        <v>Invalid file format.</v>
+        <v>Failed to add files to workshop</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>errors.WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B430" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
-      </c>
-      <c r="C430" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>Failed to add cover to workshop</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.INVALID_FILE_FORMAT</v>
       </c>
       <c r="B431" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
-      </c>
-      <c r="C431" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>Invalid file format.</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>errors.WORKSHOP_FILE_DOWNLOAD_NOT_AUTHORIZED</v>
+        <v>errors.WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B432" t="str">
-        <v>Please register for the workshop to download the file.</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
+      </c>
+      <c r="C432" t="str">
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>errors.USER_WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.WORKSHOP_FILE_DOWNLOAD_NOT_AUTHORIZED</v>
       </c>
       <c r="B433" t="str">
-        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
-      </c>
-      <c r="C433" t="str">
-        <v>请求文件不存在，请稍后再试或联系开发团队</v>
+        <v>Please register for the workshop to download the file.</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>button.generate</v>
+        <v>errors.INVALID_DATAPACK_HASH</v>
       </c>
       <c r="B434" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C434" t="str">
-        <v>绘制</v>
+        <v>Invalid treatise datapack hash provided.</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.USER_FETCH_HISTORY_FAILED</v>
       </c>
       <c r="B435" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C435" t="str">
-        <v>绘制图表</v>
+        <v>Failed to fetch user history. Please try again later.</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>button.remove-cache</v>
+        <v>errors.USER_DELETE_HISTORY_FAILED</v>
       </c>
       <c r="B436" t="str">
-        <v>Remove Cache</v>
-      </c>
-      <c r="C436" t="str">
-        <v>清除缓存</v>
+        <v>Failed to delete user history. Please try again later</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>button.confirm-selection</v>
+        <v>errors.USER_FETCH_HISTORY_METADATA_FAILED</v>
       </c>
       <c r="B437" t="str">
-        <v>Confirm Selection</v>
-      </c>
-      <c r="C437" t="str">
-        <v>确认选择</v>
+        <v>Failed to fetch user history metadata. Please try again later</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>errors.USER_FETCH_HISTORY_FAILED_DATAPACKS_MISSING</v>
       </c>
       <c r="B438" t="str">
-        <v>Generate Cross Plot</v>
+        <v>This chart entry couldn't be loaded due to missing files and has been removed from your history.</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>yes</v>
+        <v>button.generate</v>
       </c>
       <c r="B439" t="str">
-        <v>Yes</v>
+        <v>Generate</v>
       </c>
       <c r="C439" t="str">
-        <v>是</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>no</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B440" t="str">
-        <v>No</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C440" t="str">
-        <v>否</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>languageNames.en-US</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B441" t="str">
-        <v>English</v>
+        <v>Remove Cache</v>
+      </c>
+      <c r="C441" t="str">
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>languageNames.en</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B442" t="str">
-        <v>English</v>
+        <v>Confirm Selection</v>
+      </c>
+      <c r="C442" t="str">
+        <v>确认选择</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>languageNames.zh</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B443" t="str">
-        <v>中文</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.quit</v>
+        <v>yes</v>
       </c>
       <c r="B444" t="str">
-        <v>Quit Tour</v>
+        <v>Yes</v>
       </c>
       <c r="C444" t="str">
-        <v>退出导览</v>
+        <v>是</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.finish</v>
+        <v>no</v>
       </c>
       <c r="B445" t="str">
-        <v>Finish Tour</v>
+        <v>No</v>
       </c>
       <c r="C445" t="str">
-        <v>结束导览</v>
+        <v>否</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.next</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B446" t="str">
-        <v>Next</v>
-      </c>
-      <c r="C446" t="str">
-        <v>下一步</v>
+        <v>English</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.back</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B447" t="str">
-        <v>Back</v>
-      </c>
-      <c r="C447" t="str">
-        <v>上一步</v>
+        <v>English</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.qsg.step1</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
-      </c>
-      <c r="C448" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.qsg.step2</v>
+        <v>tours.quit</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C449" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>tours.qsg.step3</v>
+        <v>tours.finish</v>
       </c>
       <c r="B450" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+        <v>Finish Tour</v>
       </c>
       <c r="C450" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>tours.qsg.step4</v>
+        <v>tours.next</v>
       </c>
       <c r="B451" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+        <v>Next</v>
       </c>
       <c r="C451" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>tours.qsg.step5</v>
+        <v>tours.back</v>
       </c>
       <c r="B452" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+        <v>Back</v>
       </c>
       <c r="C452" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
-        <v>tours.qsg.step6</v>
+        <v>tours.qsg.step1</v>
       </c>
       <c r="B453" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
       </c>
       <c r="C453" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="str">
-        <v>tours.qsg.step7</v>
+        <v>tours.qsg.step2</v>
       </c>
       <c r="B454" t="str">
-        <v>The About Page provides information about our development team.</v>
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
       </c>
       <c r="C454" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="str">
-        <v>tours.qsg.step8</v>
+        <v>tours.qsg.step3</v>
       </c>
       <c r="B455" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
       </c>
       <c r="C455" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="str">
-        <v>tours.datapack.step1</v>
+        <v>tours.qsg.step4</v>
       </c>
       <c r="B456" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
       </c>
       <c r="C456" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="str">
-        <v>tours.datapack.step2</v>
+        <v>tours.qsg.step5</v>
       </c>
       <c r="B457" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
       </c>
       <c r="C457" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="str">
-        <v>tours.datapack.step3</v>
+        <v>tours.qsg.step6</v>
       </c>
       <c r="B458" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
       </c>
       <c r="C458" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="str">
-        <v>tours.datapack.step4</v>
+        <v>tours.qsg.step7</v>
       </c>
       <c r="B459" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>The About Page provides information about our development team.</v>
       </c>
       <c r="C459" t="str">
-        <v>记得确认您的选择</v>
+        <v>关于页面提供了我们开发团队的信息。</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="str">
-        <v>tours.settings.step1</v>
+        <v>tours.qsg.step8</v>
       </c>
       <c r="B460" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
       </c>
       <c r="C460" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="str">
-        <v>tours.settings.step2</v>
+        <v>tours.datapack.step1</v>
       </c>
       <c r="B461" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
       </c>
       <c r="C461" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="str">
-        <v>tours.settings.step3</v>
+        <v>tours.datapack.step2</v>
       </c>
       <c r="B462" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>Add a datapack by clicking the checkbox</v>
       </c>
       <c r="C462" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>勾选添加您想要的数据包</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="str">
-        <v>tours.settings.step4</v>
+        <v>tours.datapack.step3</v>
       </c>
       <c r="B463" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+        <v>Click the deselect icon to deselect all datapacks</v>
       </c>
       <c r="C463" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>点此取消选择所有数据包</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="str">
-        <v>tours.settings.step5</v>
+        <v>tours.datapack.step4</v>
       </c>
       <c r="B464" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+        <v>Remember to confirm your selection</v>
       </c>
       <c r="C464" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>记得确认您的选择</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="str">
-        <v>tours.settings.step6</v>
+        <v>tours.settings.step1</v>
       </c>
       <c r="B465" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
       </c>
       <c r="C465" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.settings.step2</v>
       </c>
       <c r="B466" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
       </c>
       <c r="C466" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.settings.step3</v>
+      </c>
+      <c r="B467" t="str">
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
       </c>
       <c r="C467" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.settings.step4</v>
+      </c>
+      <c r="B468" t="str">
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
       </c>
       <c r="C468" t="str">
-        <v>English</v>
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="str">
-        <v>language-names.en</v>
+        <v>tours.settings.step5</v>
+      </c>
+      <c r="B469" t="str">
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
       </c>
       <c r="C469" t="str">
-        <v>English</v>
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="str">
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B470" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+      </c>
+      <c r="C470" t="str">
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="str">
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B471" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+      </c>
+      <c r="C471" t="str">
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="str">
+        <v>settings.column.tooltip.note-in-range</v>
+      </c>
+      <c r="C472" t="str">
+        <v>数据不在所选时间区间内</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C473" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C474" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C470" t="str">
+      <c r="C475" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C470"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C475"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed empty sx and changed workshop tooltip
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -636,7 +636,7 @@
         <v>landing-page.carousel.upload.collaborate.description</v>
       </c>
       <c r="B32" t="str">
-        <v>View other users' datapacks and collaborate to expand your knowledge and expertise.</v>
+        <v>View other users&amp;apos; datapacks and collaborate to expand your knowledge and expertise.</v>
       </c>
     </row>
     <row r="33">
@@ -813,7 +813,7 @@
         <v>login.signup</v>
       </c>
       <c r="B53" t="str">
-        <v>Don't have an account? Sign Up</v>
+        <v>Don&amp;apos;t have an account? Sign Up</v>
       </c>
       <c r="C53" t="str">
         <v>还没有账户？注册账户</v>
@@ -1467,7 +1467,7 @@
         <v>workshops.details-page.download-tooltip-not-registered</v>
       </c>
       <c r="B113" t="str">
-        <v>Please register for the workshop to download the files.</v>
+        <v>Contact jogg@purdue.edu to register!</v>
       </c>
     </row>
     <row r="114">
@@ -2167,7 +2167,7 @@
         <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B184" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Do not use the Data-Pack&amp;apos;s suggested age span</v>
       </c>
       <c r="C184" t="str">
         <v>禁用数据包建议的时间区间</v>
@@ -2200,7 +2200,7 @@
         <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B187" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>This will overwrite any changes you&amp;apos;ve made!</v>
       </c>
       <c r="C187" t="str">
         <v>这将覆盖你所做的任何更改！</v>
@@ -3571,7 +3571,7 @@
         <v>help.qsg.content</v>
       </c>
       <c r="B316" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the &amp;apos;Start QSG&amp;apos; button to begin.</v>
       </c>
       <c r="C316" t="str">
         <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
@@ -4820,7 +4820,7 @@
         <v>errors.USER_FETCH_HISTORY_FAILED_DATAPACKS_MISSING</v>
       </c>
       <c r="B438" t="str">
-        <v>This chart entry couldn't be loaded due to missing files and has been removed from your history.</v>
+        <v>This chart entry couldn&amp;apos;t be loaded due to missing files and has been removed from your history.</v>
       </c>
     </row>
     <row r="439">

</xml_diff>

<commit_message>
add the translation fixes
</commit_message>
<xml_diff>
--- a/server/assets/translation.xlsx
+++ b/server/assets/translation.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C453"/>
+  <dimension ref="A1:C475"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1464,303 +1464,303 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>workshops.calendar.switchLabel</v>
+        <v>workshops.details-page.download-tooltip-not-registered</v>
       </c>
       <c r="B113" t="str">
-        <v>Toggle calendar</v>
+        <v>Contact jogg@purdue.edu to register!</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>workshops.calendar.month</v>
+        <v>workshops.calendar.switchLabel</v>
       </c>
       <c r="B114" t="str">
-        <v>Month</v>
+        <v>Toggle calendar</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>workshops.calendar.week</v>
+        <v>workshops.calendar.month</v>
       </c>
       <c r="B115" t="str">
-        <v>Week</v>
+        <v>Month</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>workshops.calendar.days.sunday</v>
+        <v>workshops.calendar.week</v>
       </c>
       <c r="B116" t="str">
-        <v>Sun</v>
+        <v>Week</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>workshops.calendar.days.monday</v>
+        <v>workshops.calendar.days.sunday</v>
       </c>
       <c r="B117" t="str">
-        <v>Mon</v>
+        <v>Sun</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>workshops.calendar.days.tuesday</v>
+        <v>workshops.calendar.days.monday</v>
       </c>
       <c r="B118" t="str">
-        <v>Tue</v>
+        <v>Mon</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>workshops.calendar.days.wednesday</v>
+        <v>workshops.calendar.days.tuesday</v>
       </c>
       <c r="B119" t="str">
-        <v>Wed</v>
+        <v>Tue</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>workshops.calendar.days.thursday</v>
+        <v>workshops.calendar.days.wednesday</v>
       </c>
       <c r="B120" t="str">
-        <v>Thu</v>
+        <v>Wed</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>workshops.calendar.days.friday</v>
+        <v>workshops.calendar.days.thursday</v>
       </c>
       <c r="B121" t="str">
-        <v>Fri</v>
+        <v>Thu</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>workshops.calendar.days.saturday</v>
+        <v>workshops.calendar.days.friday</v>
       </c>
       <c r="B122" t="str">
-        <v>Sat</v>
+        <v>Fri</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>workshops.calendar.months.1</v>
+        <v>workshops.calendar.days.saturday</v>
       </c>
       <c r="B123" t="str">
-        <v>January</v>
-      </c>
-      <c r="C123" t="str">
-        <v>一月</v>
+        <v>Sat</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>workshops.calendar.months.2</v>
+        <v>workshops.calendar.months.1</v>
       </c>
       <c r="B124" t="str">
-        <v>February</v>
+        <v>January</v>
       </c>
       <c r="C124" t="str">
-        <v>二月</v>
+        <v>一月</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>workshops.calendar.months.3</v>
+        <v>workshops.calendar.months.2</v>
       </c>
       <c r="B125" t="str">
-        <v>March</v>
+        <v>February</v>
       </c>
       <c r="C125" t="str">
-        <v>三月</v>
+        <v>二月</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>workshops.calendar.months.4</v>
+        <v>workshops.calendar.months.3</v>
       </c>
       <c r="B126" t="str">
-        <v>April</v>
+        <v>March</v>
       </c>
       <c r="C126" t="str">
-        <v>四月</v>
+        <v>三月</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>workshops.calendar.months.5</v>
+        <v>workshops.calendar.months.4</v>
       </c>
       <c r="B127" t="str">
-        <v>May</v>
+        <v>April</v>
       </c>
       <c r="C127" t="str">
-        <v>五月</v>
+        <v>四月</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>workshops.calendar.months.6</v>
+        <v>workshops.calendar.months.5</v>
       </c>
       <c r="B128" t="str">
-        <v>June</v>
+        <v>May</v>
       </c>
       <c r="C128" t="str">
-        <v>六月</v>
+        <v>五月</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>workshops.calendar.months.7</v>
+        <v>workshops.calendar.months.6</v>
       </c>
       <c r="B129" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="C129" t="str">
-        <v>七月</v>
+        <v>六月</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>workshops.calendar.months.8</v>
+        <v>workshops.calendar.months.7</v>
       </c>
       <c r="B130" t="str">
-        <v>August</v>
+        <v>July</v>
       </c>
       <c r="C130" t="str">
-        <v>八月</v>
+        <v>七月</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>workshops.calendar.months.9</v>
+        <v>workshops.calendar.months.8</v>
       </c>
       <c r="B131" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="C131" t="str">
-        <v>九月</v>
+        <v>八月</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>workshops.calendar.months.10</v>
+        <v>workshops.calendar.months.9</v>
       </c>
       <c r="B132" t="str">
-        <v>October</v>
+        <v>September</v>
       </c>
       <c r="C132" t="str">
-        <v>十月</v>
+        <v>九月</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>workshops.calendar.months.11</v>
+        <v>workshops.calendar.months.10</v>
       </c>
       <c r="B133" t="str">
-        <v>November</v>
+        <v>October</v>
       </c>
       <c r="C133" t="str">
-        <v>十一月</v>
+        <v>十月</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>workshops.calendar.months.12</v>
+        <v>workshops.calendar.months.11</v>
       </c>
       <c r="B134" t="str">
-        <v>December</v>
+        <v>November</v>
       </c>
       <c r="C134" t="str">
-        <v>十二月</v>
+        <v>十一月</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>loading.loading-chart</v>
+        <v>workshops.calendar.months.12</v>
       </c>
       <c r="B135" t="str">
-        <v>Loading Chart...</v>
+        <v>December</v>
       </c>
       <c r="C135" t="str">
-        <v>加载图表...</v>
+        <v>十二月</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>loading.loading-datapacks</v>
+        <v>loading.loading-chart</v>
       </c>
       <c r="B136" t="str">
-        <v>Loading Datapacks</v>
+        <v>Loading Chart...</v>
       </c>
       <c r="C136" t="str">
-        <v>加载数据包</v>
+        <v>加载图表...</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>loading.time</v>
+        <v>loading.loading-datapacks</v>
       </c>
       <c r="B137" t="str">
-        <v>this could take more than a minute</v>
+        <v>Loading Datapacks</v>
       </c>
       <c r="C137" t="str">
-        <v>这可能需要超过一分钟</v>
+        <v>加载数据包</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>loading.fetching-datapacks</v>
+        <v>loading.time</v>
       </c>
       <c r="B138" t="str">
-        <v>Fetching Datapacks</v>
+        <v>this could take more than a minute</v>
+      </c>
+      <c r="C138" t="str">
+        <v>这可能需要超过一分钟</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>crossPlot.create-datapack</v>
+        <v>loading.fetching-datapacks</v>
       </c>
       <c r="B139" t="str">
-        <v>Create Datapack</v>
+        <v>Fetching Datapacks</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>crossPlot.time.no-unit-selected</v>
+        <v>crossPlot.time.select-unit</v>
       </c>
       <c r="B140" t="str">
-        <v>No unit selected</v>
+        <v>Please select a unit.</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>crossPlot.time.select-unit</v>
+        <v>crossPlot.time.no-chart-units-available</v>
       </c>
       <c r="B141" t="str">
-        <v>Please select a unit.</v>
+        <v>No units available</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>crossPlot.time.no-chart-units-available</v>
+        <v>crossPlot.time.disabled-unit-reason</v>
       </c>
       <c r="B142" t="str">
-        <v>No units available</v>
+        <v>You cannot change the age unit since it must be on the x-axis.</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>crossPlot.time.disabled-unit-reason</v>
+        <v>crossPlot.time.select-datapack</v>
       </c>
       <c r="B143" t="str">
-        <v>You cannot change the age unit since it must be on the x-axis.</v>
+        <v>Please select a datapack.</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>crossPlot.time.select-datapack</v>
+        <v>crossPlot.time.no-unit-selected</v>
       </c>
       <c r="B144" t="str">
-        <v>Please select a datapack.</v>
+        <v>No unit selected</v>
       </c>
     </row>
     <row r="145">
@@ -1797,3239 +1797,3418 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>settingsTabs.Time</v>
+        <v>crossPlot.create-datapack</v>
       </c>
       <c r="B149" t="str">
-        <v>Time</v>
-      </c>
-      <c r="C149" t="str">
-        <v>选择时间区间</v>
+        <v>Create Datapack</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>settingsTabs.Preferences</v>
+        <v>settingsTabs.Time</v>
       </c>
       <c r="B150" t="str">
-        <v>Preferences</v>
+        <v>Time</v>
       </c>
       <c r="C150" t="str">
-        <v>選擇偏好</v>
+        <v>选择时间区间</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>settingsTabs.Column</v>
+        <v>settingsTabs.Preferences</v>
       </c>
       <c r="B151" t="str">
-        <v>Column</v>
+        <v>Preferences</v>
       </c>
       <c r="C151" t="str">
-        <v>选择列</v>
+        <v>選擇偏好</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>settingsTabs.Search</v>
+        <v>settingsTabs.Column</v>
       </c>
       <c r="B152" t="str">
-        <v>Search</v>
+        <v>Column</v>
       </c>
       <c r="C152" t="str">
-        <v>搜索</v>
+        <v>选择列</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>settingsTabs.Font</v>
+        <v>settingsTabs.Search</v>
       </c>
       <c r="B153" t="str">
-        <v>Font</v>
+        <v>Search</v>
       </c>
       <c r="C153" t="str">
-        <v>字体</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>settingsTabs.Map Points</v>
+        <v>settingsTabs.Font</v>
       </c>
       <c r="B154" t="str">
-        <v>Map Points</v>
+        <v>Font</v>
       </c>
       <c r="C154" t="str">
-        <v>地图</v>
+        <v>字体</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>settingsTabs.Datapacks</v>
+        <v>settingsTabs.Map Points</v>
       </c>
       <c r="B155" t="str">
-        <v>Datapacks</v>
+        <v>Map Points</v>
       </c>
       <c r="C155" t="str">
-        <v>选择数据包</v>
+        <v>地图</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>settingsTabs.General</v>
+        <v>settingsTabs.Datapacks</v>
       </c>
       <c r="B156" t="str">
-        <v>General</v>
+        <v>Datapacks</v>
       </c>
       <c r="C156" t="str">
-        <v>基础选项</v>
+        <v>选择数据包</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>settingsTabs.Data Mining</v>
+        <v>settingsTabs.General</v>
       </c>
       <c r="B157" t="str">
-        <v>Data Mining</v>
+        <v>General</v>
       </c>
       <c r="C157" t="str">
-        <v>数据挖掘</v>
+        <v>基础选项</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>settingsTabs.Curve Drawing</v>
+        <v>settingsTabs.Data Mining</v>
       </c>
       <c r="B158" t="str">
-        <v>Curve Drawing</v>
+        <v>Data Mining</v>
       </c>
       <c r="C158" t="str">
-        <v>绘制曲线图</v>
+        <v>数据挖掘</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>settingsTabs.About</v>
+        <v>settingsTabs.Curve Drawing</v>
       </c>
       <c r="B159" t="str">
-        <v>About</v>
+        <v>Curve Drawing</v>
       </c>
       <c r="C159" t="str">
-        <v>关于</v>
+        <v>绘制曲线图</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>settingsTabs.View Data</v>
+        <v>settingsTabs.Overlay</v>
       </c>
       <c r="B160" t="str">
-        <v>View Data</v>
-      </c>
-      <c r="C160" t="str">
-        <v>查看数据</v>
+        <v>Overlay</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>settingsTabs.Discussion</v>
+        <v>settingsTabs.About</v>
       </c>
       <c r="B161" t="str">
-        <v>Discussion</v>
+        <v>About</v>
       </c>
       <c r="C161" t="str">
-        <v>讨论</v>
+        <v>关于</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>settingsTabs.Warnings</v>
+        <v>settingsTabs.View Data</v>
       </c>
       <c r="B162" t="str">
-        <v>Warnings</v>
+        <v>View Data</v>
       </c>
       <c r="C162" t="str">
-        <v>警告</v>
+        <v>查看数据</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>settingsTabs.Load/Save</v>
+        <v>settingsTabs.Discussion</v>
       </c>
       <c r="B163" t="str">
-        <v>Load/Save</v>
+        <v>Discussion</v>
+      </c>
+      <c r="C163" t="str">
+        <v>讨论</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>settingsTabs.xAxis</v>
+        <v>settingsTabs.Warnings</v>
       </c>
       <c r="B164" t="str">
-        <v>X Axis (Age-only)</v>
+        <v>Warnings</v>
+      </c>
+      <c r="C164" t="str">
+        <v>警告</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>settingsTabs.yAxis</v>
+        <v>settingsTabs.Load/Save</v>
       </c>
       <c r="B165" t="str">
-        <v>Y Axis (Age/Depth)</v>
+        <v>Load/Save</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>settings.time.interval.top</v>
+        <v>settingsTabs.xAxis</v>
       </c>
       <c r="B166" t="str">
-        <v>Top of Interval</v>
-      </c>
-      <c r="C166" t="str">
-        <v>区间顶部</v>
+        <v>X Axis (Age-only)</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>settings.time.interval.base</v>
+        <v>settingsTabs.yAxis</v>
       </c>
       <c r="B167" t="str">
-        <v>Base of Interval</v>
-      </c>
-      <c r="C167" t="str">
-        <v>区间底部</v>
+        <v>Y Axis (Age/Depth)</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>settings.time.interval.top-name</v>
+        <v>settings.time.interval.top</v>
       </c>
       <c r="B168" t="str">
-        <v>Top Age/Stage Name</v>
+        <v>Top of Interval</v>
       </c>
       <c r="C168" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间顶部</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>settings.time.interval.base-name</v>
+        <v>settings.time.interval.base</v>
       </c>
       <c r="B169" t="str">
-        <v>Base Age/Stage Name</v>
+        <v>Base of Interval</v>
       </c>
       <c r="C169" t="str">
-        <v>年代/阶段 名称</v>
+        <v>区间底部</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>settings.time.interval.not-avaliable</v>
+        <v>settings.time.interval.top-name</v>
       </c>
       <c r="B170" t="str">
-        <v>Not Available for this Unit</v>
+        <v>Top Age/Stage Name</v>
       </c>
       <c r="C170" t="str">
-        <v>该时间单位无可选年代</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>settings.time.interval.vertical-scale</v>
+        <v>settings.time.interval.base-name</v>
       </c>
       <c r="B171" t="str">
-        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+        <v>Base Age/Stage Name</v>
       </c>
       <c r="C171" t="str">
-        <v>垂直比例（厘米 每 1</v>
+        <v>年代/阶段 名称</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>settings.time.interval.helper-text</v>
+        <v>settings.time.interval.not-avaliable</v>
       </c>
       <c r="B172" t="str">
-        <v>Base age should be older than top age</v>
+        <v>Not Available for this Unit</v>
       </c>
       <c r="C172" t="str">
-        <v>区间底部年代应大于区间顶部年代</v>
+        <v>该时间单位无可选年代</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>settings.time.interval.vertical-scale-header</v>
+        <v>settings.time.interval.vertical-scale</v>
       </c>
       <c r="B173" t="str">
-        <v>Vertical Scale</v>
+        <v xml:space="preserve">Vertical Scale (cm per 1 </v>
+      </c>
+      <c r="C173" t="str">
+        <v>垂直比例（厘米 每 1</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>settings.preferences.checkboxs.skip-empty-columns</v>
+        <v>settings.time.interval.helper-text</v>
       </c>
       <c r="B174" t="str">
-        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
+        <v>Base age should be older than top age</v>
       </c>
       <c r="C174" t="str">
-        <v>在已选时间段内没有数据的列将不会被画出</v>
+        <v>区间底部年代应大于区间顶部年代</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>settings.preferences.checkboxs.mouse-over-info</v>
+        <v>settings.time.interval.vertical-scale-header</v>
       </c>
       <c r="B175" t="str">
-        <v>Add MouseOver info (popups)</v>
-      </c>
-      <c r="C175" t="str">
-        <v>鼠标移至目标上时显示详细信息</v>
+        <v>Vertical Scale</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>settings.preferences.checkboxs.global-priority</v>
+        <v>settings.preferences.checkboxs.skip-empty-columns</v>
       </c>
       <c r="B176" t="str">
-        <v>Enabled Global Priority Filtering for block columns</v>
+        <v>Gray out (and do not draw) columns which do not have data on the selected time interval</v>
       </c>
       <c r="C176" t="str">
-        <v>启用优先级过滤</v>
+        <v>在已选时间段内没有数据的列将不会被画出</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>settings.preferences.checkboxs.stage-background</v>
+        <v>settings.preferences.checkboxs.mouse-over-info</v>
       </c>
       <c r="B177" t="str">
-        <v>Enabled stage background for event columns</v>
+        <v>Add MouseOver info (popups)</v>
       </c>
       <c r="C177" t="str">
-        <v>启用事件列的背景</v>
+        <v>鼠标移至目标上时显示详细信息</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>settings.preferences.checkboxs.enable-legend</v>
+        <v>settings.preferences.checkboxs.global-priority</v>
       </c>
       <c r="B178" t="str">
-        <v>Enable legend for the chart</v>
+        <v>Enabled Global Priority Filtering for block columns</v>
       </c>
       <c r="C178" t="str">
-        <v>启用添加图例</v>
+        <v>启用优先级过滤</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
+        <v>settings.preferences.checkboxs.stage-background</v>
       </c>
       <c r="B179" t="str">
-        <v>Do not auto-indent lithology patterns</v>
+        <v>Enabled stage background for event columns</v>
       </c>
       <c r="C179" t="str">
-        <v>禁用自动缩进岩性图案</v>
+        <v>启用事件列的背景</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>settings.preferences.checkboxs.conserve-chart</v>
+        <v>settings.preferences.checkboxs.enable-legend</v>
       </c>
       <c r="B180" t="str">
-        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
+        <v>Enable legend for the chart</v>
       </c>
       <c r="C180" t="str">
-        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
+        <v>启用添加图例</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>settings.preferences.checkboxs.hide-block-labels</v>
+        <v>settings.preferences.checkboxs.lithology-auto-indent</v>
       </c>
       <c r="B181" t="str">
-        <v>Hide block labels based on priority</v>
+        <v>Do not auto-indent lithology patterns</v>
       </c>
       <c r="C181" t="str">
-        <v>根据优先级隐藏组标签</v>
+        <v>禁用自动缩进岩性图案</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
+        <v>settings.preferences.checkboxs.conserve-chart</v>
       </c>
       <c r="B182" t="str">
-        <v>Do not use the Data-Pack's suggested age span</v>
+        <v>Conserve Chart Space in Family Tree Plotting (Not implemented)</v>
       </c>
       <c r="C182" t="str">
-        <v>禁用数据包建议的时间区间</v>
+        <v>使用家谱绘图时节省图表空间（暂无该功能）</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>settings.preferences.settings-file.load</v>
+        <v>settings.preferences.checkboxs.hide-block-labels</v>
       </c>
       <c r="B183" t="str">
-        <v>Load Settings</v>
+        <v>Hide block labels based on priority</v>
       </c>
       <c r="C183" t="str">
-        <v>上传设置</v>
+        <v>根据优先级隐藏组标签</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>settings.preferences.settings-file.save</v>
+        <v>settings.preferences.checkboxs.use-suggested-age-spans</v>
       </c>
       <c r="B184" t="str">
-        <v>Save Settings</v>
+        <v>Do not use the Data-Pack's suggested age span</v>
       </c>
       <c r="C184" t="str">
-        <v>保存设置</v>
+        <v>禁用数据包建议的时间区间</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>settings.preferences.settings-file.load-dialog.message</v>
+        <v>settings.preferences.settings-file.load</v>
       </c>
       <c r="B185" t="str">
-        <v>This will overwrite any changes you've made!</v>
+        <v>Load Settings</v>
       </c>
       <c r="C185" t="str">
-        <v>这将覆盖你所做的任何更改！</v>
+        <v>上传设置</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>settings.preferences.settings-file.load-dialog.cancel</v>
+        <v>settings.preferences.settings-file.save</v>
       </c>
       <c r="B186" t="str">
-        <v>Cancel</v>
+        <v>Save Settings</v>
       </c>
       <c r="C186" t="str">
-        <v>取消</v>
+        <v>保存设置</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>settings.preferences.settings-file.load-dialog.load</v>
+        <v>settings.preferences.settings-file.load-dialog.message</v>
       </c>
       <c r="B187" t="str">
-        <v>Load</v>
+        <v>This will overwrite any changes you've made!</v>
       </c>
       <c r="C187" t="str">
-        <v>上传</v>
+        <v>这将覆盖你所做的任何更改！</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>settings.preferences.settings-file.save-dialog.message</v>
+        <v>settings.preferences.settings-file.load-dialog.cancel</v>
       </c>
       <c r="B188" t="str">
-        <v>Please enter the filename below.</v>
+        <v>Cancel</v>
       </c>
       <c r="C188" t="str">
-        <v>请输入文件名</v>
+        <v>取消</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>settings.preferences.settings-file.save-dialog.cancel</v>
+        <v>settings.preferences.settings-file.load-dialog.load</v>
       </c>
       <c r="B189" t="str">
-        <v>Cancel</v>
+        <v>Load</v>
       </c>
       <c r="C189" t="str">
-        <v>取消</v>
+        <v>上传</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>settings.preferences.settings-file.save-dialog.save</v>
+        <v>settings.preferences.settings-file.save-dialog.message</v>
       </c>
       <c r="B190" t="str">
-        <v>Save</v>
+        <v>Please enter the filename below.</v>
       </c>
       <c r="C190" t="str">
-        <v>保存</v>
+        <v>请输入文件名</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>settings.column.tooltip.not-in-range</v>
+        <v>settings.preferences.settings-file.save-dialog.cancel</v>
       </c>
       <c r="B191" t="str">
-        <v>Data not included in time range</v>
+        <v>Cancel</v>
+      </c>
+      <c r="C191" t="str">
+        <v>取消</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>settings.column.tooltip.auto-scale</v>
+        <v>settings.preferences.settings-file.save-dialog.save</v>
       </c>
       <c r="B192" t="str">
-        <v>Auto Scale</v>
+        <v>Save</v>
       </c>
       <c r="C192" t="str">
-        <v>自动缩放</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>settings.column.tooltip.flip</v>
+        <v>settings.column.tooltip.not-in-range</v>
       </c>
       <c r="B193" t="str">
-        <v>Flip Range</v>
-      </c>
-      <c r="C193" t="str">
-        <v>翻转区间</v>
+        <v>Data not included in time range</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>settings.column.titles.column-menu-title</v>
+        <v>settings.column.tooltip.auto-scale</v>
       </c>
       <c r="B194" t="str">
-        <v>Column Customization</v>
+        <v>Auto Scale</v>
       </c>
       <c r="C194" t="str">
-        <v>个性化设置列</v>
+        <v>自动缩放</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>settings.column.titles.data-mining-title</v>
+        <v>settings.column.tooltip.flip</v>
       </c>
       <c r="B195" t="str">
-        <v>Data Mining Settings</v>
+        <v>Flip Range</v>
       </c>
       <c r="C195" t="str">
-        <v>数据挖掘设置</v>
+        <v>翻转区间</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>settings.column.titles.font-option-title</v>
+        <v>settings.column.titles.column-menu-title</v>
       </c>
       <c r="B196" t="str">
-        <v>Font Options for "{{name}}"</v>
+        <v>Column Customization</v>
       </c>
       <c r="C196" t="str">
-        <v>设置"{{name}}"列的字体</v>
+        <v>个性化设置列</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>settings.column.menu.shift-row</v>
+        <v>settings.column.titles.data-mining-title</v>
       </c>
       <c r="B197" t="str">
-        <v>Shift Row Positions</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C197" t="str">
-        <v>移动位置</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>settings.column.menu.edit-name</v>
+        <v>settings.column.titles.font-option-title</v>
       </c>
       <c r="B198" t="str">
-        <v>Edit Title</v>
+        <v>Font Options for "{{name}}"</v>
       </c>
       <c r="C198" t="str">
-        <v>编辑标题</v>
+        <v>设置"{{name}}"列的字体</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>settings.column.menu.background-color</v>
+        <v>settings.column.menu.shift-row</v>
       </c>
       <c r="B199" t="str">
-        <v>Background Color</v>
+        <v>Shift Row Positions</v>
       </c>
       <c r="C199" t="str">
-        <v>背景颜色</v>
+        <v>移动位置</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>settings.column.menu.enable-title</v>
+        <v>settings.column.menu.edit-name</v>
       </c>
       <c r="B200" t="str">
-        <v>Enable Title</v>
+        <v>Edit Title</v>
       </c>
       <c r="C200" t="str">
-        <v>显示标题</v>
+        <v>编辑标题</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>settings.column.menu.show-age-label</v>
+        <v>settings.column.menu.background-color</v>
       </c>
       <c r="B201" t="str">
-        <v>Show Age Label</v>
+        <v>Background Color</v>
       </c>
       <c r="C201" t="str">
-        <v>显示年代</v>
+        <v>背景颜色</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>settings.column.menu.info-box</v>
+        <v>settings.column.menu.enable-title</v>
       </c>
       <c r="B202" t="str">
-        <v>Information and References</v>
+        <v>Enable Title</v>
       </c>
       <c r="C202" t="str">
-        <v>信息与参考</v>
+        <v>显示标题</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>settings.column.menu.add-blank-column</v>
+        <v>settings.column.menu.show-age-label</v>
       </c>
       <c r="B203" t="str">
-        <v>Add Blank Column</v>
+        <v>Show Age Label</v>
       </c>
       <c r="C203" t="str">
-        <v>添加一个空白列</v>
+        <v>显示年代</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>settings.column.menu.add-age-column</v>
+        <v>settings.column.menu.info-box</v>
       </c>
       <c r="B204" t="str">
-        <v>Add Age Column</v>
+        <v>Information and References</v>
       </c>
       <c r="C204" t="str">
-        <v>添加一个年代列</v>
+        <v>信息与参考</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>settings.column.menu.width</v>
+        <v>settings.column.menu.add-blank-column</v>
       </c>
       <c r="B205" t="str">
-        <v>Width</v>
+        <v>Add Blank Column</v>
       </c>
       <c r="C205" t="str">
-        <v>宽</v>
+        <v>添加一个空白列</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>settings.column.menu.orientation.title</v>
+        <v>settings.column.menu.add-age-column</v>
       </c>
       <c r="B206" t="str">
-        <v>Label Orientation</v>
+        <v>Add Age Column</v>
       </c>
       <c r="C206" t="str">
-        <v>图标排布</v>
+        <v>添加一个年代列</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>settings.column.menu.orientation.horizontal</v>
+        <v>settings.column.menu.width</v>
       </c>
       <c r="B207" t="str">
-        <v>Horizontal</v>
+        <v>Width</v>
       </c>
       <c r="C207" t="str">
-        <v>横向</v>
+        <v>宽</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>settings.column.menu.orientation.vertical</v>
+        <v>settings.column.menu.orientation.title</v>
       </c>
       <c r="B208" t="str">
-        <v>Vertical</v>
+        <v>Label Orientation</v>
       </c>
       <c r="C208" t="str">
-        <v>纵向</v>
+        <v>图标排布</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>settings.column.menu.show-uncertainty</v>
+        <v>settings.column.menu.orientation.horizontal</v>
       </c>
       <c r="B209" t="str">
-        <v>Show Uncertainty Labels</v>
+        <v>Horizontal</v>
       </c>
       <c r="C209" t="str">
-        <v>显示不确定性</v>
+        <v>横向</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>settings.column.menu.events</v>
+        <v>settings.column.menu.orientation.vertical</v>
       </c>
       <c r="B210" t="str">
-        <v>Events</v>
+        <v>Vertical</v>
       </c>
       <c r="C210" t="str">
-        <v>事件</v>
+        <v>纵向</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>settings.column.menu.ranges</v>
+        <v>settings.column.menu.show-uncertainty</v>
       </c>
       <c r="B211" t="str">
-        <v>Ranges</v>
+        <v>Show Uncertainty Labels</v>
       </c>
       <c r="C211" t="str">
-        <v>范围</v>
+        <v>显示不确定性</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>settings.column.menu.first-occurrence</v>
+        <v>settings.column.menu.events</v>
       </c>
       <c r="B212" t="str">
-        <v>First Occurrence</v>
+        <v>Events</v>
       </c>
       <c r="C212" t="str">
-        <v>首先发生的优先</v>
+        <v>事件</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>settings.column.menu.last-occurrence</v>
+        <v>settings.column.menu.ranges</v>
       </c>
       <c r="B213" t="str">
-        <v>Last Occurrence</v>
+        <v>Ranges</v>
       </c>
       <c r="C213" t="str">
-        <v>最后发生的优先</v>
+        <v>范围</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>settings.column.menu.alphabetical</v>
+        <v>settings.column.menu.first-occurrence</v>
       </c>
       <c r="B214" t="str">
-        <v>Alphabetical</v>
+        <v>First Occurrence</v>
       </c>
       <c r="C214" t="str">
-        <v>按字母顺序排列</v>
+        <v>首先发生的优先</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>settings.column.menu.ruler.title</v>
+        <v>settings.column.menu.last-occurrence</v>
       </c>
       <c r="B215" t="str">
-        <v>Age Ruler Justification</v>
+        <v>Last Occurrence</v>
       </c>
       <c r="C215" t="str">
-        <v>调整年代刻度尺</v>
+        <v>最后发生的优先</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>settings.column.menu.ruler.left</v>
+        <v>settings.column.menu.alphabetical</v>
       </c>
       <c r="B216" t="str">
-        <v>Left</v>
+        <v>Alphabetical</v>
       </c>
       <c r="C216" t="str">
-        <v>左对齐</v>
+        <v>按字母顺序排列</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>settings.column.menu.ruler.right</v>
+        <v>settings.column.menu.ruler.title</v>
       </c>
       <c r="B217" t="str">
-        <v>Right</v>
+        <v>Age Ruler Justification</v>
       </c>
       <c r="C217" t="str">
-        <v>右对齐</v>
+        <v>调整年代刻度尺</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>settings.column.font-menu.change</v>
+        <v>settings.column.menu.ruler.left</v>
       </c>
       <c r="B218" t="str">
-        <v>Change Font</v>
+        <v>Left</v>
       </c>
       <c r="C218" t="str">
-        <v>更改字体</v>
+        <v>左对齐</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>settings.column.font-menu.additional</v>
+        <v>settings.column.menu.ruler.right</v>
       </c>
       <c r="B219" t="str">
-        <v>Additional fonts for child columns</v>
+        <v>Right</v>
       </c>
       <c r="C219" t="str">
-        <v>子列的更多字体选项</v>
+        <v>右对齐</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>settings.column.datamining-menu.title</v>
+        <v>settings.column.font-menu.change</v>
       </c>
       <c r="B220" t="str">
-        <v>Data Mining Settings</v>
+        <v>Change Font</v>
       </c>
       <c r="C220" t="str">
-        <v>数据挖掘设置</v>
+        <v>更改字体</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>settings.column.datamining-menu.window-size</v>
+        <v>settings.column.font-menu.additional</v>
       </c>
       <c r="B221" t="str">
-        <v>Window Size</v>
+        <v>Additional fonts for child columns</v>
       </c>
       <c r="C221" t="str">
-        <v>窗口大小</v>
+        <v>子列的更多字体选项</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>settings.column.datamining-menu.step-size</v>
+        <v>settings.column.datamining-menu.title</v>
       </c>
       <c r="B222" t="str">
-        <v>Step Size</v>
+        <v>Data Mining Settings</v>
       </c>
       <c r="C222" t="str">
-        <v>步长</v>
+        <v>数据挖掘设置</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>settings.column.datamining-menu.options.frequency</v>
+        <v>settings.column.datamining-menu.window-size</v>
       </c>
       <c r="B223" t="str">
-        <v>Frequency</v>
+        <v>Window Size</v>
       </c>
       <c r="C223" t="str">
-        <v>频率</v>
+        <v>窗口大小</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>settings.column.datamining-menu.options.max-val</v>
+        <v>settings.column.datamining-menu.step-size</v>
       </c>
       <c r="B224" t="str">
-        <v>Maximum Value</v>
+        <v>Step Size</v>
       </c>
       <c r="C224" t="str">
-        <v>最大值</v>
+        <v>步长</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>settings.column.datamining-menu.options.min-val</v>
+        <v>settings.column.datamining-menu.options.frequency</v>
       </c>
       <c r="B225" t="str">
-        <v>Minimum Value</v>
+        <v>Frequency</v>
       </c>
       <c r="C225" t="str">
-        <v>最小值</v>
+        <v>频率</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>settings.column.datamining-menu.options.avg-val</v>
+        <v>settings.column.datamining-menu.options.max-val</v>
       </c>
       <c r="B226" t="str">
-        <v>Average Value</v>
+        <v>Maximum Value</v>
       </c>
       <c r="C226" t="str">
-        <v>平均值</v>
+        <v>最大值</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>settings.column.datamining-menu.options.roc</v>
+        <v>settings.column.datamining-menu.options.min-val</v>
       </c>
       <c r="B227" t="str">
-        <v>Rate of Change</v>
+        <v>Minimum Value</v>
       </c>
       <c r="C227" t="str">
-        <v>变化率</v>
+        <v>最小值</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
+        <v>settings.column.datamining-menu.options.avg-val</v>
       </c>
       <c r="B228" t="str">
-        <v>Frequency of LAD</v>
+        <v>Average Value</v>
       </c>
       <c r="C228" t="str">
-        <v>LAD 频率</v>
+        <v>平均值</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
+        <v>settings.column.datamining-menu.options.roc</v>
       </c>
       <c r="B229" t="str">
-        <v>Frequency of FAD</v>
+        <v>Rate of Change</v>
       </c>
       <c r="C229" t="str">
-        <v>FAD 频率</v>
+        <v>变化率</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>settings.column.datamining-menu.options.combined-events</v>
+        <v>settings.column.datamining-menu.options.freq-of-LAD</v>
       </c>
       <c r="B230" t="str">
-        <v>Combined Events</v>
+        <v>Frequency of LAD</v>
       </c>
       <c r="C230" t="str">
-        <v>组合事件</v>
+        <v>LAD 频率</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>settings.column.datamining-menu.options-title.event</v>
+        <v>settings.column.datamining-menu.options.freq-of-FAD</v>
       </c>
       <c r="B231" t="str">
-        <v>Event Type</v>
+        <v>Frequency of FAD</v>
       </c>
       <c r="C231" t="str">
-        <v>事件类型</v>
+        <v>FAD 频率</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>settings.column.datamining-menu.options-title.chron</v>
+        <v>settings.column.datamining-menu.options.combined-events</v>
       </c>
       <c r="B232" t="str">
-        <v>Chron Type</v>
+        <v>Combined Events</v>
       </c>
       <c r="C232" t="str">
-        <v>年代类型</v>
+        <v>组合事件</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>settings.column.datamining-menu.options-title.plot</v>
+        <v>settings.column.datamining-menu.options-title.event</v>
       </c>
       <c r="B233" t="str">
-        <v>Data Type to Plot</v>
+        <v>Event Type</v>
       </c>
       <c r="C233" t="str">
-        <v>绘制数据类型</v>
+        <v>事件类型</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>settings.column.curve-drawing-menu.title</v>
+        <v>settings.column.datamining-menu.options-title.chron</v>
       </c>
       <c r="B234" t="str">
-        <v>Point Settings</v>
+        <v>Chron Type</v>
       </c>
       <c r="C234" t="str">
-        <v>点设置</v>
+        <v>年代类型</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>settings.column.curve-drawing-menu.rod</v>
+        <v>settings.column.datamining-menu.options-title.plot</v>
       </c>
       <c r="B235" t="str">
-        <v>Range of Data</v>
+        <v>Data Type to Plot</v>
       </c>
       <c r="C235" t="str">
-        <v>数据范围</v>
+        <v>绘制数据类型</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>settings.column.curve-drawing-menu.lower-range</v>
+        <v>settings.column.curve-drawing-menu.title</v>
       </c>
       <c r="B236" t="str">
-        <v>Lower Range</v>
+        <v>Point Settings</v>
       </c>
       <c r="C236" t="str">
-        <v>下限</v>
+        <v>点设置</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>settings.column.curve-drawing-menu.upper-range</v>
+        <v>settings.column.curve-drawing-menu.rod</v>
       </c>
       <c r="B237" t="str">
-        <v>Upper Range</v>
+        <v>Range of Data</v>
       </c>
       <c r="C237" t="str">
-        <v>上限</v>
+        <v>数据范围</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>settings.column.curve-drawing-menu.scale-start</v>
+        <v>settings.column.curve-drawing-menu.lower-range</v>
       </c>
       <c r="B238" t="str">
-        <v>Scale Start</v>
+        <v>Lower Range</v>
       </c>
       <c r="C238" t="str">
-        <v>刻度起点</v>
+        <v>下限</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>settings.column.curve-drawing-menu.scale-step</v>
+        <v>settings.column.curve-drawing-menu.upper-range</v>
       </c>
       <c r="B239" t="str">
-        <v>Scale Step</v>
+        <v>Upper Range</v>
       </c>
       <c r="C239" t="str">
-        <v>刻度步长</v>
+        <v>上限</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>settings.column.curve-drawing-menu.show-scale</v>
+        <v>settings.column.curve-drawing-menu.scale-start</v>
       </c>
       <c r="B240" t="str">
-        <v>Show Scale</v>
+        <v>Scale Start</v>
       </c>
       <c r="C240" t="str">
-        <v>显示刻度</v>
+        <v>刻度起点</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>settings.column.curve-drawing-menu.draw-points</v>
+        <v>settings.column.curve-drawing-menu.scale-step</v>
       </c>
       <c r="B241" t="str">
-        <v>Draw Points</v>
+        <v>Scale Step</v>
       </c>
       <c r="C241" t="str">
-        <v>绘制点</v>
+        <v>刻度步长</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>settings.column.curve-drawing-menu.point-shape</v>
+        <v>settings.column.curve-drawing-menu.show-scale</v>
       </c>
       <c r="B242" t="str">
-        <v>Point Shape</v>
+        <v>Show Scale</v>
       </c>
       <c r="C242" t="str">
-        <v>点形状</v>
+        <v>显示刻度</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>settings.column.curve-drawing-menu.line</v>
+        <v>settings.column.curve-drawing-menu.draw-points</v>
       </c>
       <c r="B243" t="str">
-        <v>Line</v>
+        <v>Draw Points</v>
       </c>
       <c r="C243" t="str">
-        <v>线条</v>
+        <v>绘制点</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>settings.column.curve-drawing-menu.fill</v>
+        <v>settings.column.curve-drawing-menu.point-shape</v>
       </c>
       <c r="B244" t="str">
-        <v>Fill</v>
+        <v>Point Shape</v>
       </c>
       <c r="C244" t="str">
-        <v>填充</v>
+        <v>点形状</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>settings.column.curve-drawing-menu.background-gradient</v>
+        <v>settings.column.curve-drawing-menu.line</v>
       </c>
       <c r="B245" t="str">
-        <v>Background Gradient</v>
+        <v>Line</v>
       </c>
       <c r="C245" t="str">
-        <v>背景渐变</v>
+        <v>线条</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>settings.column.curve-drawing-menu.curve-gradient</v>
+        <v>settings.column.curve-drawing-menu.fill</v>
       </c>
       <c r="B246" t="str">
-        <v>Curve Gradient</v>
+        <v>Fill</v>
       </c>
       <c r="C246" t="str">
-        <v>曲线渐变</v>
+        <v>填充</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
-        <v>settings.column.curve-drawing-menu.start</v>
+        <v>settings.column.curve-drawing-menu.background-gradient</v>
       </c>
       <c r="B247" t="str">
-        <v>Start</v>
+        <v>Background Gradient</v>
       </c>
       <c r="C247" t="str">
-        <v>起点</v>
+        <v>背景渐变</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
-        <v>settings.column.curve-drawing-menu.end</v>
+        <v>settings.column.curve-drawing-menu.curve-gradient</v>
       </c>
       <c r="B248" t="str">
-        <v>End</v>
+        <v>Curve Gradient</v>
       </c>
       <c r="C248" t="str">
-        <v>终点</v>
+        <v>曲线渐变</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
-        <v>settings.search.search-bar</v>
+        <v>settings.column.curve-drawing-menu.start</v>
       </c>
       <c r="B249" t="str">
-        <v>Search</v>
+        <v>Start</v>
       </c>
       <c r="C249" t="str">
-        <v>搜索</v>
+        <v>起点</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
-        <v>settings.search.found-result</v>
+        <v>settings.column.curve-drawing-menu.end</v>
       </c>
       <c r="B250" t="str">
-        <v>Found {{count}} Results</v>
+        <v>End</v>
       </c>
       <c r="C250" t="str">
-        <v>找到 {{count}} 个结果</v>
+        <v>终点</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
-        <v>settings.search.current-time-settings</v>
+        <v>settings.column.overlay-menu.title</v>
       </c>
       <c r="B251" t="str">
-        <v>Current Time Settings(Top / Base)</v>
-      </c>
-      <c r="C251" t="str">
-        <v>当前时间区间设置(顶部 / 底部)</v>
+        <v>Overlay Settings</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>settings.search.header.status</v>
+        <v>settings.column.overlay-menu.display-overlay</v>
       </c>
       <c r="B252" t="str">
-        <v>Column On?</v>
-      </c>
-      <c r="C252" t="str">
-        <v>是否已选</v>
+        <v>Display Overlay</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
-        <v>settings.search.header.center</v>
+        <v>settings.column.overlay-menu.overlay-column-header</v>
       </c>
       <c r="B253" t="str">
-        <v>Center</v>
-      </c>
-      <c r="C253" t="str">
-        <v>居中</v>
+        <v>Overlaying</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
-        <v>settings.search.header.extend</v>
+        <v>settings.column.overlay-menu.overlay-column-preposition</v>
       </c>
       <c r="B254" t="str">
-        <v>Extend</v>
-      </c>
-      <c r="C254" t="str">
-        <v>延展</v>
+        <v>On</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>settings.search.header.column</v>
+        <v>settings.column.overlay-menu.overlay-accordion-caption</v>
       </c>
       <c r="B255" t="str">
-        <v>Column</v>
-      </c>
-      <c r="C255" t="str">
-        <v>列名称</v>
+        <v>*Grayed out columns are disabled for Overlay (not Event or Point column)</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>settings.search.header.age</v>
+        <v>settings.column.overlay-menu.invalid-column-mouseover</v>
       </c>
       <c r="B256" t="str">
-        <v>Age</v>
-      </c>
-      <c r="C256" t="str">
-        <v>年代</v>
+        <v>Not an Event or Point Column</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>settings.search.header.qualifier</v>
+        <v>settings.column.overlay-menu.column-not-selected</v>
       </c>
       <c r="B257" t="str">
-        <v>Type</v>
-      </c>
-      <c r="C257" t="str">
-        <v>类别</v>
+        <v>Select Column from Menu</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>settings.search.header.notes</v>
+        <v>settings.search.search-bar</v>
       </c>
       <c r="B258" t="str">
-        <v>Notes</v>
+        <v>Search</v>
       </c>
       <c r="C258" t="str">
-        <v>注释</v>
+        <v>搜索</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
-        <v>settings.font.notes1</v>
+        <v>settings.search.found-result</v>
       </c>
       <c r="B259" t="str">
-        <v>These are the default systemwide fonts.</v>
+        <v>Found {{count}} Results</v>
       </c>
       <c r="C259" t="str">
-        <v>这些是系统默认的全局字体</v>
+        <v>找到 {{count}} 个结果</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>settings.font.notes2</v>
+        <v>settings.search.current-time-settings</v>
       </c>
       <c r="B260" t="str">
-        <v>Changing one here will affect the entire chart.</v>
+        <v>Current Time Settings(Top / Base)</v>
       </c>
       <c r="C260" t="str">
-        <v>在此处更改字体会影响整个图表</v>
+        <v>当前时间区间设置(顶部 / 底部)</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>settings.font.notes3</v>
+        <v>settings.search.header.status</v>
       </c>
       <c r="B261" t="str">
-        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
+        <v>Column On?</v>
       </c>
       <c r="C261" t="str">
-        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
+        <v>是否已选</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>settings.map-points.not-avaliable</v>
+        <v>settings.search.header.center</v>
       </c>
       <c r="B262" t="str">
-        <v>No Map Points available for this datapack</v>
+        <v>Center</v>
       </c>
       <c r="C262" t="str">
-        <v>该数据包暂无地图可用</v>
+        <v>居中</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>settings.datapacks.see-info-guidance</v>
+        <v>settings.search.header.extend</v>
       </c>
       <c r="B263" t="str">
-        <v>Click a datapack to see more information!</v>
+        <v>Extend</v>
       </c>
       <c r="C263" t="str">
-        <v>点击数据包以查看更多信息！</v>
+        <v>延展</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
-        <v>settings.datapacks.add-datapack-guidance</v>
+        <v>settings.search.header.column</v>
       </c>
       <c r="B264" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Column</v>
       </c>
       <c r="C264" t="str">
-        <v>点击加号添加数据包</v>
+        <v>列名称</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
-        <v>settings.datapacks.title.private-official</v>
+        <v>settings.search.header.age</v>
       </c>
       <c r="B265" t="str">
-        <v>Private Official Datapacks</v>
+        <v>Age</v>
+      </c>
+      <c r="C265" t="str">
+        <v>年代</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
-        <v>settings.datapacks.title.public-official</v>
+        <v>settings.search.header.qualifier</v>
       </c>
       <c r="B266" t="str">
-        <v>Official Datapacks</v>
+        <v>Type</v>
+      </c>
+      <c r="C266" t="str">
+        <v>类别</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
-        <v>settings.datapacks.title.contributed</v>
+        <v>settings.search.header.notes</v>
       </c>
       <c r="B267" t="str">
-        <v>User Contributed Datapacks</v>
+        <v>Notes</v>
+      </c>
+      <c r="C267" t="str">
+        <v>注释</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
-        <v>settings.datapacks.title.workshop</v>
+        <v>settings.font.notes1</v>
       </c>
       <c r="B268" t="str">
-        <v>Workshop Datapacks</v>
+        <v>These are the default systemwide fonts.</v>
       </c>
       <c r="C268" t="str">
-        <v>工作坊数据包</v>
+        <v>这些是系统默认的全局字体</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
-        <v>settings.datapacks.title.your</v>
+        <v>settings.font.notes2</v>
       </c>
       <c r="B269" t="str">
-        <v>Your Datapacks</v>
+        <v>Changing one here will affect the entire chart.</v>
       </c>
       <c r="C269" t="str">
-        <v>你的数据包</v>
+        <v>在此处更改字体会影响整个图表</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
-        <v>settings.datapacks.no</v>
+        <v>settings.font.notes3</v>
       </c>
       <c r="B270" t="str">
-        <v>No</v>
+        <v>NOTE: These fonts can be changed on a column by column basis by using the Font button for each column</v>
       </c>
       <c r="C270" t="str">
-        <v>暂无</v>
+        <v>注意：可以通过每列的“字体”按钮单独更改每列的字体</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
-        <v>settings.datapacks.avaliable</v>
+        <v>settings.map-points.not-avaliable</v>
       </c>
       <c r="B271" t="str">
-        <v>Avaliable</v>
+        <v>No Map Points available for this datapack</v>
       </c>
       <c r="C271" t="str">
-        <v>可用</v>
+        <v>该数据包暂无地图可用</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
-        <v>settings.datapacks.upload</v>
+        <v>settings.datapacks.see-info-guidance</v>
       </c>
       <c r="B272" t="str">
-        <v>Upload Datapack</v>
+        <v>Click a datapack to see more information!</v>
       </c>
       <c r="C272" t="str">
-        <v>上传数据包</v>
+        <v>点击数据包以查看更多信息！</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
-        <v>settings.datapacks.pdf-upload</v>
+        <v>settings.datapacks.add-datapack-guidance</v>
       </c>
       <c r="B273" t="str">
-        <v>PDF Upload</v>
+        <v>Add a datapack by clicking the checkbox</v>
+      </c>
+      <c r="C273" t="str">
+        <v>点击加号添加数据包</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>settings.datapacks.seeMore</v>
+        <v>settings.datapacks.title.private-official</v>
       </c>
       <c r="B274" t="str">
-        <v>See More...</v>
+        <v>Private Official Datapacks</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>settings.datapacks.seeLess</v>
+        <v>settings.datapacks.title.public-official</v>
       </c>
       <c r="B275" t="str">
-        <v>See Less...</v>
+        <v>Official Datapacks</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
-        <v>settings.datapacks.upload-form.title</v>
+        <v>settings.datapacks.title.contributed</v>
       </c>
       <c r="B276" t="str">
-        <v>Upload Your Own Datapack</v>
-      </c>
-      <c r="C276" t="str">
-        <v>上传你的数据包</v>
+        <v>User Contributed Datapacks</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
-        <v>settings.datapacks.upload-form.no-file</v>
+        <v>settings.datapacks.title.workshop</v>
       </c>
       <c r="B277" t="str">
-        <v>No file selected</v>
+        <v>Workshop Datapacks</v>
       </c>
       <c r="C277" t="str">
-        <v>没有选择文件</v>
+        <v>工作坊数据包</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
-        <v>settings.datapacks.upload-form.name</v>
+        <v>settings.datapacks.title.your</v>
       </c>
       <c r="B278" t="str">
-        <v>Datapack Name</v>
+        <v>Your Datapacks</v>
       </c>
       <c r="C278" t="str">
-        <v>数据包名称</v>
+        <v>你的数据包</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
-        <v>settings.datapacks.upload-form.name-placeholder</v>
+        <v>settings.datapacks.title.treatise</v>
       </c>
       <c r="B279" t="str">
-        <v>Enter a name for your datapack.</v>
-      </c>
-      <c r="C279" t="str">
-        <v>请为你的数据包输入名称</v>
+        <v>Treatise Datapacks</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
-        <v>settings.datapacks.upload-form.author</v>
+        <v>settings.datapacks.no</v>
       </c>
       <c r="B280" t="str">
-        <v>Authored By</v>
+        <v>No</v>
       </c>
       <c r="C280" t="str">
-        <v>作者</v>
+        <v>暂无</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="str">
-        <v>settings.datapacks.upload-form.author-placeholder</v>
+        <v>settings.datapacks.avaliable</v>
       </c>
       <c r="B281" t="str">
-        <v>Credited to...</v>
+        <v>Avaliable</v>
       </c>
       <c r="C281" t="str">
-        <v>作者为...</v>
+        <v>可用</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="str">
-        <v>settings.datapacks.upload-form.description</v>
+        <v>settings.datapacks.upload</v>
       </c>
       <c r="B282" t="str">
-        <v>Datapack Description</v>
+        <v>Upload Datapack</v>
       </c>
       <c r="C282" t="str">
-        <v>数据包概述</v>
+        <v>上传数据包</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="str">
-        <v>settings.datapacks.upload-form.description-placeholder</v>
+        <v>settings.datapacks.seeMore</v>
       </c>
       <c r="B283" t="str">
-        <v>Enter a description for your datapack.</v>
-      </c>
-      <c r="C283" t="str">
-        <v>请为你的数据包添加概述</v>
+        <v>See More...</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="str">
-        <v>settings.datapacks.upload-form.tags</v>
+        <v>settings.datapacks.seeLess</v>
       </c>
       <c r="B284" t="str">
-        <v>Tags</v>
-      </c>
-      <c r="C284" t="str">
-        <v>标签</v>
+        <v>See Less...</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="str">
-        <v>settings.datapacks.upload-form.make-public</v>
+        <v>settings.datapacks.upload-form.title</v>
       </c>
       <c r="B285" t="str">
-        <v>Make Datapack Publicly Accessible</v>
+        <v>Upload Your Own Datapack</v>
       </c>
       <c r="C285" t="str">
-        <v>使数据包对公共可见</v>
+        <v>上传你的数据包</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="str">
-        <v>settings.datapacks.upload-form.button.add-ref</v>
+        <v>settings.datapacks.upload-form.no-file</v>
       </c>
       <c r="B286" t="str">
-        <v>Add Reference</v>
+        <v>No file selected</v>
       </c>
       <c r="C286" t="str">
-        <v>添加引用</v>
+        <v>没有选择文件</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="str">
-        <v>settings.datapacks.upload-form.button.more</v>
+        <v>settings.datapacks.upload-form.name</v>
       </c>
       <c r="B287" t="str">
-        <v>More Options</v>
+        <v>Datapack Name</v>
       </c>
       <c r="C287" t="str">
-        <v>更多选项</v>
+        <v>数据包名称</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="str">
-        <v>settings.datapacks.upload-form.button.finish</v>
+        <v>settings.datapacks.upload-form.name-placeholder</v>
       </c>
       <c r="B288" t="str">
-        <v>Finish &amp; Upload</v>
+        <v>Enter a name for your datapack.</v>
       </c>
       <c r="C288" t="str">
-        <v>完成并上传</v>
+        <v>请为你的数据包输入名称</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="str">
-        <v>settings.datapacks.upload-form.button.startover</v>
+        <v>settings.datapacks.upload-form.author</v>
       </c>
       <c r="B289" t="str">
-        <v>Start Over</v>
+        <v>Authored By</v>
       </c>
       <c r="C289" t="str">
-        <v>重新开始</v>
+        <v>作者</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="str">
-        <v>settings.datapacks.upload-form.reference</v>
+        <v>settings.datapacks.upload-form.author-placeholder</v>
       </c>
       <c r="B290" t="str">
-        <v>Reference</v>
+        <v>Credited to...</v>
       </c>
       <c r="C290" t="str">
-        <v>引用</v>
+        <v>作者为...</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="str">
-        <v>settings.datapacks.upload-form.contact</v>
+        <v>settings.datapacks.upload-form.description</v>
       </c>
       <c r="B291" t="str">
-        <v>Contact</v>
+        <v>Datapack Description</v>
       </c>
       <c r="C291" t="str">
-        <v>联系方式</v>
+        <v>数据包概述</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="str">
-        <v>settings.datapacks.upload-form.contact-placeholder</v>
+        <v>settings.datapacks.upload-form.description-placeholder</v>
       </c>
       <c r="B292" t="str">
-        <v>Enter your contact information</v>
+        <v>Enter a description for your datapack.</v>
       </c>
       <c r="C292" t="str">
-        <v>输入你的联系方式</v>
+        <v>请为你的数据包添加概述</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="str">
-        <v>settings.datapacks.upload-form.contact-helper-text</v>
+        <v>settings.datapacks.upload-form.tags</v>
       </c>
       <c r="B293" t="str">
-        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
+        <v>Tags</v>
       </c>
       <c r="C293" t="str">
-        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
+        <v>标签</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="str">
-        <v>settings.datapacks.upload-form.notes</v>
+        <v>settings.datapacks.upload-form.make-public</v>
       </c>
       <c r="B294" t="str">
-        <v>Notes</v>
+        <v>Make Datapack Publicly Accessible</v>
       </c>
       <c r="C294" t="str">
-        <v>注释</v>
+        <v>使数据包对公共可见</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="str">
-        <v>settings.datapacks.upload-form.notes-placeholder</v>
+        <v>settings.datapacks.upload-form.button.add-ref</v>
       </c>
       <c r="B295" t="str">
-        <v>Enter notes for the datapack here</v>
+        <v>Add Reference</v>
       </c>
       <c r="C295" t="str">
-        <v>为你的数据包添加注释</v>
+        <v>添加引用</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="str">
-        <v>settings.datapacks.upload-form.notes-helper-text</v>
+        <v>settings.datapacks.upload-form.button.more</v>
       </c>
       <c r="B296" t="str">
-        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
+        <v>More Options</v>
       </c>
       <c r="C296" t="str">
-        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
+        <v>更多选项</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="str">
-        <v>chart.no-chart-yet</v>
+        <v>settings.datapacks.upload-form.button.finish</v>
       </c>
       <c r="B297" t="str">
-        <v>You have not made a chart yet</v>
+        <v>Finish &amp; Upload</v>
       </c>
       <c r="C297" t="str">
-        <v>您还未制作任何图表</v>
+        <v>完成并上传</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="str">
-        <v>chart.save</v>
+        <v>settings.datapacks.upload-form.button.startover</v>
       </c>
       <c r="B298" t="str">
-        <v>Save Chart</v>
+        <v>Start Over</v>
       </c>
       <c r="C298" t="str">
-        <v>保存图表</v>
+        <v>重新开始</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="str">
-        <v>dialogs.confirm-datapack-change.title</v>
+        <v>settings.datapacks.upload-form.reference</v>
       </c>
       <c r="B299" t="str">
-        <v>Confirm Datapack Selection Change</v>
+        <v>Reference</v>
       </c>
       <c r="C299" t="str">
-        <v>确认更改数据包</v>
+        <v>引用</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="str">
-        <v>dialogs.confirm-datapack-change.message</v>
+        <v>settings.datapacks.upload-form.contact</v>
       </c>
       <c r="B300" t="str">
-        <v>You have unsaved changes! Do you want to save your changes?</v>
+        <v>Contact</v>
       </c>
       <c r="C300" t="str">
-        <v>你有未保存的更改! 你想保存你的更改吗?</v>
+        <v>联系方式</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="str">
-        <v>dialogs.confirm-datapack-change.yes</v>
+        <v>settings.datapacks.upload-form.contact-placeholder</v>
       </c>
       <c r="B301" t="str">
-        <v>Save</v>
+        <v>Enter your contact information</v>
       </c>
       <c r="C301" t="str">
-        <v>保存</v>
+        <v>输入你的联系方式</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="str">
-        <v>dialogs.confirm-datapack-change.no</v>
+        <v>settings.datapacks.upload-form.contact-helper-text</v>
       </c>
       <c r="B302" t="str">
-        <v>Discard</v>
+        <v>(OPTIONAL) If you would like others to contact you about this datapack</v>
       </c>
       <c r="C302" t="str">
-        <v>不保存</v>
+        <v>如果想要其他用户就此数据包问题联系你，请填写</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="str">
-        <v>dialogs.default-age.title</v>
+        <v>settings.datapacks.upload-form.notes</v>
       </c>
       <c r="B303" t="str">
-        <v>Use default age range?</v>
+        <v>Notes</v>
       </c>
       <c r="C303" t="str">
-        <v>使用默认时间区间？</v>
+        <v>注释</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="str">
-        <v>dialogs.confirm-changes.message</v>
+        <v>settings.datapacks.upload-form.notes-placeholder</v>
       </c>
       <c r="B304" t="str">
-        <v>Are you sure you want to discard your changes?</v>
+        <v>Enter notes for the datapack here</v>
+      </c>
+      <c r="C304" t="str">
+        <v>为你的数据包添加注释</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="str">
-        <v>help.qsg.title</v>
+        <v>settings.datapacks.upload-form.notes-helper-text</v>
       </c>
       <c r="B305" t="str">
-        <v>Quick Start Quide</v>
+        <v>(OPTIONAL) Generally notes are settings recommendations/How to use your datapack most efficiently</v>
       </c>
       <c r="C305" t="str">
-        <v>快速指南</v>
+        <v>如果想要指导其他用户如何有效地使用此数据包，请填写</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="str">
-        <v>help.qsg.content</v>
+        <v>settings.datapacks.pdf-upload</v>
       </c>
       <c r="B306" t="str">
-        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
-      </c>
-      <c r="C306" t="str">
-        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
+        <v>PDF Upload</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="str">
-        <v>help.qsg.button</v>
+        <v>chart.no-chart-yet</v>
       </c>
       <c r="B307" t="str">
-        <v>Start QSG</v>
+        <v>You have not made a chart yet</v>
       </c>
       <c r="C307" t="str">
-        <v>开始快速指南</v>
+        <v>您还未制作任何图表</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="str">
-        <v>help.tour.title</v>
+        <v>chart.save</v>
       </c>
       <c r="B308" t="str">
-        <v>Tour</v>
+        <v>Save Chart</v>
       </c>
       <c r="C308" t="str">
-        <v>导览</v>
+        <v>保存图表</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="str">
-        <v>help.tour.content.datapacks</v>
+        <v>dialogs.confirm-datapack-change.title</v>
       </c>
       <c r="B309" t="str">
-        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
+        <v>Confirm Datapack Selection Change</v>
       </c>
       <c r="C309" t="str">
-        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
+        <v>确认更改数据包</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="str">
-        <v>help.tour.content.settings</v>
+        <v>dialogs.confirm-datapack-change.message</v>
       </c>
       <c r="B310" t="str">
-        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
+        <v>You have unsaved changes! Do you want to save your changes?</v>
       </c>
       <c r="C310" t="str">
-        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
+        <v>你有未保存的更改! 你想保存你的更改吗?</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="str">
-        <v>help.tour.button.datapacks</v>
+        <v>dialogs.confirm-datapack-change.yes</v>
       </c>
       <c r="B311" t="str">
-        <v>Start Datapacks Tour</v>
+        <v>Save</v>
       </c>
       <c r="C311" t="str">
-        <v>开始数据包导览</v>
+        <v>保存</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="str">
-        <v>help.tour.button.settings</v>
+        <v>dialogs.confirm-datapack-change.no</v>
       </c>
       <c r="B312" t="str">
-        <v>Start Settings Tour</v>
+        <v>Discard</v>
       </c>
       <c r="C312" t="str">
-        <v>开始设置导览</v>
+        <v>不保存</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="str">
-        <v>help.license</v>
+        <v>dialogs.default-age.title</v>
       </c>
       <c r="B313" t="str">
-        <v>Software License</v>
+        <v>Use default age range?</v>
       </c>
       <c r="C313" t="str">
-        <v>软件许可</v>
+        <v>使用默认时间区间？</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="str">
-        <v>help.file-format-info.title</v>
+        <v>dialogs.confirm-changes.message</v>
       </c>
       <c r="B314" t="str">
-        <v>File Format Info</v>
-      </c>
-      <c r="C314" t="str">
-        <v>文件格式信息</v>
+        <v>Are you sure you want to discard your changes?</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="str">
-        <v>help.file-format-info.link</v>
+        <v>help.qsg.title</v>
       </c>
       <c r="B315" t="str">
-        <v>View File Format Info</v>
+        <v>Quick Start Quide</v>
       </c>
       <c r="C315" t="str">
-        <v>查看文件格式信息</v>
+        <v>快速指南</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="str">
-        <v>errors.title</v>
+        <v>help.qsg.content</v>
       </c>
       <c r="B316" t="str">
-        <v>Error</v>
+        <v>Welcome to Time Scale Creator Online! In this Quick Start Guide, you will quickly learn about the functions of each tab on the Nav bar. Click the 'Start QSG' button to begin.</v>
       </c>
       <c r="C316" t="str">
-        <v>错误</v>
+        <v>欢迎使用Time Scale Creator在线版！在这个快速指南中，您将迅速了解导航栏上每个标签页的功能。点击“开始快速指南”按钮开始体验。</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="str">
-        <v>errors.SERVER_RESPONSE_ERROR</v>
+        <v>help.qsg.button</v>
       </c>
       <c r="B317" t="str">
-        <v>Server response error. Please try again later.</v>
+        <v>Start QSG</v>
       </c>
       <c r="C317" t="str">
-        <v>服务器错误。请稍后再试。</v>
+        <v>开始快速指南</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="str">
-        <v>errors.INVALID_DATAPACK_INFO</v>
+        <v>help.tour.title</v>
       </c>
       <c r="B318" t="str">
-        <v>Invalid datapack info received from server. Please try again later.</v>
+        <v>Tour</v>
       </c>
       <c r="C318" t="str">
-        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
+        <v>导览</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="str">
-        <v>errors.INVALID_PRESET_INFO</v>
+        <v>help.tour.content.datapacks</v>
       </c>
       <c r="B319" t="str">
-        <v>Invalid preset info received from server. Please try again later.</v>
+        <v>In the datapacks tour you will explore the Datapacks page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C319" t="str">
-        <v>从服务器接收到的预置无效。请稍后再试。</v>
+        <v>在数据包导览中，您将深入探索数据包页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="str">
-        <v>errors.INVALID_PATTERN_INFO</v>
+        <v>help.tour.content.settings</v>
       </c>
       <c r="B320" t="str">
-        <v>Invalid pattern info received from server. Please try again later.</v>
+        <v>In the settings tour you will explore the Settings page in depth. Click the button to start your tour!</v>
       </c>
       <c r="C320" t="str">
-        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
+        <v>在设置导览中，您将深入探索设置页面。点击按钮开始您的导览！</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="str">
-        <v>errors.INVALID_TIME_SCALE</v>
+        <v>help.tour.button.datapacks</v>
       </c>
       <c r="B321" t="str">
-        <v>Invalid time scale received from server. Please try again later.</v>
+        <v>Start Datapacks Tour</v>
       </c>
       <c r="C321" t="str">
-        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
+        <v>开始数据包导览</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="str">
-        <v>errors.INVALID_DATAPACK_CONFIG</v>
+        <v>help.tour.button.settings</v>
       </c>
       <c r="B322" t="str">
-        <v>Datapacks were not properly set. Please try again later.</v>
+        <v>Start Settings Tour</v>
       </c>
       <c r="C322" t="str">
-        <v>数据包未正确设置。请稍后再试。</v>
+        <v>开始设置导览</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="str">
-        <v>errors.INVALID_SVG_READY_RESPONSE</v>
+        <v>help.license</v>
       </c>
       <c r="B323" t="str">
-        <v>Invalid SVG ready response received from server. Please try again later.</v>
+        <v>Software License</v>
       </c>
       <c r="C323" t="str">
-        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
+        <v>软件许可</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="str">
-        <v>errors.INVALID_SETTINGS_RESPONSE</v>
+        <v>help.file-format-info.title</v>
       </c>
       <c r="B324" t="str">
-        <v>Invalid settings response received from server. Please try again later.</v>
+        <v>File Format Info</v>
       </c>
       <c r="C324" t="str">
-        <v>从服务器收到的设置响应无效。请稍后再试。</v>
+        <v>文件格式信息</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="str">
-        <v>errors.INVALID_CHART_RESPONSE</v>
+        <v>help.file-format-info.link</v>
       </c>
       <c r="B325" t="str">
-        <v>Invalid chart response received from server. Please try again later.</v>
+        <v>View File Format Info</v>
       </c>
       <c r="C325" t="str">
-        <v>从服务器收到的图表响应无效。请稍后再试。</v>
+        <v>查看文件格式信息</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="str">
-        <v>errors.INVALID_PATH</v>
+        <v>errors.title</v>
       </c>
       <c r="B326" t="str">
-        <v>The requested path was invalid. Please ensure the path is correct.</v>
+        <v>Error</v>
       </c>
       <c r="C326" t="str">
-        <v>请求的文件路径无效。请确保文件路径正确。</v>
+        <v>错误</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="str">
-        <v>errors.INVALID_DATAPACK_UPLOAD</v>
+        <v>errors.SERVER_RESPONSE_ERROR</v>
       </c>
       <c r="B327" t="str">
-        <v>Invalid datapack upload.</v>
+        <v>Server response error. Please try again later.</v>
       </c>
       <c r="C327" t="str">
-        <v>无效的数据包上传</v>
+        <v>服务器错误。请稍后再试。</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="str">
-        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
+        <v>errors.INVALID_DATAPACK_INFO</v>
       </c>
       <c r="B328" t="str">
-        <v>Uploaded datapack is over 3000 characters.</v>
+        <v>Invalid datapack info received from server. Please try again later.</v>
+      </c>
+      <c r="C328" t="str">
+        <v>从服务器接收到的数据包信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="str">
-        <v>errors.INVALID_USER_DATAPACKS</v>
+        <v>errors.INVALID_PRESET_INFO</v>
       </c>
       <c r="B329" t="str">
-        <v>Invalid user datapacks received from server. Please try again later.</v>
+        <v>Invalid preset info received from server. Please try again later.</v>
       </c>
       <c r="C329" t="str">
-        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
+        <v>从服务器接收到的预置无效。请稍后再试。</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="str">
-        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
+        <v>errors.INVALID_PATTERN_INFO</v>
       </c>
       <c r="B330" t="str">
-        <v>Invalid public datapacks received from server. Please try again later.</v>
+        <v>Invalid pattern info received from server. Please try again later.</v>
       </c>
       <c r="C330" t="str">
-        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
+        <v>从服务器接收到的模式信息无效。请稍后再试。</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="str">
-        <v>errors.NO_DATAPACK_FILE_FOUND</v>
+        <v>errors.INVALID_TIME_SCALE</v>
       </c>
       <c r="B331" t="str">
-        <v>No datapack file found. Please upload a datapack file first.</v>
+        <v>Invalid time scale received from server. Please try again later.</v>
       </c>
       <c r="C331" t="str">
-        <v>暂无数据包。请先上传一个数据包。</v>
+        <v>从服务器收到的时间刻度无效。请稍后再试。</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="str">
-        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
+        <v>errors.INVALID_DATAPACK_CONFIG</v>
       </c>
       <c r="B332" t="str">
-        <v>Datapack file name is too long. Please shorten the file name.</v>
+        <v>Datapacks were not properly set. Please try again later.</v>
       </c>
       <c r="C332" t="str">
-        <v>数据包名称过长。请缩短名称。</v>
+        <v>数据包未正确设置。请稍后再试。</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
+        <v>errors.INVALID_SVG_READY_RESPONSE</v>
       </c>
       <c r="B333" t="str">
-        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
+        <v>Invalid SVG ready response received from server. Please try again later.</v>
       </c>
       <c r="C333" t="str">
-        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
+        <v>从服务器收到的SVG就绪响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="str">
-        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
+        <v>errors.INVALID_SETTINGS_RESPONSE</v>
       </c>
       <c r="B334" t="str">
-        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
+        <v>Invalid settings response received from server. Please try again later.</v>
       </c>
       <c r="C334" t="str">
-        <v>无法识别数据包。请上传有效文件。</v>
+        <v>从服务器收到的设置响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="str">
-        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
+        <v>errors.INVALID_CHART_RESPONSE</v>
       </c>
       <c r="B335" t="str">
-        <v>Please finish the datapack upload form before attempting to upload the file.</v>
+        <v>Invalid chart response received from server. Please try again later.</v>
       </c>
       <c r="C335" t="str">
-        <v>请完成数据包上传表单后再尝试上传文件。</v>
+        <v>从服务器收到的图表响应无效。请稍后再试。</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="str">
-        <v>errors.DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.INVALID_PATH</v>
       </c>
       <c r="B336" t="str">
-        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
+        <v>The requested path was invalid. Please ensure the path is correct.</v>
       </c>
       <c r="C336" t="str">
-        <v>数据包已存在。请上传不重名的数据包。</v>
+        <v>请求的文件路径无效。请确保文件路径正确。</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="str">
-        <v>errors.NO_DATAPACKS_SELECTED</v>
+        <v>errors.INVALID_DATAPACK_UPLOAD</v>
       </c>
       <c r="B337" t="str">
-        <v>No datapacks selected. Please select at least one datapack to generate.</v>
+        <v>Invalid datapack upload.</v>
       </c>
       <c r="C337" t="str">
-        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
+        <v>无效的数据包上传</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="str">
-        <v>errors.NO_COLUMNS_SELECTED</v>
+        <v>errors.INVALID_DATAPACK_PHYLUM</v>
       </c>
       <c r="B338" t="str">
-        <v>No columns selected. Please select at least one column to generate.</v>
-      </c>
-      <c r="C338" t="str">
-        <v>未选择列。请至少选择一个列进行绘制。</v>
+        <v>Invalid treatise datapack phylum provided.</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="str">
-        <v>errors.IS_BAD_RANGE</v>
+        <v>errors.REGULAR_USER_UPLOAD_DATAPACK_TOO_LARGE</v>
       </c>
       <c r="B339" t="str">
-        <v>Base age must be greater than the top age.</v>
-      </c>
-      <c r="C339" t="str">
-        <v>区间底部年代应大于区间顶部年代。</v>
+        <v>Uploaded datapack is over 3000 characters.</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="str">
-        <v>errors.INVALID_MAPPACK_INFO</v>
+        <v>errors.INVALID_USER_DATAPACKS</v>
       </c>
       <c r="B340" t="str">
-        <v>Invalid mappack info received from server. Please try again later.</v>
+        <v>Invalid user datapacks received from server. Please try again later.</v>
       </c>
       <c r="C340" t="str">
-        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
+        <v>从服务器收到的用户数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="str">
-        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
+        <v>errors.INVALID_PUBLIC_DATAPACKS</v>
       </c>
       <c r="B341" t="str">
-        <v>Unable to login due to server error. Please try again later.</v>
+        <v>Invalid public datapacks received from server. Please try again later.</v>
       </c>
       <c r="C341" t="str">
-        <v>由于服务器错误无法登陆。请稍后再试。</v>
+        <v>从服务器收到的公共数据包无效。请稍后再试。</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="str">
-        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
+        <v>errors.NO_DATAPACK_FILE_FOUND</v>
       </c>
       <c r="B342" t="str">
-        <v>Unable to login with Google credentials. Please try again.</v>
+        <v>No datapack file found. Please upload a datapack file first.</v>
       </c>
       <c r="C342" t="str">
-        <v>无法使用Google登陆。请稍后再试。</v>
+        <v>暂无数据包。请先上传一个数据包。</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="str">
-        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
+        <v>errors.DATAPACK_FILE_NAME_TOO_LONG</v>
       </c>
       <c r="B343" t="str">
-        <v>Invalid username or password. Please try again.</v>
+        <v>Datapack file name is too long. Please shorten the file name.</v>
       </c>
       <c r="C343" t="str">
-        <v>无效的用户名或密码。请稍后再试。</v>
+        <v>数据包名称过长。请缩短名称。</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="str">
-        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_EXTENSION</v>
       </c>
       <c r="B344" t="str">
-        <v>User with that email already exists. Please log in or sign up with a different email.</v>
+        <v>Unrecognized datapack extension. File must be of type .dpk, .mdpk, .map, .txt. Please upload a valid datapack file.</v>
       </c>
       <c r="C344" t="str">
-        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
+        <v>无法识别数据包扩展名。文件必须是 .dpk, .mdpk, .map, .txt格式。请上传有效文件格式。</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="str">
-        <v>errors.UNABLE_TO_LOGOUT</v>
+        <v>errors.UNRECOGNIZED_DATAPACK_FILE</v>
       </c>
       <c r="B345" t="str">
-        <v>Unable to logout. Please try again later.</v>
+        <v>Unrecognized datapack file. Please upload a valid datapack file.</v>
       </c>
       <c r="C345" t="str">
-        <v>无法登出。请稍后再试。</v>
+        <v>无法识别数据包。请上传有效文件。</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
+        <v>errors.UNFINISHED_DATAPACK_UPLOAD_FORM</v>
       </c>
       <c r="B346" t="str">
-        <v>Unable to sign up due to server error. Please try again later.</v>
+        <v>Please finish the datapack upload form before attempting to upload the file.</v>
       </c>
       <c r="C346" t="str">
-        <v>由于服务器错误无法注册。请稍后再试。</v>
+        <v>请完成数据包上传表单后再尝试上传文件。</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="str">
-        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
+        <v>errors.DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B347" t="str">
-        <v>Email or username already exists. Please try again with a different email or username.</v>
+        <v>Datapack already exists. Please upload a datapack with a unique title.</v>
       </c>
       <c r="C347" t="str">
-        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
+        <v>数据包已存在。请上传不重名的数据包。</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="str">
-        <v>errors.INVALID_FORM</v>
+        <v>errors.NO_DATAPACKS_SELECTED</v>
       </c>
       <c r="B348" t="str">
-        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
+        <v>No datapacks selected. Please select at least one datapack to generate.</v>
       </c>
       <c r="C348" t="str">
-        <v>表格无效。请确保所有栏目填写正确。</v>
+        <v>未选择数据包。请至少选择一个数据包进行绘制。</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
+        <v>errors.NO_COLUMNS_SELECTED</v>
       </c>
       <c r="B349" t="str">
-        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
+        <v>No columns selected. Please select at least one column to generate.</v>
       </c>
       <c r="C349" t="str">
-        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
+        <v>未选择列。请至少选择一个列进行绘制。</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="str">
-        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
+        <v>errors.IS_BAD_RANGE</v>
       </c>
       <c r="B350" t="str">
-        <v>Account is already verified. Please log in.</v>
+        <v>Base age must be greater than the top age.</v>
       </c>
       <c r="C350" t="str">
-        <v>帐户已验证。请登录。</v>
+        <v>区间底部年代应大于区间顶部年代。</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="str">
-        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
+        <v>errors.INVALID_MAPPACK_INFO</v>
       </c>
       <c r="B351" t="str">
-        <v>Unable to verify account due to server error. Please try again later.</v>
+        <v>Invalid mappack info received from server. Please try again later.</v>
       </c>
       <c r="C351" t="str">
-        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
+        <v>从服务器接收到无效的地图包信息。请稍后再试。</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="str">
-        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
+        <v>errors.UNABLE_TO_LOGIN_SERVER</v>
       </c>
       <c r="B352" t="str">
-        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
+        <v>Unable to login due to server error. Please try again later.</v>
       </c>
       <c r="C352" t="str">
-        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
+        <v>由于服务器错误无法登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="str">
-        <v>errors.UNABLE_TO_SEND_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGIN_GOOGLE_CREDENTIAL</v>
       </c>
       <c r="B353" t="str">
-        <v>Unable to send email. Please try again later.</v>
+        <v>Unable to login with Google credentials. Please try again.</v>
       </c>
       <c r="C353" t="str">
-        <v>无法发送邮件。请稍后再试。</v>
+        <v>无法使用Google登陆。请稍后再试。</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="str">
-        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
+        <v>errors.UNABLE_TO_LOGIN_USERNAME_OR_PASSWORD</v>
       </c>
       <c r="B354" t="str">
-        <v>Unable to reset password. Please try again later.</v>
+        <v>Invalid username or password. Please try again.</v>
       </c>
       <c r="C354" t="str">
-        <v>无法重置密码。请稍后再试。</v>
+        <v>无效的用户名或密码。请稍后再试。</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="str">
-        <v>errors.UNABLE_TO_RESET_EMAIL</v>
+        <v>errors.UNABLE_TO_LOGIN_EXISTING_USER</v>
       </c>
       <c r="B355" t="str">
-        <v>Unable to reset email. Please try again later.</v>
+        <v>User with that email already exists. Please log in or sign up with a different email.</v>
       </c>
       <c r="C355" t="str">
-        <v>无法重置邮箱。请稍后再试。</v>
+        <v>已存在使用该电子邮件的用户。请登录或使用其他电子邮件注册。</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="str">
-        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
+        <v>errors.UNABLE_TO_LOGOUT</v>
       </c>
       <c r="B356" t="str">
-        <v>Your account has been locked. Please check your email for more information or contact support.</v>
+        <v>Unable to logout. Please try again later.</v>
       </c>
       <c r="C356" t="str">
-        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
+        <v>无法登出。请稍后再试。</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="str">
-        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
+        <v>errors.UNABLE_TO_SIGNUP_SERVER</v>
       </c>
       <c r="B357" t="str">
-        <v>Unable to recover account. Please contact support for more information.</v>
+        <v>Unable to sign up due to server error. Please try again later.</v>
       </c>
       <c r="C357" t="str">
-        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
+        <v>由于服务器错误无法注册。请稍后再试。</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="str">
-        <v>errors.NOT_LOGGED_IN</v>
+        <v>errors.UNABLE_TO_SIGNUP_USERNAME_OR_EMAIL</v>
       </c>
       <c r="B358" t="str">
-        <v>You are not logged in. Please log in to access this page.</v>
+        <v>Email or username already exists. Please try again with a different email or username.</v>
       </c>
       <c r="C358" t="str">
-        <v>您尚未登录。请登录后访问此页面。</v>
+        <v>电子邮件或用户名已存在。请使用不同的电子邮件或用户名重试。</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="str">
-        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
+        <v>errors.INVALID_FORM</v>
       </c>
       <c r="B359" t="str">
-        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
+        <v>Invalid form. Please ensure all fields are filled out correctly.</v>
       </c>
       <c r="C359" t="str">
-        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
+        <v>表格无效。请确保所有栏目填写正确。</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="str">
-        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT</v>
       </c>
       <c r="B360" t="str">
-        <v>Unable to encrypt the file, please try again later.</v>
+        <v>Your email is not verified. Please verify your email first. If you did not receive an email, please resend.</v>
       </c>
       <c r="C360" t="str">
-        <v>无法加密文件。请稍后再试。</v>
+        <v>您的电子邮件未经验证。请先验证您的电子邮件。如果您没有收到电子邮件，请重新发送。</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="str">
-        <v>errors.TOO_MANY_REQUESTS</v>
+        <v>errors.ALREADY_VERIFIED_ACCOUNT</v>
       </c>
       <c r="B361" t="str">
-        <v>You have made too many requests. Please try again later.</v>
+        <v>Account is already verified. Please log in.</v>
       </c>
       <c r="C361" t="str">
-        <v>请求过于频繁。请稍后再试。</v>
+        <v>帐户已验证。请登录。</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="str">
-        <v>errors.RECAPTCHA_FAILED</v>
+        <v>errors.UNABLE_TO_VERIFY_ACCOUNT_SERVER</v>
       </c>
       <c r="B362" t="str">
-        <v>Recaptcha failed. Please try again.</v>
+        <v>Unable to verify account due to server error. Please try again later.</v>
       </c>
       <c r="C362" t="str">
-        <v>验证失败. 请稍后再试。</v>
+        <v>由于服务器错误，无法验证帐户。请稍后再试。</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="str">
-        <v>errors.COOKIE_REJECTED</v>
+        <v>errors.TOKEN_EXPIRED_OR_INVALID</v>
       </c>
       <c r="B363" t="str">
-        <v>You must accept cookies to sign in.</v>
+        <v>Your token is either invalid or has expired. Please request a new verification email.</v>
       </c>
       <c r="C363" t="str">
-        <v>您必须接受 Cookie 才能登录。</v>
+        <v>您的令牌无效或已过期。请申请新的验证电子邮件。</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="str">
-        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
+        <v>errors.UNABLE_TO_SEND_EMAIL</v>
       </c>
       <c r="B364" t="str">
-        <v>Unrecognized image extension. Please upload a valid image file.</v>
+        <v>Unable to send email. Please try again later.</v>
       </c>
       <c r="C364" t="str">
-        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
+        <v>无法发送邮件。请稍后再试。</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="str">
-        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
+        <v>errors.UNABLE_TO_RESET_PASSWORD</v>
       </c>
       <c r="B365" t="str">
-        <v>Unable to upload profile picture. Please try again later.</v>
+        <v>Unable to reset password. Please try again later.</v>
       </c>
       <c r="C365" t="str">
-        <v>无法上传个人资料图片。请稍后再试。</v>
+        <v>无法重置密码。请稍后再试。</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="str">
-        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
+        <v>errors.UNABLE_TO_RESET_EMAIL</v>
       </c>
       <c r="B366" t="str">
-        <v>Unable to change username. Please try again later.</v>
+        <v>Unable to reset email. Please try again later.</v>
       </c>
       <c r="C366" t="str">
-        <v>无法更改用户名。请稍后再试。</v>
+        <v>无法重置邮箱。请稍后再试。</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="str">
-        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
+        <v>errors.UNABLE_TO_LOGIN_ACCOUNT_LOCKED</v>
       </c>
       <c r="B367" t="str">
-        <v>Unable to delete profile. Please try again later.</v>
+        <v>Your account has been locked. Please check your email for more information or contact support.</v>
       </c>
       <c r="C367" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>您的账户已被锁定。请查看您的电子邮件以获取更多信息或联系技术支持获得帮助。</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="str">
-        <v>errors.INCORRECT_PASSWORD</v>
+        <v>errors.UNABLE_TO_RECOVER_ACCOUNT</v>
       </c>
       <c r="B368" t="str">
-        <v>Incorrect password. Please try again.</v>
+        <v>Unable to recover account. Please contact support for more information.</v>
       </c>
       <c r="C368" t="str">
-        <v>密码错误。请稍后再试。</v>
+        <v>无法恢复账户。请联系技术支持获取更多信息。</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="str">
-        <v>errors.USERNAME_TAKEN</v>
+        <v>errors.NOT_LOGGED_IN</v>
       </c>
       <c r="B369" t="str">
-        <v>Username is already taken. Please try a different username.</v>
+        <v>You are not logged in. Please log in to access this page.</v>
       </c>
       <c r="C369" t="str">
-        <v>用户名已被使用。请使用一个新的用户名。</v>
+        <v>您尚未登录。请登录后访问此页面。</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="str">
-        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
+        <v>errors.USER_DATAPACK_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B370" t="str">
-        <v>Unable to read file or file is empty. Please try again.</v>
+        <v>The datapack requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C370" t="str">
-        <v>无法读取文件或文件为空。请稍后再试。</v>
+        <v>服务器上未找到所请求的数据包。请稍后再试，或联系我们的技术支持团队。</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="str">
-        <v>errors.FETCH_USERS_FAILED</v>
+        <v>errors.INCORRECT_ENCRYPTION_HEADER</v>
       </c>
       <c r="B371" t="str">
-        <v>Unable to fetch users for admin display. Please try again later.</v>
+        <v>Unable to encrypt the file, please try again later.</v>
       </c>
       <c r="C371" t="str">
-        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
+        <v>无法加密文件。请稍后再试。</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="str">
-        <v>errors.ADMIN_ADD_USER_FAILED</v>
+        <v>errors.TOO_MANY_REQUESTS</v>
       </c>
       <c r="B372" t="str">
-        <v>Unable to add user. Please try again later.</v>
+        <v>You have made too many requests. Please try again later.</v>
       </c>
       <c r="C372" t="str">
-        <v>无法添加用户。请稍后再试。</v>
+        <v>请求过于频繁。请稍后再试。</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="str">
-        <v>errors.SERVER_TIMEOUT</v>
+        <v>errors.RECAPTCHA_FAILED</v>
       </c>
       <c r="B373" t="str">
-        <v>Server timed out. Please try again later.</v>
+        <v>Recaptcha failed. Please try again.</v>
       </c>
       <c r="C373" t="str">
-        <v>服务器超时。请稍后再试。</v>
+        <v>验证失败. 请稍后再试。</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="str">
-        <v>errors.SERVER_BUSY</v>
+        <v>errors.COOKIE_REJECTED</v>
       </c>
       <c r="B374" t="str">
-        <v>Server is too busy. Please try again later.</v>
+        <v>You must accept cookies to sign in.</v>
       </c>
       <c r="C374" t="str">
-        <v>服务器忙。请稍后再试。</v>
+        <v>您必须接受 Cookie 才能登录。</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="str">
-        <v>errors.ADMIN_DELETE_USER_FAILED</v>
+        <v>errors.UNRECOGNIZED_IMAGE_FILE</v>
       </c>
       <c r="B375" t="str">
-        <v>Unable to delete user. Please try again later.</v>
+        <v>Unrecognized image extension. Please upload a valid image file.</v>
       </c>
       <c r="C375" t="str">
-        <v>无法删除用户。请稍后再试。</v>
+        <v>图像扩展名无法识别。请上传有效的图像文件。</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="str">
-        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
+        <v>errors.UPLOAD_PROFILE_PICTURE_FAILED</v>
       </c>
       <c r="B376" t="str">
-        <v>Unable to fetch datapacks. Please try again later.</v>
+        <v>Unable to upload profile picture. Please try again later.</v>
+      </c>
+      <c r="C376" t="str">
+        <v>无法上传个人资料图片。请稍后再试。</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="str">
-        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
+        <v>errors.UNABLE_TO_CHANGE_USERNAME</v>
       </c>
       <c r="B377" t="str">
-        <v>Unable to fetch user datapacks. Please try again later.</v>
+        <v>Unable to change username. Please try again later.</v>
       </c>
       <c r="C377" t="str">
-        <v>无法获取用户数据包。请稍后再试。</v>
+        <v>无法更改用户名。请稍后再试。</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="str">
-        <v>errors.CANNOT_DELETE_ROOT_USER</v>
+        <v>errors.UNABLE_TO_DELETE_PROFILE</v>
       </c>
       <c r="B378" t="str">
-        <v>Cannot delete root user.</v>
+        <v>Unable to delete profile. Please try again later.</v>
       </c>
       <c r="C378" t="str">
-        <v>不能删除根用户。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="str">
-        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
+        <v>errors.INCORRECT_PASSWORD</v>
       </c>
       <c r="B379" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Incorrect password. Please try again.</v>
       </c>
       <c r="C379" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>密码错误。请稍后再试。</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="str">
-        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
+        <v>errors.USERNAME_TAKEN</v>
       </c>
       <c r="B380" t="str">
-        <v>Unable to delete server datapack. Please try again later.</v>
+        <v>Username is already taken. Please try a different username.</v>
       </c>
       <c r="C380" t="str">
-        <v>无法删除服务器数据包。请稍后再试。</v>
+        <v>用户名已被使用。请使用一个新的用户名。</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="str">
-        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
+        <v>errors.UNABLE_TO_READ_FILE_OR_EMPTY_FILE</v>
       </c>
       <c r="B381" t="str">
-        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
+        <v>Unable to read file or file is empty. Please try again.</v>
       </c>
       <c r="C381" t="str">
-        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
+        <v>无法读取文件或文件为空。请稍后再试。</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="str">
-        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
+        <v>errors.FETCH_USERS_FAILED</v>
       </c>
       <c r="B382" t="str">
-        <v>Invalid server datapack request. Please try again later.</v>
+        <v>Unable to fetch users for admin display. Please try again later.</v>
       </c>
       <c r="C382" t="str">
-        <v>无效的服务器数据包请求。请稍后再试。</v>
+        <v>无法获取用户信息供管理员查阅。请稍后再试。</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>errors.SERVER_FILE_METADATA_ERROR</v>
+        <v>errors.ADMIN_ADD_USER_FAILED</v>
       </c>
       <c r="B383" t="str">
-        <v>Server file metadata error. Please try again later.</v>
+        <v>Unable to add user. Please try again later.</v>
       </c>
       <c r="C383" t="str">
-        <v>服务器文件元数据错误。请稍后再试。</v>
+        <v>无法添加用户。请稍后再试。</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="str">
-        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
+        <v>errors.SERVER_TIMEOUT</v>
       </c>
       <c r="B384" t="str">
-        <v>Unable to delete user datapack. Please try again later.</v>
+        <v>Server timed out. Please try again later.</v>
       </c>
       <c r="C384" t="str">
-        <v>无法删除用户数据包。请稍后再试。</v>
+        <v>服务器超时。请稍后再试。</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="str">
-        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
+        <v>errors.SERVER_BUSY</v>
       </c>
       <c r="B385" t="str">
-        <v>Failed to process datapack config. Please try again later.</v>
+        <v>Server is too busy. Please try again later.</v>
       </c>
       <c r="C385" t="str">
-        <v>处理数据包配置失败。请稍后再试。</v>
+        <v>服务器忙。请稍后再试。</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="str">
-        <v>errors.INVALID_SETTINGS</v>
+        <v>errors.ADMIN_DELETE_USER_FAILED</v>
       </c>
       <c r="B386" t="str">
-        <v>Invalid settings. Please try again.</v>
+        <v>Unable to delete user. Please try again later.</v>
       </c>
       <c r="C386" t="str">
-        <v>无效的设置。请稍后再试。</v>
+        <v>无法删除用户。请稍后再试。</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="str">
-        <v>errors.INTERNAL_ERROR</v>
+        <v>errors.UNABLE_TO_FETCH_DATAPACKS</v>
       </c>
       <c r="B387" t="str">
-        <v>There was an internal error while generating the chart. Please try again later.</v>
-      </c>
-      <c r="C387" t="str">
-        <v>生成图表时出现内部错误。请稍后再试。</v>
+        <v>Unable to fetch datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
+        <v>errors.UNABLE_TO_FETCH_USER_DATAPACKS</v>
       </c>
       <c r="B388" t="str">
-        <v>Unable to add users to workshop. Please try again later.</v>
+        <v>Unable to fetch user datapacks. Please try again later.</v>
       </c>
       <c r="C388" t="str">
-        <v>无法将用户添加到工作坊。请稍后再试。</v>
+        <v>无法获取用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="str">
-        <v>errors.ADMIN_EMAIL_INVALID</v>
+        <v>errors.CANNOT_DELETE_ROOT_USER</v>
       </c>
       <c r="B389" t="str">
-        <v>Invalid email. Please fix the email and try again.</v>
+        <v>Cannot delete root user.</v>
       </c>
       <c r="C389" t="str">
-        <v>电子邮件无效。请修复电子邮件并重试。</v>
+        <v>不能删除根用户。</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="str">
-        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
+        <v>errors.ADMIN_DELETE_USER_DATAPACK_FAILED</v>
       </c>
       <c r="B390" t="str">
-        <v>You must provide at least one field to add users to a workshop.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C390" t="str">
-        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="str">
-        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
+        <v>errors.ADMIN_MODIFY_USER_FAILED</v>
       </c>
       <c r="B391" t="str">
-        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
-      </c>
-      <c r="C391" t="str">
-        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
+        <v>Unable to modify user. Please try again later.</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="str">
-        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.ADMIN_DELETE_SERVER_DATAPACK_FAILED</v>
       </c>
       <c r="B392" t="str">
-        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+        <v>Unable to delete server datapack. Please try again later.</v>
       </c>
       <c r="C392" t="str">
-        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
+        <v>无法删除服务器数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="str">
-        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
+        <v>errors.ADMIN_CANNOT_DELETE_ROOT_DATAPACK</v>
       </c>
       <c r="B393" t="str">
-        <v>The start date must be before the end date.</v>
+        <v>Cannot delete root datapack. Ask server admin for assistance.</v>
       </c>
       <c r="C393" t="str">
-        <v>开始日期必须早于结束日期</v>
+        <v>无法删除根数据包。请向服务器管理员寻求帮助。</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="str">
-        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
+        <v>errors.INVALID_SERVER_DATAPACK_REQUEST</v>
       </c>
       <c r="B394" t="str">
-        <v>Unable to create workshop. Please try again later.</v>
+        <v>Invalid server datapack request. Please try again later.</v>
       </c>
       <c r="C394" t="str">
-        <v>无法创建工作坊。请稍后再试。</v>
+        <v>无效的服务器数据包请求。请稍后再试。</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="str">
-        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
+        <v>errors.SERVER_FILE_METADATA_ERROR</v>
       </c>
       <c r="B395" t="str">
-        <v>Workshop with that title and dates already exists. Please try again.</v>
+        <v>Server file metadata error. Please try again later.</v>
       </c>
       <c r="C395" t="str">
-        <v>该工作坊名称已存在。请另选名称。</v>
+        <v>服务器文件元数据错误。请稍后再试。</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="str">
-        <v>errors.ADMIN_FETCH_WORKSHOPS_FAILED</v>
+        <v>errors.USER_DELETE_DATAPACK_FAILED</v>
       </c>
       <c r="B396" t="str">
-        <v>Unable to fetch workshops. Please try again later.</v>
+        <v>Unable to delete user datapack. Please try again later.</v>
       </c>
       <c r="C396" t="str">
-        <v>无法抓取工作坊。请稍后再试。</v>
+        <v>无法删除用户数据包。请稍后再试。</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="str">
-        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
+        <v>errors.UNABLE_TO_PROCESS_DATAPACK_CONFIG</v>
       </c>
       <c r="B397" t="str">
-        <v>Unable to delete workshop. Please try again later.</v>
+        <v>Failed to process datapack config. Please try again later.</v>
+      </c>
+      <c r="C397" t="str">
+        <v>处理数据包配置失败。请稍后再试。</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="str">
-        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
+        <v>errors.INVALID_SETTINGS</v>
       </c>
       <c r="B398" t="str">
-        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+        <v>Invalid settings. Please try again.</v>
       </c>
       <c r="C398" t="str">
-        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
+        <v>无效的设置。请稍后再试。</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="str">
-        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
+        <v>errors.INTERNAL_ERROR</v>
       </c>
       <c r="B399" t="str">
-        <v>Unable to edit workshop. Please try again later.</v>
+        <v>There was an internal error while generating the chart. Please try again later.</v>
+      </c>
+      <c r="C399" t="str">
+        <v>生成图表时出现内部错误。请稍后再试。</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="str">
-        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_ADD_USERS_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B400" t="str">
-        <v>Failed to edit user datapack. Please try again later.</v>
+        <v>Unable to add users to workshop. Please try again later.</v>
+      </c>
+      <c r="C400" t="str">
+        <v>无法将用户添加到工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="str">
-        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_EMAIL_INVALID</v>
       </c>
       <c r="B401" t="str">
-        <v>Failed to fetch user datapack. Please try again later.</v>
+        <v>Invalid email. Please fix the email and try again.</v>
+      </c>
+      <c r="C401" t="str">
+        <v>电子邮件无效。请修复电子邮件并重试。</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_FIELDS_EMPTY</v>
       </c>
       <c r="B402" t="str">
-        <v>Failed to replace user datapack file. Please try again later.</v>
+        <v>You must provide at least one field to add users to a workshop.</v>
+      </c>
+      <c r="C402" t="str">
+        <v>您必须提供至少一个领域才能将用户添加到工作坊。</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="str">
-        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
+        <v>errors.UNRECOGNIZED_EXCEL_FILE</v>
       </c>
       <c r="B403" t="str">
-        <v>Failed to replace user datapack profile image. Please try again later.</v>
+        <v>Unrecognized Excel file. Please upload a valid Excel file.</v>
+      </c>
+      <c r="C403" t="str">
+        <v>无法识别 Excel 文件。请上传有效的 Excel 文件。</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="str">
-        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
+        <v>errors.SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B404" t="str">
-        <v>Datapack title cannot have leading or trailing whitespace.</v>
+        <v>Server datapack already exists. Please upload a unique datapack (different title).</v>
+      </c>
+      <c r="C404" t="str">
+        <v>服务器数据包已存在。请上传一个独特的数据包（不同的文件名）。</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="str">
-        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_START_AFTER_END</v>
       </c>
       <c r="B405" t="str">
-        <v>Failed to fetch private datapacks. Please try again later.</v>
+        <v>The start date must be before the end date.</v>
+      </c>
+      <c r="C405" t="str">
+        <v>开始日期必须早于结束日期</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
+        <v>errors.ADMIN_CREATE_WORKSHOP_FAILED</v>
       </c>
       <c r="B406" t="str">
-        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
+        <v>Unable to create workshop. Please try again later.</v>
+      </c>
+      <c r="C406" t="str">
+        <v>无法创建工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_ALREADY_EXISTS</v>
       </c>
       <c r="B407" t="str">
-        <v>Failed to add official datapack to workshop. Please try again later.</v>
+        <v>Workshop with that title and dates already exists. Please try again.</v>
+      </c>
+      <c r="C407" t="str">
+        <v>该工作坊名称已存在。请另选名称。</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="str">
-        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
+        <v>errors.FETCH_WORKSHOPS_FAILED</v>
       </c>
       <c r="B408" t="str">
-        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
+        <v>Unable to fetch workshops. Please try again later.</v>
+      </c>
+      <c r="C408" t="str">
+        <v>无法抓取工作坊。请稍后再试。</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="str">
-        <v>errors.ADMIN_WORKSHOP_ENDED</v>
+        <v>errors.ADMIN_DELETE_WORKSHOP_FAILED</v>
       </c>
       <c r="B409" t="str">
-        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
+        <v>Unable to delete workshop. Please try again later.</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="str">
-        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
+        <v>errors.ADMIN_WORKSHOP_NOT_FOUND</v>
       </c>
       <c r="B410" t="str">
-        <v>Failed to fetch workshop datapacks. Please try again later.</v>
+        <v>Workshop not found on server, it has likely ended or been deleted.</v>
+      </c>
+      <c r="C410" t="str">
+        <v>服务器未找到工作坊。该工作坊可能已结束或被删除。</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="str">
-        <v>errors.METADATA_NOT_FOUND</v>
+        <v>errors.ADMIN_WORKSHOP_EDIT_FAILED</v>
       </c>
       <c r="B411" t="str">
-        <v>Metadata not found. Please try again later.</v>
+        <v>Unable to edit workshop. Please try again later.</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="str">
-        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
+        <v>errors.USER_EDIT_DATAPACK_FAILED</v>
       </c>
       <c r="B412" t="str">
-        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
+        <v>Failed to edit user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="str">
-        <v>errors.INVALID_CROSSPLOT_UNITS</v>
+        <v>errors.USER_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B413" t="str">
-        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
+        <v>Failed to fetch user datapack. Please try again later.</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="str">
-        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
+        <v>errors.USER_REPLACE_DATAPACK_FILE_FAILED</v>
       </c>
       <c r="B414" t="str">
-        <v>Crossplot conversion failed. Please try again later.</v>
+        <v>Failed to replace user datapack file. Please try again later.</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="str">
-        <v>errors.NO_MODELS</v>
+        <v>errors.USER_REPLACE_DATAPACK_PROFILE_IMAGE_FAILED</v>
       </c>
       <c r="B415" t="str">
-        <v>No models available. Please add a model by clicking the chart in the main view.</v>
+        <v>Failed to replace user datapack profile image. Please try again later.</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="str">
-        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
+        <v>errors.DATAPACK_TITLE_LEADING_TRAILING_WHITESPACE</v>
       </c>
       <c r="B416" t="str">
-        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
+        <v>Datapack title cannot have leading or trailing whitespace.</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="str">
-        <v>button.generate</v>
+        <v>errors.ADMIN_FETCH_PRIVATE_DATAPACKS_FAILED</v>
       </c>
       <c r="B417" t="str">
-        <v>Generate</v>
-      </c>
-      <c r="C417" t="str">
-        <v>绘制</v>
+        <v>Failed to fetch private datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="str">
-        <v>button.generate-chart</v>
+        <v>errors.ADMIN_PRIORITY_BATCH_UPDATE_FAILED</v>
       </c>
       <c r="B418" t="str">
-        <v>Generate Chart</v>
-      </c>
-      <c r="C418" t="str">
-        <v>绘制图表</v>
+        <v>Failed to update datapack priorities. Please contact a server admin for assistance.</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="str">
-        <v>button.remove-cache</v>
+        <v>errors.ADMIN_ADD_OFFICIAL_DATAPACK_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B419" t="str">
-        <v>Remove Cache</v>
-      </c>
-      <c r="C419" t="str">
-        <v>清除缓存</v>
+        <v>Failed to add official datapack to workshop. Please try again later.</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="str">
-        <v>button.confirm-selection</v>
+        <v>errors.ADMIN_SERVER_DATAPACK_ALREADY_EXISTS</v>
       </c>
       <c r="B420" t="str">
-        <v>Confirm Selection</v>
-      </c>
-      <c r="C420" t="str">
-        <v>确认选择</v>
+        <v>Server datapack already exists in workshop. Please choose a different datapack.</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="str">
-        <v>button.generate-cross-plot</v>
+        <v>errors.ADMIN_WORKSHOP_ENDED</v>
       </c>
       <c r="B421" t="str">
-        <v>Generate Cross Plot</v>
+        <v>Workshop has ended. You can no longer edit or add datapacks to it.</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="str">
-        <v>yes</v>
+        <v>errors.WORKSHOP_FETCH_DATAPACK_FAILED</v>
       </c>
       <c r="B422" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="C422" t="str">
-        <v>是</v>
+        <v>Failed to fetch workshop datapacks. Please try again later.</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="str">
-        <v>no</v>
+        <v>errors.METADATA_NOT_FOUND</v>
       </c>
       <c r="B423" t="str">
-        <v>No</v>
-      </c>
-      <c r="C423" t="str">
-        <v>否</v>
+        <v>Metadata not found. Please try again later.</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="str">
-        <v>languageNames.en-US</v>
+        <v>errors.INVALID_CROSSPLOT_CONVERSION</v>
       </c>
       <c r="B424" t="str">
-        <v>English</v>
+        <v>Invalid crossplot conversion. Please select a valid chart for the Y Axis.</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="str">
-        <v>languageNames.en</v>
+        <v>errors.INVALID_CROSSPLOT_UNITS</v>
       </c>
       <c r="B425" t="str">
-        <v>English</v>
+        <v>Please select a different unit for the Y Axis. This unit cannot be converted.</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="str">
-        <v>languageNames.zh</v>
+        <v>errors.CROSSPLOT_CONVERSION_FAILED</v>
       </c>
       <c r="B426" t="str">
-        <v>中文</v>
+        <v>Crossplot conversion failed. Please try again later.</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="str">
-        <v>tours.quit</v>
+        <v>errors.NO_MODELS</v>
       </c>
       <c r="B427" t="str">
-        <v>Quit Tour</v>
-      </c>
-      <c r="C427" t="str">
-        <v>退出导览</v>
+        <v>At least 2 models are required for conversion. Please add a model by clicking the chart in the main view.</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="str">
-        <v>tours.finish</v>
+        <v>errors.CROSSPLOT_SETTINGS_MISMATCH</v>
       </c>
       <c r="B428" t="str">
-        <v>Finish Tour</v>
-      </c>
-      <c r="C428" t="str">
-        <v>结束导览</v>
+        <v>Crossplot settings mismatch. Please generate the crossplot with your most recent changes.</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="str">
-        <v>tours.next</v>
+        <v>errors.ADMIN_ADD_FILES_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B429" t="str">
-        <v>Next</v>
-      </c>
-      <c r="C429" t="str">
-        <v>下一步</v>
+        <v>Failed to add files to workshop</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="str">
-        <v>tours.back</v>
+        <v>errors.ADMIN_ADD_COVER_TO_WORKSHOP_FAILED</v>
       </c>
       <c r="B430" t="str">
-        <v>Back</v>
-      </c>
-      <c r="C430" t="str">
-        <v>上一步</v>
+        <v>Failed to add cover to workshop</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="str">
-        <v>tours.qsg.step1</v>
+        <v>errors.INVALID_FILE_FORMAT</v>
       </c>
       <c r="B431" t="str">
-        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
-      </c>
-      <c r="C431" t="str">
-        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+        <v>Invalid file format.</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="str">
-        <v>tours.qsg.step2</v>
+        <v>errors.WORKSHOP_FILE_NOT_FOUND_FOR_DOWNLOAD</v>
       </c>
       <c r="B432" t="str">
-        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+        <v>The workshop file requested was not found on the server. Please try again later or contact our support team.</v>
       </c>
       <c r="C432" t="str">
-        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+        <v>请求文件不存在，请稍后再试或联系开发团队</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="str">
-        <v>tours.qsg.step3</v>
+        <v>errors.WORKSHOP_FILE_DOWNLOAD_NOT_AUTHORIZED</v>
       </c>
       <c r="B433" t="str">
-        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
-      </c>
-      <c r="C433" t="str">
-        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+        <v>Please register for the workshop to download the file.</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="str">
-        <v>tours.qsg.step4</v>
+        <v>errors.INVALID_DATAPACK_HASH</v>
       </c>
       <c r="B434" t="str">
-        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
-      </c>
-      <c r="C434" t="str">
-        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+        <v>Invalid treatise datapack hash provided.</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="str">
-        <v>tours.qsg.step5</v>
+        <v>errors.USER_FETCH_HISTORY_FAILED</v>
       </c>
       <c r="B435" t="str">
-        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
-      </c>
-      <c r="C435" t="str">
-        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+        <v>Failed to fetch user history. Please try again later.</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="str">
-        <v>tours.qsg.step6</v>
+        <v>errors.USER_DELETE_HISTORY_FAILED</v>
       </c>
       <c r="B436" t="str">
-        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
-      </c>
-      <c r="C436" t="str">
-        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+        <v>Failed to delete user history. Please try again later</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="str">
-        <v>tours.qsg.step7</v>
+        <v>errors.USER_FETCH_HISTORY_METADATA_FAILED</v>
       </c>
       <c r="B437" t="str">
-        <v>The About Page provides information about our development team.</v>
-      </c>
-      <c r="C437" t="str">
-        <v>关于页面提供了我们开发团队的信息。</v>
+        <v>Failed to fetch user history metadata. Please try again later</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="str">
-        <v>tours.qsg.step8</v>
+        <v>errors.USER_FETCH_HISTORY_FAILED_DATAPACKS_MISSING</v>
       </c>
       <c r="B438" t="str">
-        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
-      </c>
-      <c r="C438" t="str">
-        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+        <v>This chart entry couldn&amp;apos;t be loaded due to missing files and has been removed from your history.</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="str">
-        <v>tours.datapack.step1</v>
+        <v>button.generate</v>
       </c>
       <c r="B439" t="str">
-        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+        <v>Generate</v>
       </c>
       <c r="C439" t="str">
-        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+        <v>绘制</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="str">
-        <v>tours.datapack.step2</v>
+        <v>button.generate-chart</v>
       </c>
       <c r="B440" t="str">
-        <v>Add a datapack by clicking the checkbox</v>
+        <v>Generate Chart</v>
       </c>
       <c r="C440" t="str">
-        <v>勾选添加您想要的数据包</v>
+        <v>绘制图表</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="str">
-        <v>tours.datapack.step3</v>
+        <v>button.remove-cache</v>
       </c>
       <c r="B441" t="str">
-        <v>Click the deselect icon to deselect all datapacks</v>
+        <v>Remove Cache</v>
       </c>
       <c r="C441" t="str">
-        <v>点此取消选择所有数据包</v>
+        <v>清除缓存</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="str">
-        <v>tours.datapack.step4</v>
+        <v>button.confirm-selection</v>
       </c>
       <c r="B442" t="str">
-        <v>Remember to confirm your selection</v>
+        <v>Confirm Selection</v>
       </c>
       <c r="C442" t="str">
-        <v>记得确认您的选择</v>
+        <v>确认选择</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="str">
-        <v>tours.settings.step1</v>
+        <v>button.generate-cross-plot</v>
       </c>
       <c r="B443" t="str">
-        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
-      </c>
-      <c r="C443" t="str">
-        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+        <v>Generate Cross Plot</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="str">
-        <v>tours.settings.step2</v>
+        <v>yes</v>
       </c>
       <c r="B444" t="str">
-        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+        <v>Yes</v>
       </c>
       <c r="C444" t="str">
-        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+        <v>是</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="str">
-        <v>tours.settings.step3</v>
+        <v>no</v>
       </c>
       <c r="B445" t="str">
-        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+        <v>No</v>
       </c>
       <c r="C445" t="str">
-        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+        <v>否</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="str">
-        <v>tours.settings.step4</v>
+        <v>languageNames.en-US</v>
       </c>
       <c r="B446" t="str">
-        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
-      </c>
-      <c r="C446" t="str">
-        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="str">
-        <v>tours.settings.step5</v>
+        <v>languageNames.en</v>
       </c>
       <c r="B447" t="str">
-        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
-      </c>
-      <c r="C447" t="str">
-        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+        <v>English</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="str">
-        <v>tours.settings.step6</v>
+        <v>languageNames.zh</v>
       </c>
       <c r="B448" t="str">
-        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
-      </c>
-      <c r="C448" t="str">
-        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+        <v>中文</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
-        <v>tours.settings.step7</v>
+        <v>tours.quit</v>
       </c>
       <c r="B449" t="str">
-        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+        <v>Quit Tour</v>
       </c>
       <c r="C449" t="str">
-        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+        <v>退出导览</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="str">
-        <v>settings.column.tooltip.note-in-range</v>
+        <v>tours.finish</v>
+      </c>
+      <c r="B450" t="str">
+        <v>Finish Tour</v>
       </c>
       <c r="C450" t="str">
-        <v>数据不在所选时间区间内</v>
+        <v>结束导览</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="str">
-        <v>language-names.en-US</v>
+        <v>tours.next</v>
+      </c>
+      <c r="B451" t="str">
+        <v>Next</v>
       </c>
       <c r="C451" t="str">
-        <v>English</v>
+        <v>下一步</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="str">
-        <v>language-names.en</v>
+        <v>tours.back</v>
+      </c>
+      <c r="B452" t="str">
+        <v>Back</v>
       </c>
       <c r="C452" t="str">
-        <v>English</v>
+        <v>上一步</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="str">
+        <v>tours.qsg.step1</v>
+      </c>
+      <c r="B453" t="str">
+        <v>In the Presets page, we offer pre-configured settings that allow you to rapidly generate specific types of charts without configuring all options from the beginning. Each preset comes equipped with designated data packs, visual styles, and settings, enabling you to create charts with just a single click.</v>
+      </c>
+      <c r="C453" t="str">
+        <v>在预设页面中，我们提供了预设置，允许您快速生成特定类型的图表，无需从头开始配置所有选项。每个预设都配备了指定的数据包、视觉样式和设置，使您能够一键创建图表</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="str">
+        <v>tours.qsg.step2</v>
+      </c>
+      <c r="B454" t="str">
+        <v>In the Datapacks page, you can select the datapacks required to generate your charts. We offer nine official data packs, each containing a curated collection of datasets tailored for specific thematic explorations. For more detailed guidance on Datapacks, please refer to the Datapacks Tour under the "Tours" section</v>
+      </c>
+      <c r="C454" t="str">
+        <v>在数据包页面，您可以选择生成图表所需的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合集。如需更详细的数据包指导，请参考“导览”部分下的数据包导览。</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="str">
+        <v>tours.qsg.step3</v>
+      </c>
+      <c r="B455" t="str">
+        <v>In the Chart page, you can view the charts you have created and explore the detailed visualizations of geologic events. Additionally, you have the option to download and save these charts for your reference or further analysis.</v>
+      </c>
+      <c r="C455" t="str">
+        <v>在图表页面，您可以查看已创建的图表并探索地质事件的详细可视化图。此外，您还可以下载并保存这些图表以供参考或进一步分析。</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="str">
+        <v>tours.qsg.step4</v>
+      </c>
+      <c r="B456" t="str">
+        <v>In the Settings page, you can customize all aspects of your charts. This includes adjusting the scale and time range, selecting which rows to display, setting the background color and font style, etc. Tailor your charts to meet your specific needs and preferences to optimize your visual analysis. For more detailed guidance on Settings, please refer to the Settings Tour under the "Tours" section</v>
+      </c>
+      <c r="C456" t="str">
+        <v>在设置页面，您可以自定义图表的所有方面。这包括调整比例和时间范围、选择显示哪些行、设置背景色和字体样式等。根据您的具体需求和偏好调整图表，以优化您的视觉分析。如需更详细的设置指导，请参考“导览”部分下的设置导览。</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="str">
+        <v>tours.qsg.step5</v>
+      </c>
+      <c r="B457" t="str">
+        <v>In the Help Page, you can find detailed assistance and information on how to use the website.</v>
+      </c>
+      <c r="C457" t="str">
+        <v>在帮助页面，您可以找到关于如何使用网站的详细帮助和信息。</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="str">
+        <v>tours.qsg.step6</v>
+      </c>
+      <c r="B458" t="str">
+        <v>In the Workshops Page, you can access a range of educational and experimental tutorials that offer in-depth guidance. Here, you can explore the workshops you have registered for, allowing you to engage with the content and enhance your skills in a hands-on learning environment.</v>
+      </c>
+      <c r="C458" t="str">
+        <v>在工作坊页面，您可以访问一系列提供深入指导的教育和实验教程。在这里，您可以探索已注册的研讨会，通过亲身实践的学习环境来提升您的技能。</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="str">
+        <v>tours.qsg.step7</v>
+      </c>
+      <c r="B459" t="str">
+        <v>The About Page provides information about our development team.</v>
+      </c>
+      <c r="C459" t="str">
+        <v>关于页面提供了我们开发团队的信息。</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="str">
+        <v>tours.qsg.step8</v>
+      </c>
+      <c r="B460" t="str">
+        <v>Click here to sign in and unlock the features mentioned earlier, such as accessing registered workshops. Once logged in, you will also have the ability to upload datapacks and take full advantage of all functionalities.</v>
+      </c>
+      <c r="C460" t="str">
+        <v>点击此处登录并解锁前面提到的功能，例如访问工作坊界面。登陆后，您还将能够上传数据包并充分利用所有功能。</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="str">
+        <v>tours.datapack.step1</v>
+      </c>
+      <c r="B461" t="str">
+        <v>Switch between different display types for datapacks: rows, cards, or compact view.</v>
+      </c>
+      <c r="C461" t="str">
+        <v>在数据包显示类型之间切换：行视图、卡片视图或紧凑视图。</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="str">
+        <v>tours.datapack.step2</v>
+      </c>
+      <c r="B462" t="str">
+        <v>Add a datapack by clicking the checkbox</v>
+      </c>
+      <c r="C462" t="str">
+        <v>勾选添加您想要的数据包</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="str">
+        <v>tours.datapack.step3</v>
+      </c>
+      <c r="B463" t="str">
+        <v>Click the deselect icon to deselect all datapacks</v>
+      </c>
+      <c r="C463" t="str">
+        <v>点此取消选择所有数据包</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="str">
+        <v>tours.datapack.step4</v>
+      </c>
+      <c r="B464" t="str">
+        <v>Remember to confirm your selection</v>
+      </c>
+      <c r="C464" t="str">
+        <v>记得确认您的选择</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="str">
+        <v>tours.settings.step1</v>
+      </c>
+      <c r="B465" t="str">
+        <v>In the Time settings, you can Set the "Top of Interval" and "Base of Interval" for your data. These fields allow you to define the starting and ending ages or stages, which can be adjusted by entering values or using the dropdown selectors. Adjust the vertical scale to change how much vertical space each million years occupies on your charts. For example, setting it higher will spread the intervals further apart, making each period easier to examine closely.</v>
+      </c>
+      <c r="C465" t="str">
+        <v>在时间设置中，您可以为您的数据设置“时间段顶部”和“时间段底部”。调整这两个值将改变图表的时间跨度，您可以通过输入值或使用下拉选择器进行调整。您还可以调整垂直比例，以改变图表中每百万年占据的垂直空间量。例如，将其设置得更高将使时间间隔进一步分开，使每个时期更易于仔细检查。</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="str">
+        <v>tours.settings.step2</v>
+      </c>
+      <c r="B466" t="str">
+        <v>In the Preferences settings, you can customize the display options. For instance, you may choose to gray out columns with no data for selected time periods, add tooltips for additional information, or enable filtering and legend options for charts. Furthermore, you can load your settings from a file or save your current settings to a file. This feature is useful for backing up your configurations, sharing them with others, or quickly applying previously saved configurations to your chart.</v>
+      </c>
+      <c r="C466" t="str">
+        <v>在偏好中，您可以自定义显示选项。例如，您可以选择在选定时间段内将无数据的列显示为灰色，添加工具提示以提供额外信息，或启用图表的筛选和图例选项。此外，您可以从文件加载您的设置或将当前设置保存到文件中。此功能使您可以备份设置、与他人分享或快速应用以前保存的设置到您的图表中。</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="str">
+        <v>tours.settings.step3</v>
+      </c>
+      <c r="B467" t="str">
+        <v>In Column Settings, you can deeply customize the appearance and organization of your charts.In the "Column Customization" area, you can adjust titles and shift row positions to streamline how data is displayed on your charts. Enable or disable specific elements like the chart title and Ma markers to suit your presentation needs. In the "Font Options" section, refine the appearance of your charts by choosing different fonts, sizes, and styles for headers and labels, ensuring important data stands out or meets formatting requirements. Please note that the advanced settings for columns can vary depending on the datapack you are working with, allowing for tailored configurations that best fit the data characteristics.</v>
+      </c>
+      <c r="C467" t="str">
+        <v>在列设置中，您可以深度自定义图表的外观和组织。在“列自定义”区域，您可以调整标题和移动行位置，以简化图表上数据的显示方式。根据您的展示需求启用或禁用特定元素，如图表标题和百万年标记。在“字体选项”部分，通过选择不同的字体、大小和样式为标题和标签，细化您的图表外观，确保重要数据突出显示或符合格式要求。请注意，列高级设置可能根据您正在使用的数据包而有所不同，每个数据包都有最适合数据特性的列高级设置。</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="str">
+        <v>tours.settings.step4</v>
+      </c>
+      <c r="B468" t="str">
+        <v>In the Search Settings, you can quickly locate specific columns by entering keywords and then directly add them to your chart. Simply enter a term related to the setting you are looking for, and the system will display all relevant results.This feature is particularly useful when managing numerous data points or when you need to make quick adjustments without browsing through extensive lists.</v>
+      </c>
+      <c r="C468" t="str">
+        <v>在搜索中，您可以通过输入关键词快速定位特定列，然后直接将其添加到您的图表中。只需输入一个与您正在寻找的设置相关的词语，系统便会显示所有相关结果。此功能可以帮助您管理众多数据点，或进行快速调整而无需浏览繁杂列表。请注意目前只支持英文搜索。</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="str">
+        <v>tours.settings.step5</v>
+      </c>
+      <c r="B469" t="str">
+        <v>The Font Settings section allows you to customize the appearance of text within your charts. You can adjust font styles, sizes, and formatting for various elements such as column headers, age labels, and more. Each setting is inheritable, ensuring consistency across related elements unless specified otherwise. Changing a font setting here applies it system-wide, but you can override these for individual columns by using the "Change Font" option within each columns settings.Experiment with different fonts and sizes to enhance readability and visual appeal of your charts.</v>
+      </c>
+      <c r="C469" t="str">
+        <v>在字体设置中您可以自定义图表内的文本外观。您可以为各种元素如列标题、年龄标签等调整字体样式、大小和格式。每项设置都是可继承的，确保相关元素间的一致性，除非另行设置。在这里更改字体设置将系统范围内应用，但您可以使用每个列设置中的“更改字体”选项覆盖这些设置。尝试不同的字体和大小，以增强图表的可读性和视觉吸引力。</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="str">
+        <v>tours.settings.step6</v>
+      </c>
+      <c r="B470" t="str">
+        <v>In the Map Points Settings, you can access and manage geographic data points for different locations. This feature allows you to view specific location details directly on the interactive map. You can toggle different map layers and visualize data points with detailed descriptions, like latitude, longitude, and additional notes. Please note, however, that not all datapacks contain map points.</v>
+      </c>
+      <c r="C470" t="str">
+        <v>在地图点设置中，您可以访问和管理不同位置的地理数据点。此功能允许您直接在交互式地图上查看特定位置的详细信息。您可以切换不同的地图层，并用详细描述（如纬度、经度和附加说明）可视化数据点。请注意，并非所有数据包都包含地图点。</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="str">
+        <v>tours.settings.step7</v>
+      </c>
+      <c r="B471" t="str">
+        <v>In the Datapacks Settings, you can select the datapacks you wish to use for generating charts. We offer nine official datapacks, each comprising a curated collection of datasets tailored for specific thematic explorations. You might notice that this page resembles the Datapack page; selections can be configured here or there interchangeably. For more detailed guidance on how to utilize datapacks, please refer to the Datapacks Tour in the Help page "Tours" section.</v>
+      </c>
+      <c r="C471" t="str">
+        <v>在数据包设置中，您可以选择您希望用于生成图表的数据包。我们提供九个官方数据包，每个数据包都包含为特定主题探索量身定制的数据集合。您也许已经注意到，此页面与"数据包"页面内容相同；您在两个地方都可以进行选择和设置。如需更详细的关于如何利用数据包的指导，请参阅帮助页面“导览”部分中的数据包导览。</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="str">
+        <v>settings.column.tooltip.note-in-range</v>
+      </c>
+      <c r="C472" t="str">
+        <v>数据不在所选时间区间内</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="str">
+        <v>language-names.en-US</v>
+      </c>
+      <c r="C473" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="str">
+        <v>language-names.en</v>
+      </c>
+      <c r="C474" t="str">
+        <v>English</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="str">
         <v>language-names.zh</v>
       </c>
-      <c r="C453" t="str">
+      <c r="C475" t="str">
         <v>中文</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C453"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C475"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>